<commit_message>
Fixes with reporter and updates for stuff
</commit_message>
<xml_diff>
--- a/netcalls.xlsx
+++ b/netcalls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cc948d2fdda6f6d9/^JData Backup/Projects/C^N/UncreatedWarfare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:40009_{46A2828C-718E-41F1-A065-9491A5788052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C78B2A7-6C0A-4DDA-8405-4416627D25D3}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:40009_{46A2828C-718E-41F1-A065-9491A5788052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE81AF1B-B98D-47A8-959A-464D10637F71}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="45" windowWidth="28770" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="netcalls" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="177">
   <si>
     <t>SendPlayerList</t>
   </si>
@@ -542,6 +542,15 @@
   </si>
   <si>
     <t>string exceptionReadout</t>
+  </si>
+  <si>
+    <t>SendServerInfo</t>
+  </si>
+  <si>
+    <t>Data.NetCall</t>
+  </si>
+  <si>
+    <t>WarfareServerInfo info</t>
   </si>
 </sst>
 </file>
@@ -1086,10 +1095,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E94" totalsRowShown="0">
-  <autoFilter ref="A1:E94" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E94">
-    <sortCondition ref="B1:B94"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E95" totalsRowShown="0">
+  <autoFilter ref="A1:E95" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E95">
+    <sortCondition ref="B1:B95"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="NetCall Field Name"/>
@@ -1399,10 +1408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E94"/>
+  <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1569,27 +1578,27 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>174</v>
       </c>
       <c r="B10">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>175</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -1598,15 +1607,15 @@
         <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -1620,27 +1629,27 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>111</v>
+        <v>20</v>
       </c>
       <c r="B13">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="C13" t="s">
-        <v>115</v>
+        <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>116</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B14">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="C14" t="s">
         <v>115</v>
@@ -1654,10 +1663,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B15">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="C15" t="s">
         <v>115</v>
@@ -1666,15 +1675,15 @@
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B16">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="C16" t="s">
         <v>115</v>
@@ -1683,32 +1692,32 @@
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>114</v>
       </c>
       <c r="B17">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="C17" t="s">
-        <v>1</v>
+        <v>115</v>
       </c>
       <c r="D17" t="s">
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>22</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B18">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="C18" t="s">
         <v>1</v>
@@ -1717,15 +1726,15 @@
         <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B19">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
@@ -1734,15 +1743,15 @@
         <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B20">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="C20" t="s">
         <v>1</v>
@@ -1751,106 +1760,106 @@
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>170</v>
+        <v>27</v>
       </c>
       <c r="B21">
-        <v>1023</v>
+        <v>1019</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>171</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>170</v>
       </c>
       <c r="B22">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="C22" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="D22" t="s">
         <v>17</v>
       </c>
       <c r="E22" t="s">
-        <v>30</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B23">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="D23" t="s">
         <v>17</v>
       </c>
       <c r="E23" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B24">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="C24" t="s">
         <v>32</v>
       </c>
       <c r="D24" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B25">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="C25" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="D25" t="s">
         <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B26">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E26" t="s">
         <v>37</v>
@@ -1858,41 +1867,41 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="C27" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="D27" t="s">
         <v>17</v>
+      </c>
+      <c r="E27" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B28">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="C28" t="s">
         <v>40</v>
       </c>
       <c r="D28" t="s">
-        <v>2</v>
-      </c>
-      <c r="E28" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B29">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="C29" t="s">
         <v>40</v>
@@ -1901,117 +1910,117 @@
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B30">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="C30" t="s">
         <v>40</v>
       </c>
       <c r="D30" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B31">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="C31" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="D31" t="s">
         <v>17</v>
       </c>
       <c r="E31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B32">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="C32" t="s">
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E32" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B33">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="C33" t="s">
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E33" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B34">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="C34" t="s">
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E34" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B35">
-        <v>1100</v>
+        <v>1036</v>
       </c>
       <c r="C35" t="s">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E35" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B36">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="C36" t="s">
         <v>54</v>
@@ -2020,32 +2029,32 @@
         <v>17</v>
       </c>
       <c r="E36" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B37">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="C37" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="D37" t="s">
         <v>17</v>
       </c>
       <c r="E37" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B38">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="C38" t="s">
         <v>5</v>
@@ -2059,10 +2068,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B39">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="C39" t="s">
         <v>5</v>
@@ -2076,10 +2085,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B40">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="C40" t="s">
         <v>5</v>
@@ -2093,10 +2102,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B41">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="C41" t="s">
         <v>5</v>
@@ -2110,10 +2119,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B42">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="C42" t="s">
         <v>5</v>
@@ -2127,95 +2136,95 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B43">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="C43" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="D43" t="s">
         <v>17</v>
       </c>
       <c r="E43" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B44">
-        <v>1112</v>
+        <v>1109</v>
       </c>
       <c r="C44" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="D44" t="s">
         <v>17</v>
       </c>
       <c r="E44" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B45">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="C45" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="D45" t="s">
         <v>17</v>
       </c>
       <c r="E45" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B46">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C46" t="s">
         <v>54</v>
       </c>
       <c r="D46" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E46" t="s">
-        <v>98</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B47">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="C47" t="s">
         <v>54</v>
       </c>
       <c r="D47" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E47" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B48">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="C48" t="s">
         <v>54</v>
@@ -2224,32 +2233,32 @@
         <v>17</v>
       </c>
       <c r="E48" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B49">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="C49" t="s">
         <v>54</v>
       </c>
       <c r="D49" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E49" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B50">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="C50" t="s">
         <v>54</v>
@@ -2258,182 +2267,182 @@
         <v>2</v>
       </c>
       <c r="E50" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B51">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="C51" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="D51" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E51" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="B52">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="C52" t="s">
         <v>32</v>
       </c>
       <c r="D52" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E52" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="B53">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="C53" t="s">
         <v>32</v>
       </c>
       <c r="D53" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E53" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="B54">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="C54" t="s">
         <v>32</v>
       </c>
       <c r="D54" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E54" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="B55">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="C55" t="s">
         <v>32</v>
       </c>
       <c r="D55" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E55" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B56">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C56" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
       <c r="D56" t="s">
         <v>17</v>
-      </c>
-      <c r="E56" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B57">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C57" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D57" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E57" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B58">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="C58" t="s">
         <v>85</v>
       </c>
       <c r="D58" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E58" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B59">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C59" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D59" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E59" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B60">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="C60" t="s">
         <v>90</v>
       </c>
       <c r="D60" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E60" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B61">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="C61" t="s">
         <v>90</v>
@@ -2441,279 +2450,279 @@
       <c r="D61" t="s">
         <v>17</v>
       </c>
+      <c r="E61" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B62">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="C62" t="s">
         <v>90</v>
       </c>
       <c r="D62" t="s">
-        <v>2</v>
-      </c>
-      <c r="E62" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>172</v>
+        <v>95</v>
       </c>
       <c r="B63">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="C63" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="D63" t="s">
         <v>2</v>
       </c>
       <c r="E63" t="s">
-        <v>173</v>
+        <v>91</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>120</v>
+        <v>172</v>
       </c>
       <c r="B64">
-        <v>2000</v>
+        <v>1131</v>
       </c>
       <c r="C64" t="s">
-        <v>119</v>
+        <v>40</v>
       </c>
       <c r="D64" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E64" t="s">
-        <v>24</v>
+        <v>173</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="B65">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="C65" t="s">
         <v>119</v>
       </c>
       <c r="D65" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E65" t="s">
-        <v>156</v>
+        <v>24</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="B66">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="C66" t="s">
         <v>119</v>
       </c>
       <c r="D66" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E66" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B67">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="C67" t="s">
         <v>119</v>
       </c>
       <c r="D67" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E67" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="B68">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="C68" t="s">
         <v>119</v>
       </c>
       <c r="D68" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E68" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="B69">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="C69" t="s">
         <v>119</v>
       </c>
       <c r="D69" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E69" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="B70">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="C70" t="s">
         <v>119</v>
       </c>
       <c r="D70" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E70" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="B71">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="C71" t="s">
         <v>119</v>
       </c>
       <c r="D71" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E71" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="B72">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="C72" t="s">
         <v>119</v>
       </c>
       <c r="D72" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E72" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="B73">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="C73" t="s">
         <v>119</v>
       </c>
       <c r="D73" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E73" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B74">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="C74" t="s">
         <v>119</v>
       </c>
       <c r="D74" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E74" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="B75">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="C75" t="s">
         <v>119</v>
       </c>
       <c r="D75" t="s">
-        <v>2</v>
-      </c>
-      <c r="E75" t="s">
-        <v>159</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="B76">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="C76" t="s">
         <v>119</v>
       </c>
       <c r="D76" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E76" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="B77">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="C77" t="s">
         <v>119</v>
       </c>
       <c r="D77" t="s">
-        <v>2</v>
-      </c>
-      <c r="E77" t="s">
-        <v>160</v>
+        <v>17</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B78">
-        <v>2019</v>
+        <v>2013</v>
       </c>
       <c r="C78" t="s">
         <v>119</v>
@@ -2722,49 +2731,49 @@
         <v>2</v>
       </c>
       <c r="E78" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="B79">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="C79" t="s">
         <v>119</v>
       </c>
       <c r="D79" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E79" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="B80">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C80" t="s">
         <v>119</v>
       </c>
       <c r="D80" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E80" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B81">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C81" t="s">
         <v>119</v>
@@ -2773,15 +2782,15 @@
         <v>2</v>
       </c>
       <c r="E81" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B82">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C82" t="s">
         <v>119</v>
@@ -2790,15 +2799,15 @@
         <v>2</v>
       </c>
       <c r="E82" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B83">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C83" t="s">
         <v>119</v>
@@ -2807,29 +2816,32 @@
         <v>2</v>
       </c>
       <c r="E83" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="B84">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="C84" t="s">
         <v>119</v>
       </c>
       <c r="D84" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E84" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B85">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="C85" t="s">
         <v>119</v>
@@ -2840,10 +2852,10 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B86">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="C86" t="s">
         <v>119</v>
@@ -2854,10 +2866,10 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B87">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="C87" t="s">
         <v>119</v>
@@ -2868,27 +2880,24 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="B88">
-        <v>2090</v>
+        <v>2028</v>
       </c>
       <c r="C88" t="s">
         <v>119</v>
       </c>
       <c r="D88" t="s">
-        <v>2</v>
-      </c>
-      <c r="E88" t="s">
-        <v>166</v>
+        <v>17</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B89">
-        <v>2091</v>
+        <v>2090</v>
       </c>
       <c r="C89" t="s">
         <v>119</v>
@@ -2897,15 +2906,15 @@
         <v>2</v>
       </c>
       <c r="E89" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B90">
-        <v>2092</v>
+        <v>2091</v>
       </c>
       <c r="C90" t="s">
         <v>119</v>
@@ -2914,15 +2923,15 @@
         <v>2</v>
       </c>
       <c r="E90" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B91">
-        <v>2093</v>
+        <v>2092</v>
       </c>
       <c r="C91" t="s">
         <v>119</v>
@@ -2931,15 +2940,15 @@
         <v>2</v>
       </c>
       <c r="E91" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B92">
-        <v>2094</v>
+        <v>2093</v>
       </c>
       <c r="C92" t="s">
         <v>119</v>
@@ -2948,40 +2957,57 @@
         <v>2</v>
       </c>
       <c r="E92" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>106</v>
+        <v>148</v>
       </c>
       <c r="B93">
-        <v>4000</v>
+        <v>2094</v>
       </c>
       <c r="C93" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="D93" t="s">
         <v>2</v>
       </c>
       <c r="E93" t="s">
-        <v>108</v>
+        <v>169</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B94">
-        <v>4001</v>
+        <v>4000</v>
       </c>
       <c r="C94" t="s">
         <v>107</v>
       </c>
       <c r="D94" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E94" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>109</v>
+      </c>
+      <c r="B95">
+        <v>4001</v>
+      </c>
+      <c r="C95" t="s">
+        <v>107</v>
+      </c>
+      <c r="D95" t="s">
+        <v>17</v>
+      </c>
+      <c r="E95" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished the new commands and fixed permissions
</commit_message>
<xml_diff>
--- a/netcalls.xlsx
+++ b/netcalls.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cc948d2fdda6f6d9/^JData Backup/Projects/C^N/UncreatedWarfare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:40009_{46A2828C-718E-41F1-A065-9491A5788052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE81AF1B-B98D-47A8-959A-464D10637F71}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="13_ncr:40009_{46A2828C-718E-41F1-A065-9491A5788052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{516C8C8C-290D-43A2-8E9C-C6807981CD2D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="6675" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="netcalls" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="193">
   <si>
     <t>SendPlayerList</t>
   </si>
@@ -181,21 +181,6 @@
     <t>ulong player, bool isOnline</t>
   </si>
   <si>
-    <t>GiveKitAccess</t>
-  </si>
-  <si>
-    <t>KitManager.NetCalls</t>
-  </si>
-  <si>
-    <t>ulong target, string kitName, EKitAccessType accessType</t>
-  </si>
-  <si>
-    <t>RemoveKitAccess</t>
-  </si>
-  <si>
-    <t>ulong target, string kitName</t>
-  </si>
-  <si>
     <t>GrantAdminRequest</t>
   </si>
   <si>
@@ -551,6 +536,69 @@
   </si>
   <si>
     <t>WarfareServerInfo info</t>
+  </si>
+  <si>
+    <t>RequestCreateLoadout</t>
+  </si>
+  <si>
+    <t>SendAckCreateLoadout</t>
+  </si>
+  <si>
+    <t>string kitName, int signIndex</t>
+  </si>
+  <si>
+    <t>ulong fromPlayer, ulong player, byte team, EClass @class, string displayName</t>
+  </si>
+  <si>
+    <t>RequestSetKitAccess</t>
+  </si>
+  <si>
+    <t>ulong target, string kitName, EKitAccessType accessType, bool state</t>
+  </si>
+  <si>
+    <t>SendAckSetKitAccess</t>
+  </si>
+  <si>
+    <t>bool foundKit</t>
+  </si>
+  <si>
+    <t>SendAckSetKitsAccess</t>
+  </si>
+  <si>
+    <t>bool[] success</t>
+  </si>
+  <si>
+    <t>RequestSetKitsAccess</t>
+  </si>
+  <si>
+    <t>KitEx.NetCalls</t>
+  </si>
+  <si>
+    <t>ulong admin, ulong player, string[] kits, EKitAccessType type, bool state</t>
+  </si>
+  <si>
+    <t>RequestKitAccess</t>
+  </si>
+  <si>
+    <t>string kit, ulong player</t>
+  </si>
+  <si>
+    <t>SendKitAccess</t>
+  </si>
+  <si>
+    <t>RequestKitsAccess</t>
+  </si>
+  <si>
+    <t>string[] kits, ulong player</t>
+  </si>
+  <si>
+    <t>SendKitsAccess</t>
+  </si>
+  <si>
+    <t>byte status, bool hasAccess</t>
+  </si>
+  <si>
+    <t>byte status, byte[] errorCodes</t>
   </si>
 </sst>
 </file>
@@ -1095,10 +1143,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E95" totalsRowShown="0">
-  <autoFilter ref="A1:E95" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E95">
-    <sortCondition ref="B1:B95"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E103" totalsRowShown="0">
+  <autoFilter ref="A1:E103" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E103">
+    <sortCondition ref="B1:B103"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="NetCall Field Name"/>
@@ -1408,10 +1456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E95"/>
+  <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1425,19 +1473,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1578,19 +1626,19 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B10">
         <v>1008</v>
       </c>
       <c r="C10" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D10" t="s">
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1646,70 +1694,70 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B14">
         <v>1012</v>
       </c>
       <c r="C14" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D14" t="s">
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B15">
         <v>1013</v>
       </c>
       <c r="C15" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D15" t="s">
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B16">
         <v>1014</v>
       </c>
       <c r="C16" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D16" t="s">
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B17">
         <v>1015</v>
       </c>
       <c r="C17" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D17" t="s">
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1782,7 +1830,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B22">
         <v>1023</v>
@@ -1794,7 +1842,7 @@
         <v>17</v>
       </c>
       <c r="E22" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2017,41 +2065,41 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>53</v>
+        <v>176</v>
       </c>
       <c r="B36">
         <v>1100</v>
       </c>
       <c r="C36" t="s">
-        <v>54</v>
+        <v>183</v>
       </c>
       <c r="D36" t="s">
         <v>17</v>
       </c>
       <c r="E36" t="s">
-        <v>55</v>
+        <v>177</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>178</v>
       </c>
       <c r="B37">
         <v>1101</v>
       </c>
       <c r="C37" t="s">
-        <v>54</v>
+        <v>183</v>
       </c>
       <c r="D37" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E37" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B38">
         <v>1103</v>
@@ -2068,7 +2116,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B39">
         <v>1104</v>
@@ -2085,7 +2133,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B40">
         <v>1105</v>
@@ -2102,7 +2150,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B41">
         <v>1106</v>
@@ -2119,7 +2167,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B42">
         <v>1107</v>
@@ -2136,7 +2184,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B43">
         <v>1108</v>
@@ -2153,180 +2201,180 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B44">
         <v>1109</v>
       </c>
       <c r="C44" t="s">
-        <v>54</v>
+        <v>183</v>
       </c>
       <c r="D44" t="s">
         <v>17</v>
       </c>
       <c r="E44" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>66</v>
+        <v>172</v>
       </c>
       <c r="B45">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="C45" t="s">
-        <v>5</v>
+        <v>183</v>
       </c>
       <c r="D45" t="s">
         <v>17</v>
       </c>
       <c r="E45" t="s">
-        <v>47</v>
+        <v>175</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>67</v>
+        <v>173</v>
       </c>
       <c r="B46">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="C46" t="s">
-        <v>54</v>
+        <v>183</v>
       </c>
       <c r="D46" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E46" t="s">
-        <v>68</v>
+        <v>174</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B47">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="C47" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="D47" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E47" t="s">
-        <v>98</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B48">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="C48" t="s">
-        <v>54</v>
+        <v>183</v>
       </c>
       <c r="D48" t="s">
         <v>17</v>
       </c>
       <c r="E48" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B49">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="C49" t="s">
-        <v>54</v>
+        <v>183</v>
       </c>
       <c r="D49" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E49" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B50">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="C50" t="s">
-        <v>54</v>
+        <v>183</v>
       </c>
       <c r="D50" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E50" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B51">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="C51" t="s">
-        <v>54</v>
+        <v>183</v>
       </c>
       <c r="D51" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E51" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B52">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="C52" t="s">
-        <v>32</v>
+        <v>183</v>
       </c>
       <c r="D52" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E52" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>96</v>
+        <v>69</v>
       </c>
       <c r="B53">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="C53" t="s">
-        <v>32</v>
+        <v>183</v>
       </c>
       <c r="D53" t="s">
         <v>2</v>
       </c>
       <c r="E53" t="s">
-        <v>97</v>
+        <v>70</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B54">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="C54" t="s">
         <v>32</v>
@@ -2335,15 +2383,15 @@
         <v>17</v>
       </c>
       <c r="E54" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="B55">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="C55" t="s">
         <v>32</v>
@@ -2352,15 +2400,15 @@
         <v>2</v>
       </c>
       <c r="E55" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B56">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="C56" t="s">
         <v>32</v>
@@ -2368,483 +2416,486 @@
       <c r="D56" t="s">
         <v>17</v>
       </c>
+      <c r="E56" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="B57">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="C57" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
       <c r="D57" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E57" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B58">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="C58" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
       <c r="D58" t="s">
-        <v>2</v>
-      </c>
-      <c r="E58" t="s">
-        <v>86</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B59">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="C59" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="D59" t="s">
         <v>17</v>
       </c>
       <c r="E59" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B60">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="C60" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D60" t="s">
         <v>2</v>
       </c>
       <c r="E60" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B61">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="C61" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D61" t="s">
         <v>17</v>
       </c>
       <c r="E61" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B62">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="C62" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D62" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E62" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B63">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="C63" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D63" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E63" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>172</v>
+        <v>89</v>
       </c>
       <c r="B64">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="C64" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="D64" t="s">
-        <v>2</v>
-      </c>
-      <c r="E64" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="B65">
-        <v>2000</v>
+        <v>1130</v>
       </c>
       <c r="C65" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="D65" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E65" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>134</v>
+        <v>167</v>
       </c>
       <c r="B66">
-        <v>2001</v>
+        <v>1131</v>
       </c>
       <c r="C66" t="s">
-        <v>119</v>
+        <v>40</v>
       </c>
       <c r="D66" t="s">
         <v>2</v>
       </c>
       <c r="E66" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>121</v>
+        <v>182</v>
       </c>
       <c r="B67">
-        <v>2002</v>
+        <v>1132</v>
       </c>
       <c r="C67" t="s">
-        <v>119</v>
+        <v>183</v>
       </c>
       <c r="D67" t="s">
         <v>17</v>
       </c>
       <c r="E67" t="s">
-        <v>149</v>
+        <v>184</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>132</v>
+        <v>180</v>
       </c>
       <c r="B68">
-        <v>2003</v>
+        <v>1133</v>
       </c>
       <c r="C68" t="s">
-        <v>119</v>
+        <v>183</v>
       </c>
       <c r="D68" t="s">
         <v>2</v>
       </c>
       <c r="E68" t="s">
-        <v>154</v>
+        <v>181</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>122</v>
+        <v>185</v>
       </c>
       <c r="B69">
-        <v>2004</v>
+        <v>1134</v>
       </c>
       <c r="C69" t="s">
-        <v>119</v>
+        <v>183</v>
       </c>
       <c r="D69" t="s">
         <v>17</v>
       </c>
       <c r="E69" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>133</v>
+        <v>187</v>
       </c>
       <c r="B70">
-        <v>2005</v>
+        <v>1135</v>
       </c>
       <c r="C70" t="s">
-        <v>119</v>
+        <v>183</v>
       </c>
       <c r="D70" t="s">
         <v>2</v>
       </c>
       <c r="E70" t="s">
-        <v>155</v>
+        <v>191</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>123</v>
+        <v>188</v>
       </c>
       <c r="B71">
-        <v>2006</v>
+        <v>1136</v>
       </c>
       <c r="C71" t="s">
-        <v>119</v>
+        <v>183</v>
       </c>
       <c r="D71" t="s">
         <v>17</v>
       </c>
       <c r="E71" t="s">
-        <v>151</v>
+        <v>189</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>135</v>
+        <v>190</v>
       </c>
       <c r="B72">
-        <v>2007</v>
+        <v>1137</v>
       </c>
       <c r="C72" t="s">
-        <v>119</v>
+        <v>183</v>
       </c>
       <c r="D72" t="s">
         <v>2</v>
       </c>
       <c r="E72" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B73">
-        <v>2008</v>
+        <v>2000</v>
       </c>
       <c r="C73" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D73" t="s">
         <v>17</v>
       </c>
       <c r="E73" t="s">
-        <v>152</v>
+        <v>24</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B74">
-        <v>2009</v>
+        <v>2001</v>
       </c>
       <c r="C74" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D74" t="s">
         <v>2</v>
       </c>
       <c r="E74" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B75">
-        <v>2010</v>
+        <v>2002</v>
       </c>
       <c r="C75" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D75" t="s">
         <v>17</v>
+      </c>
+      <c r="E75" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B76">
-        <v>2011</v>
+        <v>2003</v>
       </c>
       <c r="C76" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D76" t="s">
         <v>2</v>
       </c>
       <c r="E76" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B77">
-        <v>2012</v>
+        <v>2004</v>
       </c>
       <c r="C77" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D77" t="s">
         <v>17</v>
+      </c>
+      <c r="E77" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B78">
-        <v>2013</v>
+        <v>2005</v>
       </c>
       <c r="C78" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D78" t="s">
         <v>2</v>
       </c>
       <c r="E78" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="B79">
-        <v>2019</v>
+        <v>2006</v>
       </c>
       <c r="C79" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D79" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E79" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B80">
-        <v>2020</v>
+        <v>2007</v>
       </c>
       <c r="C80" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D80" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E80" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="B81">
-        <v>2021</v>
+        <v>2008</v>
       </c>
       <c r="C81" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D81" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E81" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B82">
-        <v>2022</v>
+        <v>2009</v>
       </c>
       <c r="C82" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D82" t="s">
         <v>2</v>
       </c>
       <c r="E82" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="B83">
-        <v>2023</v>
+        <v>2010</v>
       </c>
       <c r="C83" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D83" t="s">
-        <v>2</v>
-      </c>
-      <c r="E83" t="s">
-        <v>164</v>
+        <v>17</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B84">
-        <v>2024</v>
+        <v>2011</v>
       </c>
       <c r="C84" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D84" t="s">
         <v>2</v>
       </c>
       <c r="E84" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B85">
-        <v>2025</v>
+        <v>2012</v>
       </c>
       <c r="C85" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D85" t="s">
         <v>17</v>
@@ -2852,163 +2903,296 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B86">
-        <v>2026</v>
+        <v>2013</v>
       </c>
       <c r="C86" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D86" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E86" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B87">
-        <v>2027</v>
+        <v>2019</v>
       </c>
       <c r="C87" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D87" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E87" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B88">
-        <v>2028</v>
+        <v>2020</v>
       </c>
       <c r="C88" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D88" t="s">
         <v>17</v>
+      </c>
+      <c r="E88" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B89">
-        <v>2090</v>
+        <v>2021</v>
       </c>
       <c r="C89" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D89" t="s">
         <v>2</v>
       </c>
       <c r="E89" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B90">
-        <v>2091</v>
+        <v>2022</v>
       </c>
       <c r="C90" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D90" t="s">
         <v>2</v>
       </c>
       <c r="E90" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="B91">
-        <v>2092</v>
+        <v>2023</v>
       </c>
       <c r="C91" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D91" t="s">
         <v>2</v>
       </c>
       <c r="E91" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B92">
-        <v>2093</v>
+        <v>2024</v>
       </c>
       <c r="C92" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D92" t="s">
         <v>2</v>
       </c>
       <c r="E92" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="B93">
-        <v>2094</v>
+        <v>2025</v>
       </c>
       <c r="C93" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D93" t="s">
-        <v>2</v>
-      </c>
-      <c r="E93" t="s">
-        <v>169</v>
+        <v>17</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="B94">
-        <v>4000</v>
+        <v>2026</v>
       </c>
       <c r="C94" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="D94" t="s">
-        <v>2</v>
-      </c>
-      <c r="E94" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="B95">
+        <v>2027</v>
+      </c>
+      <c r="C95" t="s">
+        <v>114</v>
+      </c>
+      <c r="D95" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>126</v>
+      </c>
+      <c r="B96">
+        <v>2028</v>
+      </c>
+      <c r="C96" t="s">
+        <v>114</v>
+      </c>
+      <c r="D96" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>139</v>
+      </c>
+      <c r="B97">
+        <v>2090</v>
+      </c>
+      <c r="C97" t="s">
+        <v>114</v>
+      </c>
+      <c r="D97" t="s">
+        <v>2</v>
+      </c>
+      <c r="E97" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>140</v>
+      </c>
+      <c r="B98">
+        <v>2091</v>
+      </c>
+      <c r="C98" t="s">
+        <v>114</v>
+      </c>
+      <c r="D98" t="s">
+        <v>2</v>
+      </c>
+      <c r="E98" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>141</v>
+      </c>
+      <c r="B99">
+        <v>2092</v>
+      </c>
+      <c r="C99" t="s">
+        <v>114</v>
+      </c>
+      <c r="D99" t="s">
+        <v>2</v>
+      </c>
+      <c r="E99" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>142</v>
+      </c>
+      <c r="B100">
+        <v>2093</v>
+      </c>
+      <c r="C100" t="s">
+        <v>114</v>
+      </c>
+      <c r="D100" t="s">
+        <v>2</v>
+      </c>
+      <c r="E100" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>143</v>
+      </c>
+      <c r="B101">
+        <v>2094</v>
+      </c>
+      <c r="C101" t="s">
+        <v>114</v>
+      </c>
+      <c r="D101" t="s">
+        <v>2</v>
+      </c>
+      <c r="E101" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>101</v>
+      </c>
+      <c r="B102">
+        <v>4000</v>
+      </c>
+      <c r="C102" t="s">
+        <v>102</v>
+      </c>
+      <c r="D102" t="s">
+        <v>2</v>
+      </c>
+      <c r="E102" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>104</v>
+      </c>
+      <c r="B103">
         <v>4001</v>
       </c>
-      <c r="C95" t="s">
-        <v>107</v>
-      </c>
-      <c r="D95" t="s">
-        <v>17</v>
-      </c>
-      <c r="E95" t="s">
-        <v>110</v>
+      <c r="C103" t="s">
+        <v>102</v>
+      </c>
+      <c r="D103" t="s">
+        <v>17</v>
+      </c>
+      <c r="E103" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upgrades for new offense logging and queuing.
</commit_message>
<xml_diff>
--- a/netcalls.xlsx
+++ b/netcalls.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cc948d2fdda6f6d9/^JData Backup/Projects/C^N/UncreatedWarfare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="13_ncr:40009_{46A2828C-718E-41F1-A065-9491A5788052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{516C8C8C-290D-43A2-8E9C-C6807981CD2D}"/>
+  <xr:revisionPtr revIDLastSave="144" documentId="13_ncr:40009_{46A2828C-718E-41F1-A065-9491A5788052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC227A1A-29F1-4027-86A1-5C98D1E0EA60}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="6675" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2895" yWindow="1305" windowWidth="28770" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="netcalls" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="205">
   <si>
     <t>SendPlayerList</t>
   </si>
@@ -599,6 +599,42 @@
   </si>
   <si>
     <t>byte status, byte[] errorCodes</t>
+  </si>
+  <si>
+    <t>AckPlayerBanned</t>
+  </si>
+  <si>
+    <t>AckPlayerUnbanned</t>
+  </si>
+  <si>
+    <t>AckPlayerKicked</t>
+  </si>
+  <si>
+    <t>AckPlayerWarned</t>
+  </si>
+  <si>
+    <t>AckPlayerBattleyeKicked</t>
+  </si>
+  <si>
+    <t>AckTeamkill</t>
+  </si>
+  <si>
+    <t>AckVehicleTeamkill</t>
+  </si>
+  <si>
+    <t>AckPlayerUnmuted</t>
+  </si>
+  <si>
+    <t>AckPlayerMuted</t>
+  </si>
+  <si>
+    <t>SendPlayerUnmuted</t>
+  </si>
+  <si>
+    <t>ulong player, ulong admin, DateTime timestamp</t>
+  </si>
+  <si>
+    <t>SendUnmuteRequest</t>
   </si>
 </sst>
 </file>
@@ -1143,10 +1179,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E103" totalsRowShown="0">
-  <autoFilter ref="A1:E103" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E103">
-    <sortCondition ref="B1:B103"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E114" totalsRowShown="0">
+  <autoFilter ref="A1:E114" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E114">
+    <sortCondition ref="B1:B114"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="NetCall Field Name"/>
@@ -1456,10 +1492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E103"/>
+  <dimension ref="A1:E114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1830,211 +1866,211 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="B22">
-        <v>1023</v>
+        <v>1020</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>166</v>
+        <v>203</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>204</v>
       </c>
       <c r="B23">
-        <v>1024</v>
+        <v>1021</v>
       </c>
       <c r="C23" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D23" t="s">
         <v>17</v>
       </c>
       <c r="E23" t="s">
-        <v>30</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>165</v>
       </c>
       <c r="B24">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="C24" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D24" t="s">
         <v>17</v>
       </c>
       <c r="E24" t="s">
-        <v>33</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B25">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E25" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B26">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="C26" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="D26" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E26" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B27">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="D27" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B28">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B29">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E29" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B30">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="C30" t="s">
         <v>40</v>
       </c>
       <c r="D30" t="s">
-        <v>2</v>
-      </c>
-      <c r="E30" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B31">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="C31" t="s">
         <v>40</v>
       </c>
       <c r="D31" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B32">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="C32" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="D32" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E32" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B33">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="C33" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="D33" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E33" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B34">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="C34" t="s">
         <v>1</v>
@@ -2048,10 +2084,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B35">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="C35" t="s">
         <v>1</v>
@@ -2060,83 +2096,83 @@
         <v>2</v>
       </c>
       <c r="E35" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>176</v>
+        <v>50</v>
       </c>
       <c r="B36">
-        <v>1100</v>
+        <v>1035</v>
       </c>
       <c r="C36" t="s">
-        <v>183</v>
+        <v>1</v>
       </c>
       <c r="D36" t="s">
         <v>17</v>
       </c>
       <c r="E36" t="s">
-        <v>177</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>178</v>
+        <v>51</v>
       </c>
       <c r="B37">
-        <v>1101</v>
+        <v>1036</v>
       </c>
       <c r="C37" t="s">
-        <v>183</v>
+        <v>1</v>
       </c>
       <c r="D37" t="s">
         <v>2</v>
       </c>
       <c r="E37" t="s">
-        <v>179</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>53</v>
+        <v>176</v>
       </c>
       <c r="B38">
-        <v>1103</v>
+        <v>1100</v>
       </c>
       <c r="C38" t="s">
-        <v>5</v>
+        <v>183</v>
       </c>
       <c r="D38" t="s">
         <v>17</v>
       </c>
       <c r="E38" t="s">
-        <v>47</v>
+        <v>177</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>178</v>
       </c>
       <c r="B39">
-        <v>1104</v>
+        <v>1101</v>
       </c>
       <c r="C39" t="s">
-        <v>5</v>
+        <v>183</v>
       </c>
       <c r="D39" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E39" t="s">
-        <v>47</v>
+        <v>179</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B40">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="C40" t="s">
         <v>5</v>
@@ -2150,10 +2186,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B41">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="C41" t="s">
         <v>5</v>
@@ -2167,10 +2203,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B42">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="C42" t="s">
         <v>5</v>
@@ -2184,10 +2220,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B43">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="C43" t="s">
         <v>5</v>
@@ -2201,112 +2237,112 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B44">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="C44" t="s">
-        <v>183</v>
+        <v>5</v>
       </c>
       <c r="D44" t="s">
         <v>17</v>
       </c>
       <c r="E44" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>172</v>
+        <v>58</v>
       </c>
       <c r="B45">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="C45" t="s">
-        <v>183</v>
+        <v>5</v>
       </c>
       <c r="D45" t="s">
         <v>17</v>
       </c>
       <c r="E45" t="s">
-        <v>175</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>173</v>
+        <v>59</v>
       </c>
       <c r="B46">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="C46" t="s">
         <v>183</v>
       </c>
       <c r="D46" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E46" t="s">
-        <v>174</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>61</v>
+        <v>172</v>
       </c>
       <c r="B47">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="C47" t="s">
-        <v>5</v>
+        <v>183</v>
       </c>
       <c r="D47" t="s">
         <v>17</v>
       </c>
       <c r="E47" t="s">
-        <v>47</v>
+        <v>175</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>62</v>
+        <v>173</v>
       </c>
       <c r="B48">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="C48" t="s">
         <v>183</v>
       </c>
       <c r="D48" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E48" t="s">
-        <v>63</v>
+        <v>174</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B49">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="C49" t="s">
-        <v>183</v>
+        <v>5</v>
       </c>
       <c r="D49" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E49" t="s">
-        <v>93</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B50">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="C50" t="s">
         <v>183</v>
@@ -2320,95 +2356,95 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B51">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="C51" t="s">
         <v>183</v>
       </c>
       <c r="D51" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E51" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B52">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="C52" t="s">
         <v>183</v>
       </c>
       <c r="D52" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E52" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B53">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="C53" t="s">
         <v>183</v>
       </c>
       <c r="D53" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E53" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B54">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="C54" t="s">
-        <v>32</v>
+        <v>183</v>
       </c>
       <c r="D54" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E54" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="B55">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="C55" t="s">
-        <v>32</v>
+        <v>183</v>
       </c>
       <c r="D55" t="s">
         <v>2</v>
       </c>
       <c r="E55" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B56">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="C56" t="s">
         <v>32</v>
@@ -2417,15 +2453,15 @@
         <v>17</v>
       </c>
       <c r="E56" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B57">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="C57" t="s">
         <v>32</v>
@@ -2434,15 +2470,15 @@
         <v>2</v>
       </c>
       <c r="E57" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B58">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="C58" t="s">
         <v>32</v>
@@ -2450,180 +2486,180 @@
       <c r="D58" t="s">
         <v>17</v>
       </c>
+      <c r="E58" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="B59">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="C59" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="D59" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E59" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B60">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="C60" t="s">
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="D60" t="s">
-        <v>2</v>
-      </c>
-      <c r="E60" t="s">
-        <v>81</v>
+        <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B61">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="C61" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D61" t="s">
         <v>17</v>
       </c>
       <c r="E61" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B62">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="C62" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D62" t="s">
         <v>2</v>
       </c>
       <c r="E62" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B63">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="C63" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D63" t="s">
         <v>17</v>
       </c>
       <c r="E63" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B64">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="C64" t="s">
         <v>85</v>
       </c>
       <c r="D64" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E64" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B65">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="C65" t="s">
         <v>85</v>
       </c>
       <c r="D65" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E65" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>167</v>
+        <v>89</v>
       </c>
       <c r="B66">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="C66" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="D66" t="s">
-        <v>2</v>
-      </c>
-      <c r="E66" t="s">
-        <v>168</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>182</v>
+        <v>90</v>
       </c>
       <c r="B67">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="C67" t="s">
-        <v>183</v>
+        <v>85</v>
       </c>
       <c r="D67" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E67" t="s">
-        <v>184</v>
+        <v>86</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="B68">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="C68" t="s">
-        <v>183</v>
+        <v>40</v>
       </c>
       <c r="D68" t="s">
         <v>2</v>
       </c>
       <c r="E68" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B69">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="C69" t="s">
         <v>183</v>
@@ -2632,15 +2668,15 @@
         <v>17</v>
       </c>
       <c r="E69" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B70">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="C70" t="s">
         <v>183</v>
@@ -2649,15 +2685,15 @@
         <v>2</v>
       </c>
       <c r="E70" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B71">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="C71" t="s">
         <v>183</v>
@@ -2666,15 +2702,15 @@
         <v>17</v>
       </c>
       <c r="E71" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B72">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="C72" t="s">
         <v>183</v>
@@ -2683,188 +2719,164 @@
         <v>2</v>
       </c>
       <c r="E72" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>115</v>
+        <v>188</v>
       </c>
       <c r="B73">
-        <v>2000</v>
+        <v>1136</v>
       </c>
       <c r="C73" t="s">
-        <v>114</v>
+        <v>183</v>
       </c>
       <c r="D73" t="s">
         <v>17</v>
       </c>
       <c r="E73" t="s">
-        <v>24</v>
+        <v>189</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>129</v>
+        <v>190</v>
       </c>
       <c r="B74">
-        <v>2001</v>
+        <v>1137</v>
       </c>
       <c r="C74" t="s">
-        <v>114</v>
+        <v>183</v>
       </c>
       <c r="D74" t="s">
         <v>2</v>
       </c>
       <c r="E74" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>116</v>
+        <v>193</v>
       </c>
       <c r="B75">
-        <v>2002</v>
+        <v>1138</v>
       </c>
       <c r="C75" t="s">
-        <v>114</v>
+        <v>5</v>
       </c>
       <c r="D75" t="s">
         <v>17</v>
-      </c>
-      <c r="E75" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>127</v>
+        <v>194</v>
       </c>
       <c r="B76">
-        <v>2003</v>
+        <v>1139</v>
       </c>
       <c r="C76" t="s">
-        <v>114</v>
+        <v>5</v>
       </c>
       <c r="D76" t="s">
-        <v>2</v>
-      </c>
-      <c r="E76" t="s">
-        <v>149</v>
+        <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>117</v>
+        <v>195</v>
       </c>
       <c r="B77">
-        <v>2004</v>
+        <v>1140</v>
       </c>
       <c r="C77" t="s">
-        <v>114</v>
+        <v>5</v>
       </c>
       <c r="D77" t="s">
         <v>17</v>
-      </c>
-      <c r="E77" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>128</v>
+        <v>196</v>
       </c>
       <c r="B78">
-        <v>2005</v>
+        <v>1141</v>
       </c>
       <c r="C78" t="s">
-        <v>114</v>
+        <v>5</v>
       </c>
       <c r="D78" t="s">
-        <v>2</v>
-      </c>
-      <c r="E78" t="s">
-        <v>150</v>
+        <v>17</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>118</v>
+        <v>197</v>
       </c>
       <c r="B79">
-        <v>2006</v>
+        <v>1142</v>
       </c>
       <c r="C79" t="s">
-        <v>114</v>
+        <v>5</v>
       </c>
       <c r="D79" t="s">
         <v>17</v>
-      </c>
-      <c r="E79" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>130</v>
+        <v>198</v>
       </c>
       <c r="B80">
-        <v>2007</v>
+        <v>1143</v>
       </c>
       <c r="C80" t="s">
-        <v>114</v>
+        <v>5</v>
       </c>
       <c r="D80" t="s">
-        <v>2</v>
-      </c>
-      <c r="E80" t="s">
-        <v>152</v>
+        <v>17</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>119</v>
+        <v>201</v>
       </c>
       <c r="B81">
-        <v>2008</v>
+        <v>1144</v>
       </c>
       <c r="C81" t="s">
-        <v>114</v>
+        <v>5</v>
       </c>
       <c r="D81" t="s">
         <v>17</v>
-      </c>
-      <c r="E81" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>131</v>
+        <v>199</v>
       </c>
       <c r="B82">
-        <v>2009</v>
+        <v>1145</v>
       </c>
       <c r="C82" t="s">
-        <v>114</v>
+        <v>5</v>
       </c>
       <c r="D82" t="s">
-        <v>2</v>
-      </c>
-      <c r="E82" t="s">
-        <v>153</v>
+        <v>17</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="B83">
-        <v>2010</v>
+        <v>1146</v>
       </c>
       <c r="C83" t="s">
-        <v>114</v>
+        <v>5</v>
       </c>
       <c r="D83" t="s">
         <v>17</v>
@@ -2872,58 +2884,61 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="B84">
-        <v>2011</v>
+        <v>2000</v>
       </c>
       <c r="C84" t="s">
         <v>114</v>
       </c>
       <c r="D84" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E84" t="s">
-        <v>154</v>
+        <v>24</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B85">
-        <v>2012</v>
+        <v>2001</v>
       </c>
       <c r="C85" t="s">
         <v>114</v>
       </c>
       <c r="D85" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E85" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="B86">
-        <v>2013</v>
+        <v>2002</v>
       </c>
       <c r="C86" t="s">
         <v>114</v>
       </c>
       <c r="D86" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E86" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B87">
-        <v>2019</v>
+        <v>2003</v>
       </c>
       <c r="C87" t="s">
         <v>114</v>
@@ -2932,15 +2947,15 @@
         <v>2</v>
       </c>
       <c r="E87" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B88">
-        <v>2020</v>
+        <v>2004</v>
       </c>
       <c r="C88" t="s">
         <v>114</v>
@@ -2949,15 +2964,15 @@
         <v>17</v>
       </c>
       <c r="E88" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B89">
-        <v>2021</v>
+        <v>2005</v>
       </c>
       <c r="C89" t="s">
         <v>114</v>
@@ -2966,32 +2981,32 @@
         <v>2</v>
       </c>
       <c r="E89" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="B90">
-        <v>2022</v>
+        <v>2006</v>
       </c>
       <c r="C90" t="s">
         <v>114</v>
       </c>
       <c r="D90" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E90" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B91">
-        <v>2023</v>
+        <v>2007</v>
       </c>
       <c r="C91" t="s">
         <v>114</v>
@@ -3000,46 +3015,49 @@
         <v>2</v>
       </c>
       <c r="E91" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="B92">
-        <v>2024</v>
+        <v>2008</v>
       </c>
       <c r="C92" t="s">
         <v>114</v>
       </c>
       <c r="D92" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E92" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="B93">
-        <v>2025</v>
+        <v>2009</v>
       </c>
       <c r="C93" t="s">
         <v>114</v>
       </c>
       <c r="D93" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E93" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B94">
-        <v>2026</v>
+        <v>2010</v>
       </c>
       <c r="C94" t="s">
         <v>114</v>
@@ -3050,24 +3068,27 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="B95">
-        <v>2027</v>
+        <v>2011</v>
       </c>
       <c r="C95" t="s">
         <v>114</v>
       </c>
       <c r="D95" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E95" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B96">
-        <v>2028</v>
+        <v>2012</v>
       </c>
       <c r="C96" t="s">
         <v>114</v>
@@ -3078,10 +3099,10 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B97">
-        <v>2090</v>
+        <v>2013</v>
       </c>
       <c r="C97" t="s">
         <v>114</v>
@@ -3090,15 +3111,15 @@
         <v>2</v>
       </c>
       <c r="E97" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B98">
-        <v>2091</v>
+        <v>2019</v>
       </c>
       <c r="C98" t="s">
         <v>114</v>
@@ -3107,32 +3128,32 @@
         <v>2</v>
       </c>
       <c r="E98" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="B99">
-        <v>2092</v>
+        <v>2020</v>
       </c>
       <c r="C99" t="s">
         <v>114</v>
       </c>
       <c r="D99" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E99" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B100">
-        <v>2093</v>
+        <v>2021</v>
       </c>
       <c r="C100" t="s">
         <v>114</v>
@@ -3141,15 +3162,15 @@
         <v>2</v>
       </c>
       <c r="E100" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B101">
-        <v>2094</v>
+        <v>2022</v>
       </c>
       <c r="C101" t="s">
         <v>114</v>
@@ -3158,47 +3179,223 @@
         <v>2</v>
       </c>
       <c r="E101" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>101</v>
+        <v>137</v>
       </c>
       <c r="B102">
-        <v>4000</v>
+        <v>2023</v>
       </c>
       <c r="C102" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="D102" t="s">
         <v>2</v>
       </c>
       <c r="E102" t="s">
-        <v>103</v>
+        <v>159</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
+        <v>138</v>
+      </c>
+      <c r="B103">
+        <v>2024</v>
+      </c>
+      <c r="C103" t="s">
+        <v>114</v>
+      </c>
+      <c r="D103" t="s">
+        <v>2</v>
+      </c>
+      <c r="E103" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>123</v>
+      </c>
+      <c r="B104">
+        <v>2025</v>
+      </c>
+      <c r="C104" t="s">
+        <v>114</v>
+      </c>
+      <c r="D104" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>124</v>
+      </c>
+      <c r="B105">
+        <v>2026</v>
+      </c>
+      <c r="C105" t="s">
+        <v>114</v>
+      </c>
+      <c r="D105" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>125</v>
+      </c>
+      <c r="B106">
+        <v>2027</v>
+      </c>
+      <c r="C106" t="s">
+        <v>114</v>
+      </c>
+      <c r="D106" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>126</v>
+      </c>
+      <c r="B107">
+        <v>2028</v>
+      </c>
+      <c r="C107" t="s">
+        <v>114</v>
+      </c>
+      <c r="D107" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>139</v>
+      </c>
+      <c r="B108">
+        <v>2090</v>
+      </c>
+      <c r="C108" t="s">
+        <v>114</v>
+      </c>
+      <c r="D108" t="s">
+        <v>2</v>
+      </c>
+      <c r="E108" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>140</v>
+      </c>
+      <c r="B109">
+        <v>2091</v>
+      </c>
+      <c r="C109" t="s">
+        <v>114</v>
+      </c>
+      <c r="D109" t="s">
+        <v>2</v>
+      </c>
+      <c r="E109" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>141</v>
+      </c>
+      <c r="B110">
+        <v>2092</v>
+      </c>
+      <c r="C110" t="s">
+        <v>114</v>
+      </c>
+      <c r="D110" t="s">
+        <v>2</v>
+      </c>
+      <c r="E110" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>142</v>
+      </c>
+      <c r="B111">
+        <v>2093</v>
+      </c>
+      <c r="C111" t="s">
+        <v>114</v>
+      </c>
+      <c r="D111" t="s">
+        <v>2</v>
+      </c>
+      <c r="E111" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>143</v>
+      </c>
+      <c r="B112">
+        <v>2094</v>
+      </c>
+      <c r="C112" t="s">
+        <v>114</v>
+      </c>
+      <c r="D112" t="s">
+        <v>2</v>
+      </c>
+      <c r="E112" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>101</v>
+      </c>
+      <c r="B113">
+        <v>4000</v>
+      </c>
+      <c r="C113" t="s">
+        <v>102</v>
+      </c>
+      <c r="D113" t="s">
+        <v>2</v>
+      </c>
+      <c r="E113" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>104</v>
       </c>
-      <c r="B103">
+      <c r="B114">
         <v>4001</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C114" t="s">
         <v>102</v>
       </c>
-      <c r="D103" t="s">
-        <v>17</v>
-      </c>
-      <c r="E103" t="s">
+      <c r="D114" t="s">
+        <v>17</v>
+      </c>
+      <c r="E114" t="s">
         <v>105</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
(omg a commit no way its been like 2 weeks) Redid gamemode config to be used as a test for syncing. Now have diffing working for config as well and syncing is close to working.
</commit_message>
<xml_diff>
--- a/netcalls.xlsx
+++ b/netcalls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cc948d2fdda6f6d9/^JData Backup/Projects/C^N/UncreatedWarfare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="13_ncr:40009_{46A2828C-718E-41F1-A065-9491A5788052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC227A1A-29F1-4027-86A1-5C98D1E0EA60}"/>
+  <xr:revisionPtr revIDLastSave="192" documentId="13_ncr:40009_{46A2828C-718E-41F1-A065-9491A5788052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8A420A6-E6D8-42B1-A223-0B31D749B1CA}"/>
   <bookViews>
-    <workbookView xWindow="2895" yWindow="1305" windowWidth="28770" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="6675" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="netcalls" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="214">
   <si>
     <t>SendPlayerList</t>
   </si>
@@ -635,6 +635,33 @@
   </si>
   <si>
     <t>SendUnmuteRequest</t>
+  </si>
+  <si>
+    <t>KitSync.NetCalls</t>
+  </si>
+  <si>
+    <t>Kit kit</t>
+  </si>
+  <si>
+    <t>MulticastKitUpdated</t>
+  </si>
+  <si>
+    <t>FROM_EITHER</t>
+  </si>
+  <si>
+    <t>ConfigSync.NetCalls</t>
+  </si>
+  <si>
+    <t>SyncPacket packet</t>
+  </si>
+  <si>
+    <t>ReceiveSyncPacket</t>
+  </si>
+  <si>
+    <t>SendSingleProperty</t>
+  </si>
+  <si>
+    <t>PropertyValue property</t>
   </si>
 </sst>
 </file>
@@ -1179,10 +1206,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E114" totalsRowShown="0">
-  <autoFilter ref="A1:E114" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E114">
-    <sortCondition ref="B1:B114"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E117" totalsRowShown="0">
+  <autoFilter ref="A1:E117" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E117">
+    <sortCondition ref="B1:B117"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="NetCall Field Name"/>
@@ -1492,10 +1519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E114"/>
+  <dimension ref="A1:E117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3359,35 +3386,86 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>101</v>
+        <v>207</v>
       </c>
       <c r="B113">
-        <v>4000</v>
+        <v>3001</v>
       </c>
       <c r="C113" t="s">
-        <v>102</v>
+        <v>205</v>
       </c>
       <c r="D113" t="s">
-        <v>2</v>
+        <v>208</v>
       </c>
       <c r="E113" t="s">
-        <v>103</v>
+        <v>206</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
+        <v>212</v>
+      </c>
+      <c r="B114">
+        <v>3002</v>
+      </c>
+      <c r="C114" t="s">
+        <v>209</v>
+      </c>
+      <c r="D114" t="s">
+        <v>17</v>
+      </c>
+      <c r="E114" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>211</v>
+      </c>
+      <c r="B115">
+        <v>3003</v>
+      </c>
+      <c r="C115" t="s">
+        <v>209</v>
+      </c>
+      <c r="D115" t="s">
+        <v>17</v>
+      </c>
+      <c r="E115" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>101</v>
+      </c>
+      <c r="B116">
+        <v>4000</v>
+      </c>
+      <c r="C116" t="s">
+        <v>102</v>
+      </c>
+      <c r="D116" t="s">
+        <v>2</v>
+      </c>
+      <c r="E116" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>104</v>
       </c>
-      <c r="B114">
+      <c r="B117">
         <v>4001</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C117" t="s">
         <v>102</v>
       </c>
-      <c r="D114" t="s">
-        <v>17</v>
-      </c>
-      <c r="E114" t="s">
+      <c r="D117" t="s">
+        <v>17</v>
+      </c>
+      <c r="E117" t="s">
         <v>105</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Action log fixes, gamemode fixes, possible fix to laser guided issues?
</commit_message>
<xml_diff>
--- a/netcalls.xlsx
+++ b/netcalls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cc948d2fdda6f6d9/^JData Backup/Projects/C^N/UncreatedWarfare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="207" documentId="13_ncr:40009_{46A2828C-718E-41F1-A065-9491A5788052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C630F90-72F0-4445-85BD-608E4D59FC27}"/>
+  <xr:revisionPtr revIDLastSave="213" documentId="13_ncr:40009_{46A2828C-718E-41F1-A065-9491A5788052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D6E6DD4-EB58-4802-AEB7-725975ECF068}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="6675" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="207">
   <si>
     <t>SendPlayerList</t>
   </si>
@@ -274,27 +274,12 @@
     <t>Folder modContent</t>
   </si>
   <si>
-    <t>SendLog</t>
-  </si>
-  <si>
     <t>ActionLog.NetCalls</t>
   </si>
   <si>
-    <t>byte[] fileContents, DateTime startDate</t>
-  </si>
-  <si>
-    <t>AckLog</t>
-  </si>
-  <si>
-    <t>DateTime startDate</t>
-  </si>
-  <si>
     <t>RequestCurrentLog</t>
   </si>
   <si>
-    <t>SendCurrentLog</t>
-  </si>
-  <si>
     <t>SendItemInfo</t>
   </si>
   <si>
@@ -644,6 +629,18 @@
   </si>
   <si>
     <t>RequestFullSyncPacket</t>
+  </si>
+  <si>
+    <t>SendLogs</t>
+  </si>
+  <si>
+    <t>&lt;CUSTOM&gt;</t>
+  </si>
+  <si>
+    <t>AckLogs</t>
+  </si>
+  <si>
+    <t>DateTimeOffset[] received</t>
   </si>
 </sst>
 </file>
@@ -1188,10 +1185,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E110" totalsRowShown="0">
-  <autoFilter ref="A1:E110" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E110">
-    <sortCondition ref="B1:B110"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E109" totalsRowShown="0">
+  <autoFilter ref="A1:E109" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E109">
+    <sortCondition ref="B1:B109"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="NetCall Field Name"/>
@@ -1501,10 +1498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E110"/>
+  <dimension ref="A1:E109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1518,19 +1515,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1671,19 +1668,19 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B10">
         <v>1008</v>
       </c>
       <c r="C10" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D10" t="s">
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1739,70 +1736,70 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B14">
         <v>1012</v>
       </c>
       <c r="C14" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D14" t="s">
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B15">
         <v>1013</v>
       </c>
       <c r="C15" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D15" t="s">
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B16">
         <v>1014</v>
       </c>
       <c r="C16" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D16" t="s">
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B17">
         <v>1015</v>
       </c>
       <c r="C17" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D17" t="s">
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1875,7 +1872,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B22">
         <v>1020</v>
@@ -1887,12 +1884,12 @@
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B23">
         <v>1021</v>
@@ -1904,12 +1901,12 @@
         <v>17</v>
       </c>
       <c r="E23" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B24">
         <v>1023</v>
@@ -1921,7 +1918,7 @@
         <v>17</v>
       </c>
       <c r="E24" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2144,36 +2141,36 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B38">
         <v>1100</v>
       </c>
       <c r="C38" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D38" t="s">
         <v>17</v>
       </c>
       <c r="E38" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B39">
         <v>1101</v>
       </c>
       <c r="C39" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D39" t="s">
         <v>2</v>
       </c>
       <c r="E39" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -2286,7 +2283,7 @@
         <v>1109</v>
       </c>
       <c r="C46" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D46" t="s">
         <v>17</v>
@@ -2297,36 +2294,36 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B47">
         <v>1110</v>
       </c>
       <c r="C47" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D47" t="s">
         <v>17</v>
       </c>
       <c r="E47" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B48">
         <v>1111</v>
       </c>
       <c r="C48" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D48" t="s">
         <v>2</v>
       </c>
       <c r="E48" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -2354,7 +2351,7 @@
         <v>1113</v>
       </c>
       <c r="C50" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D50" t="s">
         <v>17</v>
@@ -2371,13 +2368,13 @@
         <v>1114</v>
       </c>
       <c r="C51" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D51" t="s">
         <v>2</v>
       </c>
       <c r="E51" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2388,7 +2385,7 @@
         <v>1115</v>
       </c>
       <c r="C52" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D52" t="s">
         <v>17</v>
@@ -2405,7 +2402,7 @@
         <v>1116</v>
       </c>
       <c r="C53" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D53" t="s">
         <v>17</v>
@@ -2422,7 +2419,7 @@
         <v>1117</v>
       </c>
       <c r="C54" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D54" t="s">
         <v>2</v>
@@ -2439,7 +2436,7 @@
         <v>1118</v>
       </c>
       <c r="C55" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D55" t="s">
         <v>2</v>
@@ -2467,7 +2464,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B57">
         <v>1120</v>
@@ -2479,7 +2476,7 @@
         <v>2</v>
       </c>
       <c r="E57" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2501,7 +2498,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B59">
         <v>1122</v>
@@ -2513,7 +2510,7 @@
         <v>2</v>
       </c>
       <c r="E59" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2583,47 +2580,47 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>84</v>
+        <v>203</v>
       </c>
       <c r="B64">
         <v>1127</v>
       </c>
       <c r="C64" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D64" t="s">
         <v>2</v>
       </c>
       <c r="E64" t="s">
-        <v>86</v>
+        <v>204</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>87</v>
+        <v>205</v>
       </c>
       <c r="B65">
         <v>1128</v>
       </c>
       <c r="C65" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D65" t="s">
         <v>17</v>
       </c>
       <c r="E65" t="s">
-        <v>88</v>
+        <v>206</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B66">
         <v>1129</v>
       </c>
       <c r="C66" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D66" t="s">
         <v>17</v>
@@ -2631,53 +2628,53 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>90</v>
+        <v>162</v>
       </c>
       <c r="B67">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="C67" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="D67" t="s">
         <v>2</v>
       </c>
       <c r="E67" t="s">
-        <v>86</v>
+        <v>163</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="B68">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="C68" t="s">
-        <v>40</v>
+        <v>178</v>
       </c>
       <c r="D68" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E68" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B69">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="C69" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D69" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E69" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -2685,13 +2682,13 @@
         <v>180</v>
       </c>
       <c r="B70">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="C70" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D70" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E70" t="s">
         <v>181</v>
@@ -2699,16 +2696,16 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B71">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="C71" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D71" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E71" t="s">
         <v>186</v>
@@ -2716,101 +2713,101 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B72">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="C72" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D72" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E72" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B73">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="C73" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D73" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E73" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>190</v>
+        <v>110</v>
       </c>
       <c r="B74">
-        <v>1137</v>
+        <v>2000</v>
       </c>
       <c r="C74" t="s">
-        <v>183</v>
+        <v>109</v>
       </c>
       <c r="D74" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E74" t="s">
-        <v>192</v>
+        <v>24</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="B75">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="C75" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D75" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E75" t="s">
-        <v>24</v>
+        <v>146</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="B76">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="C76" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D76" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E76" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B77">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="C77" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D77" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E77" t="s">
         <v>144</v>
@@ -2818,33 +2815,33 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="B78">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="C78" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D78" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E78" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B79">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="C79" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D79" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E79" t="s">
         <v>145</v>
@@ -2852,262 +2849,259 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="B80">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="C80" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D80" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E80" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="B81">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="C81" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D81" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E81" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="B82">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="C82" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D82" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E82" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="B83">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="C83" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D83" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E83" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="B84">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="C84" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D84" t="s">
-        <v>2</v>
-      </c>
-      <c r="E84" t="s">
-        <v>153</v>
+        <v>17</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B85">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="C85" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D85" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E85" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="B86">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="C86" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D86" t="s">
-        <v>2</v>
-      </c>
-      <c r="E86" t="s">
-        <v>154</v>
+        <v>17</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="B87">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="C87" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D87" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E87" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B88">
-        <v>2013</v>
+        <v>2019</v>
       </c>
       <c r="C88" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D88" t="s">
         <v>2</v>
       </c>
       <c r="E88" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="B89">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C89" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D89" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E89" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="B90">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C90" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D90" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E90" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B91">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C91" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D91" t="s">
         <v>2</v>
       </c>
       <c r="E91" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B92">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C92" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D92" t="s">
         <v>2</v>
       </c>
       <c r="E92" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B93">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C93" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D93" t="s">
         <v>2</v>
       </c>
       <c r="E93" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="B94">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="C94" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D94" t="s">
-        <v>2</v>
-      </c>
-      <c r="E94" t="s">
-        <v>160</v>
+        <v>17</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B95">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="C95" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D95" t="s">
         <v>17</v>
@@ -3115,13 +3109,13 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B96">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="C96" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D96" t="s">
         <v>17</v>
@@ -3129,13 +3123,13 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B97">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="C97" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D97" t="s">
         <v>17</v>
@@ -3143,101 +3137,104 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B98">
-        <v>2028</v>
+        <v>2090</v>
       </c>
       <c r="C98" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D98" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E98" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B99">
-        <v>2090</v>
+        <v>2091</v>
       </c>
       <c r="C99" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D99" t="s">
         <v>2</v>
       </c>
       <c r="E99" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B100">
-        <v>2091</v>
+        <v>2092</v>
       </c>
       <c r="C100" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D100" t="s">
         <v>2</v>
       </c>
       <c r="E100" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B101">
-        <v>2092</v>
+        <v>2093</v>
       </c>
       <c r="C101" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D101" t="s">
         <v>2</v>
       </c>
       <c r="E101" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B102">
-        <v>2093</v>
+        <v>2094</v>
       </c>
       <c r="C102" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D102" t="s">
         <v>2</v>
       </c>
       <c r="E102" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>143</v>
+        <v>193</v>
       </c>
       <c r="B103">
-        <v>2094</v>
+        <v>3001</v>
       </c>
       <c r="C103" t="s">
-        <v>114</v>
+        <v>191</v>
       </c>
       <c r="D103" t="s">
-        <v>2</v>
+        <v>194</v>
       </c>
       <c r="E103" t="s">
-        <v>164</v>
+        <v>192</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -3245,33 +3242,33 @@
         <v>198</v>
       </c>
       <c r="B104">
-        <v>3001</v>
+        <v>3002</v>
       </c>
       <c r="C104" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D104" t="s">
+        <v>194</v>
+      </c>
+      <c r="E104" t="s">
         <v>199</v>
-      </c>
-      <c r="E104" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B105">
-        <v>3002</v>
+        <v>3003</v>
       </c>
       <c r="C105" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D105" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E105" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -3279,81 +3276,64 @@
         <v>202</v>
       </c>
       <c r="B106">
-        <v>3003</v>
+        <v>3004</v>
       </c>
       <c r="C106" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D106" t="s">
-        <v>199</v>
-      </c>
-      <c r="E106" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B107">
-        <v>3004</v>
+        <v>3005</v>
       </c>
       <c r="C107" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D107" t="s">
-        <v>199</v>
+        <v>194</v>
+      </c>
+      <c r="E107" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>205</v>
+        <v>96</v>
       </c>
       <c r="B108">
-        <v>3005</v>
+        <v>4000</v>
       </c>
       <c r="C108" t="s">
-        <v>200</v>
+        <v>97</v>
       </c>
       <c r="D108" t="s">
-        <v>199</v>
+        <v>2</v>
       </c>
       <c r="E108" t="s">
-        <v>206</v>
+        <v>98</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B109">
-        <v>4000</v>
+        <v>4001</v>
       </c>
       <c r="C109" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D109" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E109" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>104</v>
-      </c>
-      <c r="B110">
-        <v>4001</v>
-      </c>
-      <c r="C110" t="s">
-        <v>102</v>
-      </c>
-      <c r="D110" t="s">
-        <v>17</v>
-      </c>
-      <c r="E110" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started working on list sync implementation
</commit_message>
<xml_diff>
--- a/netcalls.xlsx
+++ b/netcalls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cc948d2fdda6f6d9/^JData Backup/Projects/C^N/UncreatedWarfare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="213" documentId="13_ncr:40009_{46A2828C-718E-41F1-A065-9491A5788052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D6E6DD4-EB58-4802-AEB7-725975ECF068}"/>
+  <xr:revisionPtr revIDLastSave="225" documentId="13_ncr:40009_{46A2828C-718E-41F1-A065-9491A5788052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B7DB435-EE32-4CFB-8EB8-A1795DB332B4}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="6675" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="netcalls" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="209">
   <si>
     <t>SendPlayerList</t>
   </si>
@@ -517,9 +517,6 @@
     <t>SendServerInfo</t>
   </si>
   <si>
-    <t>Data.NetCall</t>
-  </si>
-  <si>
     <t>WarfareServerInfo info</t>
   </si>
   <si>
@@ -595,15 +592,6 @@
     <t>SendUnmuteRequest</t>
   </si>
   <si>
-    <t>KitSync.NetCalls</t>
-  </si>
-  <si>
-    <t>Kit kit</t>
-  </si>
-  <si>
-    <t>MulticastKitUpdated</t>
-  </si>
-  <si>
     <t>FROM_EITHER</t>
   </si>
   <si>
@@ -641,6 +629,24 @@
   </si>
   <si>
     <t>DateTimeOffset[] received</t>
+  </si>
+  <si>
+    <t>Data.NetCalls</t>
+  </si>
+  <si>
+    <t>MulticastListItemUpdated</t>
+  </si>
+  <si>
+    <t>MulticastListItemsUpdated</t>
+  </si>
+  <si>
+    <t>ListSync.NetCalls</t>
+  </si>
+  <si>
+    <t>ushort syncId, int pk</t>
+  </si>
+  <si>
+    <t>ushort syncId, int[] pks</t>
   </si>
 </sst>
 </file>
@@ -1184,11 +1190,15 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E109" totalsRowShown="0">
-  <autoFilter ref="A1:E109" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E109">
-    <sortCondition ref="B1:B109"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E110" totalsRowShown="0">
+  <autoFilter ref="A1:E110" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E110">
+    <sortCondition ref="B1:B110"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="NetCall Field Name"/>
@@ -1498,10 +1508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E109"/>
+  <dimension ref="A1:E110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1674,13 +1684,13 @@
         <v>1008</v>
       </c>
       <c r="C10" t="s">
+        <v>203</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
         <v>165</v>
-      </c>
-      <c r="D10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1872,7 +1882,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B22">
         <v>1020</v>
@@ -1884,12 +1894,12 @@
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B23">
         <v>1021</v>
@@ -1901,7 +1911,7 @@
         <v>17</v>
       </c>
       <c r="E23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2141,36 +2151,36 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B38">
         <v>1100</v>
       </c>
       <c r="C38" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D38" t="s">
         <v>17</v>
       </c>
       <c r="E38" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B39">
         <v>1101</v>
       </c>
       <c r="C39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D39" t="s">
         <v>2</v>
       </c>
       <c r="E39" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -2283,7 +2293,7 @@
         <v>1109</v>
       </c>
       <c r="C46" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D46" t="s">
         <v>17</v>
@@ -2294,36 +2304,36 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B47">
         <v>1110</v>
       </c>
       <c r="C47" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D47" t="s">
         <v>17</v>
       </c>
       <c r="E47" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B48">
         <v>1111</v>
       </c>
       <c r="C48" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D48" t="s">
         <v>2</v>
       </c>
       <c r="E48" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -2351,7 +2361,7 @@
         <v>1113</v>
       </c>
       <c r="C50" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D50" t="s">
         <v>17</v>
@@ -2368,7 +2378,7 @@
         <v>1114</v>
       </c>
       <c r="C51" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D51" t="s">
         <v>2</v>
@@ -2385,7 +2395,7 @@
         <v>1115</v>
       </c>
       <c r="C52" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D52" t="s">
         <v>17</v>
@@ -2402,7 +2412,7 @@
         <v>1116</v>
       </c>
       <c r="C53" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D53" t="s">
         <v>17</v>
@@ -2419,7 +2429,7 @@
         <v>1117</v>
       </c>
       <c r="C54" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D54" t="s">
         <v>2</v>
@@ -2436,7 +2446,7 @@
         <v>1118</v>
       </c>
       <c r="C55" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D55" t="s">
         <v>2</v>
@@ -2580,7 +2590,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B64">
         <v>1127</v>
@@ -2592,12 +2602,12 @@
         <v>2</v>
       </c>
       <c r="E64" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B65">
         <v>1128</v>
@@ -2609,7 +2619,7 @@
         <v>17</v>
       </c>
       <c r="E65" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -2645,104 +2655,104 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B68">
         <v>1132</v>
       </c>
       <c r="C68" t="s">
+        <v>177</v>
+      </c>
+      <c r="D68" t="s">
+        <v>17</v>
+      </c>
+      <c r="E68" t="s">
         <v>178</v>
-      </c>
-      <c r="D68" t="s">
-        <v>17</v>
-      </c>
-      <c r="E68" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B69">
         <v>1133</v>
       </c>
       <c r="C69" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D69" t="s">
         <v>2</v>
       </c>
       <c r="E69" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B70">
         <v>1134</v>
       </c>
       <c r="C70" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D70" t="s">
         <v>17</v>
       </c>
       <c r="E70" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B71">
         <v>1135</v>
       </c>
       <c r="C71" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D71" t="s">
         <v>2</v>
       </c>
       <c r="E71" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B72">
         <v>1136</v>
       </c>
       <c r="C72" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D72" t="s">
         <v>17</v>
       </c>
       <c r="E72" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B73">
         <v>1137</v>
       </c>
       <c r="C73" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D73" t="s">
         <v>2</v>
       </c>
       <c r="E73" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3222,117 +3232,134 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="B103">
-        <v>3001</v>
+        <v>3000</v>
       </c>
       <c r="C103" t="s">
-        <v>191</v>
+        <v>206</v>
       </c>
       <c r="D103" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E103" t="s">
-        <v>192</v>
+        <v>207</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="B104">
-        <v>3002</v>
+        <v>3001</v>
       </c>
       <c r="C104" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="D104" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E104" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B105">
-        <v>3003</v>
+        <v>3002</v>
       </c>
       <c r="C105" t="s">
+        <v>191</v>
+      </c>
+      <c r="D105" t="s">
+        <v>190</v>
+      </c>
+      <c r="E105" t="s">
         <v>195</v>
-      </c>
-      <c r="D105" t="s">
-        <v>194</v>
-      </c>
-      <c r="E105" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="B106">
-        <v>3004</v>
+        <v>3003</v>
       </c>
       <c r="C106" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D106" t="s">
-        <v>194</v>
+        <v>190</v>
+      </c>
+      <c r="E106" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B107">
-        <v>3005</v>
+        <v>3004</v>
       </c>
       <c r="C107" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D107" t="s">
-        <v>194</v>
-      </c>
-      <c r="E107" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>96</v>
+        <v>196</v>
       </c>
       <c r="B108">
-        <v>4000</v>
+        <v>3005</v>
       </c>
       <c r="C108" t="s">
-        <v>97</v>
+        <v>191</v>
       </c>
       <c r="D108" t="s">
-        <v>2</v>
+        <v>190</v>
       </c>
       <c r="E108" t="s">
-        <v>98</v>
+        <v>197</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B109">
-        <v>4001</v>
+        <v>4000</v>
       </c>
       <c r="C109" t="s">
         <v>97</v>
       </c>
       <c r="D109" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E109" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>99</v>
+      </c>
+      <c r="B110">
+        <v>4001</v>
+      </c>
+      <c r="C110" t="s">
+        <v>97</v>
+      </c>
+      <c r="D110" t="s">
+        <v>17</v>
+      </c>
+      <c r="E110" t="s">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Action log rework, untested.
</commit_message>
<xml_diff>
--- a/netcalls.xlsx
+++ b/netcalls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cc948d2fdda6f6d9/^JData Backup/Projects/C^N/UncreatedWarfare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="225" documentId="13_ncr:40009_{46A2828C-718E-41F1-A065-9491A5788052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B7DB435-EE32-4CFB-8EB8-A1795DB332B4}"/>
+  <xr:revisionPtr revIDLastSave="229" documentId="13_ncr:40009_{46A2828C-718E-41F1-A065-9491A5788052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDA6EE84-85D5-4788-8ADD-1D4BD94F43C6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3945" yWindow="9990" windowWidth="28605" windowHeight="10095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="netcalls" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="207">
   <si>
     <t>SendPlayerList</t>
   </si>
@@ -619,18 +619,6 @@
     <t>RequestFullSyncPacket</t>
   </si>
   <si>
-    <t>SendLogs</t>
-  </si>
-  <si>
-    <t>&lt;CUSTOM&gt;</t>
-  </si>
-  <si>
-    <t>AckLogs</t>
-  </si>
-  <si>
-    <t>DateTimeOffset[] received</t>
-  </si>
-  <si>
     <t>Data.NetCalls</t>
   </si>
   <si>
@@ -647,6 +635,12 @@
   </si>
   <si>
     <t>ushort syncId, int[] pks</t>
+  </si>
+  <si>
+    <t>SendLog</t>
+  </si>
+  <si>
+    <t>ActionLogMeta meta, byte[] logUtf8</t>
   </si>
 </sst>
 </file>
@@ -1195,10 +1189,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E110" totalsRowShown="0">
-  <autoFilter ref="A1:E110" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E110">
-    <sortCondition ref="B1:B110"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E109" totalsRowShown="0">
+  <autoFilter ref="A1:E109" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E109">
+    <sortCondition ref="B1:B109"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="NetCall Field Name"/>
@@ -1508,10 +1502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E110"/>
+  <dimension ref="A1:E109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E93" sqref="E93"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1684,7 +1678,7 @@
         <v>1008</v>
       </c>
       <c r="C10" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D10" t="s">
         <v>2</v>
@@ -2590,7 +2584,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="B64">
         <v>1127</v>
@@ -2602,12 +2596,12 @@
         <v>2</v>
       </c>
       <c r="E64" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>201</v>
+        <v>85</v>
       </c>
       <c r="B65">
         <v>1128</v>
@@ -2618,364 +2612,364 @@
       <c r="D65" t="s">
         <v>17</v>
       </c>
-      <c r="E65" t="s">
-        <v>202</v>
-      </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>85</v>
+        <v>162</v>
       </c>
       <c r="B66">
-        <v>1129</v>
+        <v>1131</v>
       </c>
       <c r="C66" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="D66" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E66" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="B67">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="C67" t="s">
-        <v>40</v>
+        <v>177</v>
       </c>
       <c r="D67" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E67" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B68">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="C68" t="s">
         <v>177</v>
       </c>
       <c r="D68" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E68" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="B69">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="C69" t="s">
         <v>177</v>
       </c>
       <c r="D69" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E69" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B70">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="C70" t="s">
         <v>177</v>
       </c>
       <c r="D70" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E70" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B71">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="C71" t="s">
         <v>177</v>
       </c>
       <c r="D71" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E71" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B72">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="C72" t="s">
         <v>177</v>
       </c>
       <c r="D72" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E72" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>184</v>
+        <v>110</v>
       </c>
       <c r="B73">
-        <v>1137</v>
+        <v>2000</v>
       </c>
       <c r="C73" t="s">
-        <v>177</v>
+        <v>109</v>
       </c>
       <c r="D73" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E73" t="s">
-        <v>186</v>
+        <v>24</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="B74">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="C74" t="s">
         <v>109</v>
       </c>
       <c r="D74" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E74" t="s">
-        <v>24</v>
+        <v>146</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="B75">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="C75" t="s">
         <v>109</v>
       </c>
       <c r="D75" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E75" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="B76">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="C76" t="s">
         <v>109</v>
       </c>
       <c r="D76" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E76" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B77">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="C77" t="s">
         <v>109</v>
       </c>
       <c r="D77" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E77" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="B78">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="C78" t="s">
         <v>109</v>
       </c>
       <c r="D78" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E78" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B79">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="C79" t="s">
         <v>109</v>
       </c>
       <c r="D79" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E79" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="B80">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="C80" t="s">
         <v>109</v>
       </c>
       <c r="D80" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E80" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B81">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="C81" t="s">
         <v>109</v>
       </c>
       <c r="D81" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E81" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="B82">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="C82" t="s">
         <v>109</v>
       </c>
       <c r="D82" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E82" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="B83">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="C83" t="s">
         <v>109</v>
       </c>
       <c r="D83" t="s">
-        <v>2</v>
-      </c>
-      <c r="E83" t="s">
-        <v>148</v>
+        <v>17</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="B84">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="C84" t="s">
         <v>109</v>
       </c>
       <c r="D84" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E84" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="B85">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="C85" t="s">
         <v>109</v>
       </c>
       <c r="D85" t="s">
-        <v>2</v>
-      </c>
-      <c r="E85" t="s">
-        <v>149</v>
+        <v>17</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="B86">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="C86" t="s">
         <v>109</v>
       </c>
       <c r="D86" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E86" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B87">
-        <v>2013</v>
+        <v>2019</v>
       </c>
       <c r="C87" t="s">
         <v>109</v>
@@ -2984,49 +2978,49 @@
         <v>2</v>
       </c>
       <c r="E87" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="B88">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C88" t="s">
         <v>109</v>
       </c>
       <c r="D88" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E88" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="B89">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C89" t="s">
         <v>109</v>
       </c>
       <c r="D89" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E89" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B90">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C90" t="s">
         <v>109</v>
@@ -3035,15 +3029,15 @@
         <v>2</v>
       </c>
       <c r="E90" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B91">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C91" t="s">
         <v>109</v>
@@ -3052,15 +3046,15 @@
         <v>2</v>
       </c>
       <c r="E91" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B92">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C92" t="s">
         <v>109</v>
@@ -3069,32 +3063,29 @@
         <v>2</v>
       </c>
       <c r="E92" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="B93">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="C93" t="s">
         <v>109</v>
       </c>
       <c r="D93" t="s">
-        <v>2</v>
-      </c>
-      <c r="E93" t="s">
-        <v>155</v>
+        <v>17</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B94">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="C94" t="s">
         <v>109</v>
@@ -3105,10 +3096,10 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B95">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="C95" t="s">
         <v>109</v>
@@ -3119,10 +3110,10 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B96">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="C96" t="s">
         <v>109</v>
@@ -3133,24 +3124,27 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="B97">
-        <v>2028</v>
+        <v>2090</v>
       </c>
       <c r="C97" t="s">
         <v>109</v>
       </c>
       <c r="D97" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E97" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B98">
-        <v>2090</v>
+        <v>2091</v>
       </c>
       <c r="C98" t="s">
         <v>109</v>
@@ -3159,15 +3153,15 @@
         <v>2</v>
       </c>
       <c r="E98" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B99">
-        <v>2091</v>
+        <v>2092</v>
       </c>
       <c r="C99" t="s">
         <v>109</v>
@@ -3176,15 +3170,15 @@
         <v>2</v>
       </c>
       <c r="E99" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B100">
-        <v>2092</v>
+        <v>2093</v>
       </c>
       <c r="C100" t="s">
         <v>109</v>
@@ -3193,15 +3187,15 @@
         <v>2</v>
       </c>
       <c r="E100" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B101">
-        <v>2093</v>
+        <v>2094</v>
       </c>
       <c r="C101" t="s">
         <v>109</v>
@@ -3210,66 +3204,66 @@
         <v>2</v>
       </c>
       <c r="E101" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>138</v>
+        <v>200</v>
       </c>
       <c r="B102">
-        <v>2094</v>
+        <v>3000</v>
       </c>
       <c r="C102" t="s">
-        <v>109</v>
+        <v>202</v>
       </c>
       <c r="D102" t="s">
-        <v>2</v>
+        <v>190</v>
       </c>
       <c r="E102" t="s">
-        <v>159</v>
+        <v>203</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B103">
-        <v>3000</v>
+        <v>3001</v>
       </c>
       <c r="C103" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D103" t="s">
         <v>190</v>
       </c>
       <c r="E103" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="B104">
-        <v>3001</v>
+        <v>3002</v>
       </c>
       <c r="C104" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="D104" t="s">
         <v>190</v>
       </c>
       <c r="E104" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B105">
-        <v>3002</v>
+        <v>3003</v>
       </c>
       <c r="C105" t="s">
         <v>191</v>
@@ -3278,15 +3272,15 @@
         <v>190</v>
       </c>
       <c r="E105" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="B106">
-        <v>3003</v>
+        <v>3004</v>
       </c>
       <c r="C106" t="s">
         <v>191</v>
@@ -3294,16 +3288,13 @@
       <c r="D106" t="s">
         <v>190</v>
       </c>
-      <c r="E106" t="s">
-        <v>192</v>
-      </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B107">
-        <v>3004</v>
+        <v>3005</v>
       </c>
       <c r="C107" t="s">
         <v>191</v>
@@ -3311,55 +3302,41 @@
       <c r="D107" t="s">
         <v>190</v>
       </c>
+      <c r="E107" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>196</v>
+        <v>96</v>
       </c>
       <c r="B108">
-        <v>3005</v>
+        <v>4000</v>
       </c>
       <c r="C108" t="s">
-        <v>191</v>
+        <v>97</v>
       </c>
       <c r="D108" t="s">
-        <v>190</v>
+        <v>2</v>
       </c>
       <c r="E108" t="s">
-        <v>197</v>
+        <v>98</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B109">
-        <v>4000</v>
+        <v>4001</v>
       </c>
       <c r="C109" t="s">
         <v>97</v>
       </c>
       <c r="D109" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E109" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>99</v>
-      </c>
-      <c r="B110">
-        <v>4001</v>
-      </c>
-      <c r="C110" t="s">
-        <v>97</v>
-      </c>
-      <c r="D110" t="s">
-        <v>17</v>
-      </c>
-      <c r="E110" t="s">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working and highly optimized action log, report player from discord support.
</commit_message>
<xml_diff>
--- a/netcalls.xlsx
+++ b/netcalls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cc948d2fdda6f6d9/^JData Backup/Projects/C^N/UncreatedWarfare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="229" documentId="13_ncr:40009_{46A2828C-718E-41F1-A065-9491A5788052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDA6EE84-85D5-4788-8ADD-1D4BD94F43C6}"/>
+  <xr:revisionPtr revIDLastSave="238" documentId="13_ncr:40009_{46A2828C-718E-41F1-A065-9491A5788052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA4F7E57-E87E-4170-BBEC-2C49166952AC}"/>
   <bookViews>
     <workbookView xWindow="3945" yWindow="9990" windowWidth="28605" windowHeight="10095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="209">
   <si>
     <t>SendPlayerList</t>
   </si>
@@ -641,6 +641,12 @@
   </si>
   <si>
     <t>ActionLogMeta meta, byte[] logUtf8</t>
+  </si>
+  <si>
+    <t>RequestReport</t>
+  </si>
+  <si>
+    <t>ulong player, ulong admin, string message, EReportType type</t>
   </si>
 </sst>
 </file>
@@ -1189,10 +1195,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E109" totalsRowShown="0">
-  <autoFilter ref="A1:E109" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E109">
-    <sortCondition ref="B1:B109"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E110" totalsRowShown="0">
+  <autoFilter ref="A1:E110" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E110">
+    <sortCondition ref="B1:B110"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="NetCall Field Name"/>
@@ -1502,10 +1508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E109"/>
+  <dimension ref="A1:E110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E111" sqref="E111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3340,6 +3346,23 @@
         <v>100</v>
       </c>
     </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>207</v>
+      </c>
+      <c r="B110">
+        <v>4002</v>
+      </c>
+      <c r="C110" t="s">
+        <v>97</v>
+      </c>
+      <c r="D110" t="s">
+        <v>17</v>
+      </c>
+      <c r="E110" t="s">
+        <v>208</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added player list logic
</commit_message>
<xml_diff>
--- a/netcalls.xlsx
+++ b/netcalls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cc948d2fdda6f6d9/^JData Backup/Projects/C^N/UncreatedWarfare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="238" documentId="13_ncr:40009_{46A2828C-718E-41F1-A065-9491A5788052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA4F7E57-E87E-4170-BBEC-2C49166952AC}"/>
+  <xr:revisionPtr revIDLastSave="244" documentId="13_ncr:40009_{46A2828C-718E-41F1-A065-9491A5788052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0025119-0D0A-4CFA-95BE-09620027F397}"/>
   <bookViews>
-    <workbookView xWindow="3945" yWindow="9990" windowWidth="28605" windowHeight="10095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="netcalls" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="211">
   <si>
     <t>SendPlayerList</t>
   </si>
@@ -647,6 +647,12 @@
   </si>
   <si>
     <t>ulong player, ulong admin, string message, EReportType type</t>
+  </si>
+  <si>
+    <t>PlayerList.NetCalls</t>
+  </si>
+  <si>
+    <t>SendTickPlayerList</t>
   </si>
 </sst>
 </file>
@@ -1195,10 +1201,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E110" totalsRowShown="0">
-  <autoFilter ref="A1:E110" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E110">
-    <sortCondition ref="B1:B110"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E111" totalsRowShown="0">
+  <autoFilter ref="A1:E111" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E111">
+    <sortCondition ref="B1:B111"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="NetCall Field Name"/>
@@ -1500,7 +1506,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1508,10 +1514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E110"/>
+  <dimension ref="A1:E111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E111" sqref="E111"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2185,27 +2191,24 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>210</v>
       </c>
       <c r="B40">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="C40" t="s">
-        <v>5</v>
+        <v>209</v>
       </c>
       <c r="D40" t="s">
-        <v>17</v>
-      </c>
-      <c r="E40" t="s">
-        <v>47</v>
+        <v>190</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B41">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="C41" t="s">
         <v>5</v>
@@ -2219,10 +2222,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B42">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="C42" t="s">
         <v>5</v>
@@ -2236,10 +2239,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B43">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="C43" t="s">
         <v>5</v>
@@ -2253,10 +2256,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B44">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="C44" t="s">
         <v>5</v>
@@ -2270,10 +2273,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B45">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="C45" t="s">
         <v>5</v>
@@ -2287,27 +2290,27 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B46">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="C46" t="s">
-        <v>177</v>
+        <v>5</v>
       </c>
       <c r="D46" t="s">
         <v>17</v>
       </c>
       <c r="E46" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>166</v>
+        <v>59</v>
       </c>
       <c r="B47">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="C47" t="s">
         <v>177</v>
@@ -2316,100 +2319,100 @@
         <v>17</v>
       </c>
       <c r="E47" t="s">
-        <v>169</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B48">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="C48" t="s">
         <v>177</v>
       </c>
       <c r="D48" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E48" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>61</v>
+        <v>167</v>
       </c>
       <c r="B49">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="C49" t="s">
-        <v>5</v>
+        <v>177</v>
       </c>
       <c r="D49" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E49" t="s">
-        <v>47</v>
+        <v>168</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B50">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="C50" t="s">
-        <v>177</v>
+        <v>5</v>
       </c>
       <c r="D50" t="s">
         <v>17</v>
       </c>
       <c r="E50" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B51">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C51" t="s">
         <v>177</v>
       </c>
       <c r="D51" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E51" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B52">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="C52" t="s">
         <v>177</v>
       </c>
       <c r="D52" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E52" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B53">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="C53" t="s">
         <v>177</v>
@@ -2418,32 +2421,32 @@
         <v>17</v>
       </c>
       <c r="E53" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B54">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="C54" t="s">
         <v>177</v>
       </c>
       <c r="D54" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E54" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B55">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="C55" t="s">
         <v>177</v>
@@ -2452,530 +2455,530 @@
         <v>2</v>
       </c>
       <c r="E55" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B56">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="C56" t="s">
-        <v>32</v>
+        <v>177</v>
       </c>
       <c r="D56" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E56" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="B57">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="C57" t="s">
         <v>32</v>
       </c>
       <c r="D57" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E57" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="B58">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="C58" t="s">
         <v>32</v>
       </c>
       <c r="D58" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E58" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="B59">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="C59" t="s">
         <v>32</v>
       </c>
       <c r="D59" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E59" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="B60">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="C60" t="s">
         <v>32</v>
       </c>
       <c r="D60" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E60" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B61">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C61" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="D61" t="s">
         <v>17</v>
-      </c>
-      <c r="E61" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B62">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C62" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D62" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E62" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B63">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="C63" t="s">
         <v>80</v>
       </c>
       <c r="D63" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E63" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>205</v>
+        <v>82</v>
       </c>
       <c r="B64">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C64" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D64" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E64" t="s">
-        <v>206</v>
+        <v>83</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>85</v>
+        <v>205</v>
       </c>
       <c r="B65">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="C65" t="s">
         <v>84</v>
       </c>
       <c r="D65" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E65" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>162</v>
+        <v>85</v>
       </c>
       <c r="B66">
-        <v>1131</v>
+        <v>1128</v>
       </c>
       <c r="C66" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="D66" t="s">
-        <v>2</v>
-      </c>
-      <c r="E66" t="s">
-        <v>163</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="B67">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="C67" t="s">
-        <v>177</v>
+        <v>40</v>
       </c>
       <c r="D67" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E67" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B68">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="C68" t="s">
         <v>177</v>
       </c>
       <c r="D68" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E68" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B69">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="C69" t="s">
         <v>177</v>
       </c>
       <c r="D69" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E69" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B70">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="C70" t="s">
         <v>177</v>
       </c>
       <c r="D70" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E70" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B71">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="C71" t="s">
         <v>177</v>
       </c>
       <c r="D71" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E71" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B72">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="C72" t="s">
         <v>177</v>
       </c>
       <c r="D72" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E72" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>110</v>
+        <v>184</v>
       </c>
       <c r="B73">
-        <v>2000</v>
+        <v>1137</v>
       </c>
       <c r="C73" t="s">
-        <v>109</v>
+        <v>177</v>
       </c>
       <c r="D73" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E73" t="s">
-        <v>24</v>
+        <v>186</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B74">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="C74" t="s">
         <v>109</v>
       </c>
       <c r="D74" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E74" t="s">
-        <v>146</v>
+        <v>24</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="B75">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="C75" t="s">
         <v>109</v>
       </c>
       <c r="D75" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E75" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B76">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="C76" t="s">
         <v>109</v>
       </c>
       <c r="D76" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E76" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="B77">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="C77" t="s">
         <v>109</v>
       </c>
       <c r="D77" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E77" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="B78">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="C78" t="s">
         <v>109</v>
       </c>
       <c r="D78" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E78" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="B79">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="C79" t="s">
         <v>109</v>
       </c>
       <c r="D79" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E79" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="B80">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="C80" t="s">
         <v>109</v>
       </c>
       <c r="D80" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E80" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="B81">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="C81" t="s">
         <v>109</v>
       </c>
       <c r="D81" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E81" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="B82">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="C82" t="s">
         <v>109</v>
       </c>
       <c r="D82" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E82" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="B83">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="C83" t="s">
         <v>109</v>
       </c>
       <c r="D83" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E83" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="B84">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="C84" t="s">
         <v>109</v>
       </c>
       <c r="D84" t="s">
-        <v>2</v>
-      </c>
-      <c r="E84" t="s">
-        <v>149</v>
+        <v>17</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="B85">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="C85" t="s">
         <v>109</v>
       </c>
       <c r="D85" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E85" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="B86">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="C86" t="s">
         <v>109</v>
       </c>
       <c r="D86" t="s">
-        <v>2</v>
-      </c>
-      <c r="E86" t="s">
-        <v>150</v>
+        <v>17</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B87">
-        <v>2019</v>
+        <v>2013</v>
       </c>
       <c r="C87" t="s">
         <v>109</v>
@@ -2984,49 +2987,49 @@
         <v>2</v>
       </c>
       <c r="E87" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="B88">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="C88" t="s">
         <v>109</v>
       </c>
       <c r="D88" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E88" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="B89">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C89" t="s">
         <v>109</v>
       </c>
       <c r="D89" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E89" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B90">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C90" t="s">
         <v>109</v>
@@ -3035,15 +3038,15 @@
         <v>2</v>
       </c>
       <c r="E90" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B91">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C91" t="s">
         <v>109</v>
@@ -3052,15 +3055,15 @@
         <v>2</v>
       </c>
       <c r="E91" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B92">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C92" t="s">
         <v>109</v>
@@ -3069,29 +3072,32 @@
         <v>2</v>
       </c>
       <c r="E92" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="B93">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="C93" t="s">
         <v>109</v>
       </c>
       <c r="D93" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E93" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B94">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="C94" t="s">
         <v>109</v>
@@ -3102,10 +3108,10 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B95">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="C95" t="s">
         <v>109</v>
@@ -3116,10 +3122,10 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B96">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="C96" t="s">
         <v>109</v>
@@ -3130,27 +3136,24 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="B97">
-        <v>2090</v>
+        <v>2028</v>
       </c>
       <c r="C97" t="s">
         <v>109</v>
       </c>
       <c r="D97" t="s">
-        <v>2</v>
-      </c>
-      <c r="E97" t="s">
-        <v>156</v>
+        <v>17</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B98">
-        <v>2091</v>
+        <v>2090</v>
       </c>
       <c r="C98" t="s">
         <v>109</v>
@@ -3159,15 +3162,15 @@
         <v>2</v>
       </c>
       <c r="E98" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B99">
-        <v>2092</v>
+        <v>2091</v>
       </c>
       <c r="C99" t="s">
         <v>109</v>
@@ -3176,15 +3179,15 @@
         <v>2</v>
       </c>
       <c r="E99" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B100">
-        <v>2093</v>
+        <v>2092</v>
       </c>
       <c r="C100" t="s">
         <v>109</v>
@@ -3193,15 +3196,15 @@
         <v>2</v>
       </c>
       <c r="E100" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B101">
-        <v>2094</v>
+        <v>2093</v>
       </c>
       <c r="C101" t="s">
         <v>109</v>
@@ -3210,32 +3213,32 @@
         <v>2</v>
       </c>
       <c r="E101" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>200</v>
+        <v>138</v>
       </c>
       <c r="B102">
-        <v>3000</v>
+        <v>2094</v>
       </c>
       <c r="C102" t="s">
-        <v>202</v>
+        <v>109</v>
       </c>
       <c r="D102" t="s">
-        <v>190</v>
+        <v>2</v>
       </c>
       <c r="E102" t="s">
-        <v>203</v>
+        <v>159</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B103">
-        <v>3001</v>
+        <v>3000</v>
       </c>
       <c r="C103" t="s">
         <v>202</v>
@@ -3244,32 +3247,32 @@
         <v>190</v>
       </c>
       <c r="E103" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="B104">
-        <v>3002</v>
+        <v>3001</v>
       </c>
       <c r="C104" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="D104" t="s">
         <v>190</v>
       </c>
       <c r="E104" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B105">
-        <v>3003</v>
+        <v>3002</v>
       </c>
       <c r="C105" t="s">
         <v>191</v>
@@ -3278,15 +3281,15 @@
         <v>190</v>
       </c>
       <c r="E105" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B106">
-        <v>3004</v>
+        <v>3003</v>
       </c>
       <c r="C106" t="s">
         <v>191</v>
@@ -3294,13 +3297,16 @@
       <c r="D106" t="s">
         <v>190</v>
       </c>
+      <c r="E106" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B107">
-        <v>3005</v>
+        <v>3004</v>
       </c>
       <c r="C107" t="s">
         <v>191</v>
@@ -3308,50 +3314,47 @@
       <c r="D107" t="s">
         <v>190</v>
       </c>
-      <c r="E107" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>96</v>
+        <v>196</v>
       </c>
       <c r="B108">
-        <v>4000</v>
+        <v>3005</v>
       </c>
       <c r="C108" t="s">
-        <v>97</v>
+        <v>191</v>
       </c>
       <c r="D108" t="s">
-        <v>2</v>
+        <v>190</v>
       </c>
       <c r="E108" t="s">
-        <v>98</v>
+        <v>197</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B109">
-        <v>4001</v>
+        <v>4000</v>
       </c>
       <c r="C109" t="s">
         <v>97</v>
       </c>
       <c r="D109" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E109" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>207</v>
+        <v>99</v>
       </c>
       <c r="B110">
-        <v>4002</v>
+        <v>4001</v>
       </c>
       <c r="C110" t="s">
         <v>97</v>
@@ -3360,6 +3363,23 @@
         <v>17</v>
       </c>
       <c r="E110" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>207</v>
+      </c>
+      <c r="B111">
+        <v>4002</v>
+      </c>
+      <c r="C111" t="s">
+        <v>97</v>
+      </c>
+      <c r="D111" t="s">
+        <v>17</v>
+      </c>
+      <c r="E111" t="s">
         <v>208</v>
       </c>
     </row>

</xml_diff>

<commit_message>
nitro boost detection server-side support
</commit_message>
<xml_diff>
--- a/netcalls.xlsx
+++ b/netcalls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cc948d2fdda6f6d9/^JData Backup/Projects/C^N/UncreatedWarfare/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\UncreatedWarfare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="244" documentId="13_ncr:40009_{46A2828C-718E-41F1-A065-9491A5788052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0025119-0D0A-4CFA-95BE-09620027F397}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA756BD-660B-4C46-8D4F-13C7EDA5CCF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="6675" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="netcalls" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="217">
   <si>
     <t>SendPlayerList</t>
   </si>
@@ -653,6 +653,24 @@
   </si>
   <si>
     <t>SendTickPlayerList</t>
+  </si>
+  <si>
+    <t>ulong[] players</t>
+  </si>
+  <si>
+    <t>RequestIsNitroBoosting</t>
+  </si>
+  <si>
+    <t>SendNitroBoostingUpdated</t>
+  </si>
+  <si>
+    <t>RespondIsNitroBoosting</t>
+  </si>
+  <si>
+    <t>byte[] response (0=not, 1=is, 2=unclear)</t>
+  </si>
+  <si>
+    <t>ulong[] player, byte[] code (0=not, 1=is, 2=unclear)</t>
   </si>
 </sst>
 </file>
@@ -1196,15 +1214,11 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E111" totalsRowShown="0">
-  <autoFilter ref="A1:E111" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E111">
-    <sortCondition ref="B1:B111"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E114" totalsRowShown="0">
+  <autoFilter ref="A1:E114" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E114">
+    <sortCondition ref="B1:B114"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="NetCall Field Name"/>
@@ -1506,7 +1520,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1514,10 +1528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E111"/>
+  <dimension ref="A1:E114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2760,242 +2774,245 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>110</v>
+        <v>212</v>
       </c>
       <c r="B74">
-        <v>2000</v>
+        <v>1138</v>
       </c>
       <c r="C74" t="s">
-        <v>109</v>
+        <v>177</v>
       </c>
       <c r="D74" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E74" t="s">
-        <v>24</v>
+        <v>211</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>124</v>
+        <v>214</v>
       </c>
       <c r="B75">
-        <v>2001</v>
+        <v>1139</v>
       </c>
       <c r="C75" t="s">
-        <v>109</v>
+        <v>177</v>
       </c>
       <c r="D75" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E75" t="s">
-        <v>146</v>
+        <v>215</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>111</v>
+        <v>213</v>
       </c>
       <c r="B76">
-        <v>2002</v>
+        <v>1140</v>
       </c>
       <c r="C76" t="s">
-        <v>109</v>
+        <v>177</v>
       </c>
       <c r="D76" t="s">
         <v>17</v>
       </c>
       <c r="E76" t="s">
-        <v>139</v>
+        <v>216</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B77">
-        <v>2003</v>
+        <v>2000</v>
       </c>
       <c r="C77" t="s">
         <v>109</v>
       </c>
       <c r="D77" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E77" t="s">
-        <v>144</v>
+        <v>24</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="B78">
-        <v>2004</v>
+        <v>2001</v>
       </c>
       <c r="C78" t="s">
         <v>109</v>
       </c>
       <c r="D78" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E78" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B79">
-        <v>2005</v>
+        <v>2002</v>
       </c>
       <c r="C79" t="s">
         <v>109</v>
       </c>
       <c r="D79" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E79" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B80">
-        <v>2006</v>
+        <v>2003</v>
       </c>
       <c r="C80" t="s">
         <v>109</v>
       </c>
       <c r="D80" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E80" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="B81">
-        <v>2007</v>
+        <v>2004</v>
       </c>
       <c r="C81" t="s">
         <v>109</v>
       </c>
       <c r="D81" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E81" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="B82">
-        <v>2008</v>
+        <v>2005</v>
       </c>
       <c r="C82" t="s">
         <v>109</v>
       </c>
       <c r="D82" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E82" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="B83">
-        <v>2009</v>
+        <v>2006</v>
       </c>
       <c r="C83" t="s">
         <v>109</v>
       </c>
       <c r="D83" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E83" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="B84">
-        <v>2010</v>
+        <v>2007</v>
       </c>
       <c r="C84" t="s">
         <v>109</v>
       </c>
       <c r="D84" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E84" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="B85">
-        <v>2011</v>
+        <v>2008</v>
       </c>
       <c r="C85" t="s">
         <v>109</v>
       </c>
       <c r="D85" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E85" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="B86">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="C86" t="s">
         <v>109</v>
       </c>
       <c r="D86" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E86" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="B87">
-        <v>2013</v>
+        <v>2010</v>
       </c>
       <c r="C87" t="s">
         <v>109</v>
       </c>
       <c r="D87" t="s">
-        <v>2</v>
-      </c>
-      <c r="E87" t="s">
-        <v>150</v>
+        <v>17</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B88">
-        <v>2019</v>
+        <v>2011</v>
       </c>
       <c r="C88" t="s">
         <v>109</v>
@@ -3004,15 +3021,15 @@
         <v>2</v>
       </c>
       <c r="E88" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B89">
-        <v>2020</v>
+        <v>2012</v>
       </c>
       <c r="C89" t="s">
         <v>109</v>
@@ -3020,16 +3037,13 @@
       <c r="D89" t="s">
         <v>17</v>
       </c>
-      <c r="E89" t="s">
-        <v>143</v>
-      </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B90">
-        <v>2021</v>
+        <v>2013</v>
       </c>
       <c r="C90" t="s">
         <v>109</v>
@@ -3038,15 +3052,15 @@
         <v>2</v>
       </c>
       <c r="E90" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B91">
-        <v>2022</v>
+        <v>2019</v>
       </c>
       <c r="C91" t="s">
         <v>109</v>
@@ -3055,32 +3069,32 @@
         <v>2</v>
       </c>
       <c r="E91" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="B92">
-        <v>2023</v>
+        <v>2020</v>
       </c>
       <c r="C92" t="s">
         <v>109</v>
       </c>
       <c r="D92" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E92" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B93">
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="C93" t="s">
         <v>109</v>
@@ -3089,57 +3103,66 @@
         <v>2</v>
       </c>
       <c r="E93" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="B94">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="C94" t="s">
         <v>109</v>
       </c>
       <c r="D94" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E94" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="B95">
-        <v>2026</v>
+        <v>2023</v>
       </c>
       <c r="C95" t="s">
         <v>109</v>
       </c>
       <c r="D95" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E95" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="B96">
-        <v>2027</v>
+        <v>2024</v>
       </c>
       <c r="C96" t="s">
         <v>109</v>
       </c>
       <c r="D96" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E96" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B97">
-        <v>2028</v>
+        <v>2025</v>
       </c>
       <c r="C97" t="s">
         <v>109</v>
@@ -3150,61 +3173,52 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B98">
-        <v>2090</v>
+        <v>2026</v>
       </c>
       <c r="C98" t="s">
         <v>109</v>
       </c>
       <c r="D98" t="s">
-        <v>2</v>
-      </c>
-      <c r="E98" t="s">
-        <v>156</v>
+        <v>17</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="B99">
-        <v>2091</v>
+        <v>2027</v>
       </c>
       <c r="C99" t="s">
         <v>109</v>
       </c>
       <c r="D99" t="s">
-        <v>2</v>
-      </c>
-      <c r="E99" t="s">
-        <v>145</v>
+        <v>17</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B100">
-        <v>2092</v>
+        <v>2028</v>
       </c>
       <c r="C100" t="s">
         <v>109</v>
       </c>
       <c r="D100" t="s">
-        <v>2</v>
-      </c>
-      <c r="E100" t="s">
-        <v>157</v>
+        <v>17</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B101">
-        <v>2093</v>
+        <v>2090</v>
       </c>
       <c r="C101" t="s">
         <v>109</v>
@@ -3213,15 +3227,15 @@
         <v>2</v>
       </c>
       <c r="E101" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B102">
-        <v>2094</v>
+        <v>2091</v>
       </c>
       <c r="C102" t="s">
         <v>109</v>
@@ -3230,97 +3244,100 @@
         <v>2</v>
       </c>
       <c r="E102" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>200</v>
+        <v>136</v>
       </c>
       <c r="B103">
-        <v>3000</v>
+        <v>2092</v>
       </c>
       <c r="C103" t="s">
-        <v>202</v>
+        <v>109</v>
       </c>
       <c r="D103" t="s">
-        <v>190</v>
+        <v>2</v>
       </c>
       <c r="E103" t="s">
-        <v>203</v>
+        <v>157</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>201</v>
+        <v>137</v>
       </c>
       <c r="B104">
-        <v>3001</v>
+        <v>2093</v>
       </c>
       <c r="C104" t="s">
-        <v>202</v>
+        <v>109</v>
       </c>
       <c r="D104" t="s">
-        <v>190</v>
+        <v>2</v>
       </c>
       <c r="E104" t="s">
-        <v>204</v>
+        <v>158</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>194</v>
+        <v>138</v>
       </c>
       <c r="B105">
-        <v>3002</v>
+        <v>2094</v>
       </c>
       <c r="C105" t="s">
-        <v>191</v>
+        <v>109</v>
       </c>
       <c r="D105" t="s">
-        <v>190</v>
+        <v>2</v>
       </c>
       <c r="E105" t="s">
-        <v>195</v>
+        <v>159</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="B106">
-        <v>3003</v>
+        <v>3000</v>
       </c>
       <c r="C106" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="D106" t="s">
         <v>190</v>
       </c>
       <c r="E106" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B107">
-        <v>3004</v>
+        <v>3001</v>
       </c>
       <c r="C107" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="D107" t="s">
         <v>190</v>
       </c>
+      <c r="E107" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B108">
-        <v>3005</v>
+        <v>3002</v>
       </c>
       <c r="C108" t="s">
         <v>191</v>
@@ -3329,57 +3346,105 @@
         <v>190</v>
       </c>
       <c r="E108" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>96</v>
+        <v>193</v>
       </c>
       <c r="B109">
-        <v>4000</v>
+        <v>3003</v>
       </c>
       <c r="C109" t="s">
-        <v>97</v>
+        <v>191</v>
       </c>
       <c r="D109" t="s">
-        <v>2</v>
+        <v>190</v>
       </c>
       <c r="E109" t="s">
-        <v>98</v>
+        <v>192</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>99</v>
+        <v>198</v>
       </c>
       <c r="B110">
-        <v>4001</v>
+        <v>3004</v>
       </c>
       <c r="C110" t="s">
-        <v>97</v>
+        <v>191</v>
       </c>
       <c r="D110" t="s">
-        <v>17</v>
-      </c>
-      <c r="E110" t="s">
-        <v>100</v>
+        <v>190</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
+        <v>196</v>
+      </c>
+      <c r="B111">
+        <v>3005</v>
+      </c>
+      <c r="C111" t="s">
+        <v>191</v>
+      </c>
+      <c r="D111" t="s">
+        <v>190</v>
+      </c>
+      <c r="E111" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>96</v>
+      </c>
+      <c r="B112">
+        <v>4000</v>
+      </c>
+      <c r="C112" t="s">
+        <v>97</v>
+      </c>
+      <c r="D112" t="s">
+        <v>2</v>
+      </c>
+      <c r="E112" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>99</v>
+      </c>
+      <c r="B113">
+        <v>4001</v>
+      </c>
+      <c r="C113" t="s">
+        <v>97</v>
+      </c>
+      <c r="D113" t="s">
+        <v>17</v>
+      </c>
+      <c r="E113" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>207</v>
       </c>
-      <c r="B111">
+      <c r="B114">
         <v>4002</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C114" t="s">
         <v>97</v>
       </c>
-      <c r="D111" t="s">
-        <v>17</v>
-      </c>
-      <c r="E111" t="s">
+      <c r="D114" t="s">
+        <v>17</v>
+      </c>
+      <c r="E114" t="s">
         <v>208</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixes from beta test, Added a system for having custom layouts for your kits (overriding where items are placed in your inventory). So far does not work with clothes, for simplicity i would like to add the ability to swap clothes THAT DO NOT HAVE STORAGE. There is currently an issue that needs fixing where you can have multiple transformations of the same item which can cause issues. todo investigate.
</commit_message>
<xml_diff>
--- a/netcalls.xlsx
+++ b/netcalls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\UncreatedWarfare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA756BD-660B-4C46-8D4F-13C7EDA5CCF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D844CB-D589-4D45-8D82-E923DC697BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="6675" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="netcalls" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="223">
   <si>
     <t>SendPlayerList</t>
   </si>
@@ -671,6 +671,24 @@
   </si>
   <si>
     <t>ulong[] player, byte[] code (0=not, 1=is, 2=unclear)</t>
+  </si>
+  <si>
+    <t>MulticastKitDeleted</t>
+  </si>
+  <si>
+    <t>KitSync.NetCalls</t>
+  </si>
+  <si>
+    <t>int pk</t>
+  </si>
+  <si>
+    <t>MulticastKitAccessChanged</t>
+  </si>
+  <si>
+    <t>ulong steamId</t>
+  </si>
+  <si>
+    <t>MulticastKitUpdated</t>
   </si>
 </sst>
 </file>
@@ -1215,10 +1233,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E114" totalsRowShown="0">
-  <autoFilter ref="A1:E114" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E114">
-    <sortCondition ref="B1:B114"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E117" totalsRowShown="0">
+  <autoFilter ref="A1:E117" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E117">
+    <sortCondition ref="B1:B117"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="NetCall Field Name"/>
@@ -1528,10 +1546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E114"/>
+  <dimension ref="A1:E117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3399,52 +3417,103 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>96</v>
+        <v>217</v>
       </c>
       <c r="B112">
-        <v>4000</v>
+        <v>3006</v>
       </c>
       <c r="C112" t="s">
-        <v>97</v>
+        <v>218</v>
       </c>
       <c r="D112" t="s">
-        <v>2</v>
+        <v>190</v>
       </c>
       <c r="E112" t="s">
-        <v>98</v>
+        <v>219</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>99</v>
+        <v>220</v>
       </c>
       <c r="B113">
-        <v>4001</v>
+        <v>3007</v>
       </c>
       <c r="C113" t="s">
-        <v>97</v>
+        <v>218</v>
       </c>
       <c r="D113" t="s">
-        <v>17</v>
+        <v>190</v>
       </c>
       <c r="E113" t="s">
-        <v>100</v>
+        <v>221</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
+        <v>222</v>
+      </c>
+      <c r="B114">
+        <v>3008</v>
+      </c>
+      <c r="C114" t="s">
+        <v>218</v>
+      </c>
+      <c r="D114" t="s">
+        <v>190</v>
+      </c>
+      <c r="E114" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>96</v>
+      </c>
+      <c r="B115">
+        <v>4000</v>
+      </c>
+      <c r="C115" t="s">
+        <v>97</v>
+      </c>
+      <c r="D115" t="s">
+        <v>2</v>
+      </c>
+      <c r="E115" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>99</v>
+      </c>
+      <c r="B116">
+        <v>4001</v>
+      </c>
+      <c r="C116" t="s">
+        <v>97</v>
+      </c>
+      <c r="D116" t="s">
+        <v>17</v>
+      </c>
+      <c r="E116" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>207</v>
       </c>
-      <c r="B114">
+      <c r="B117">
         <v>4002</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C117" t="s">
         <v>97</v>
       </c>
-      <c r="D114" t="s">
-        <v>17</v>
-      </c>
-      <c r="E114" t="s">
+      <c r="D117" t="s">
+        <v>17</v>
+      </c>
+      <c r="E117" t="s">
         <v>208</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Default loadout layouts for kits.
</commit_message>
<xml_diff>
--- a/netcalls.xlsx
+++ b/netcalls.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\UncreatedWarfare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D844CB-D589-4D45-8D82-E923DC697BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC7196EB-493B-4F42-AF7F-694759D0D446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="6675" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="netcalls" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="227">
   <si>
     <t>SendPlayerList</t>
   </si>
@@ -529,9 +529,6 @@
     <t>string kitName, int signIndex</t>
   </si>
   <si>
-    <t>ulong fromPlayer, ulong player, byte team, EClass @class, string displayName</t>
-  </si>
-  <si>
     <t>RequestSetKitAccess</t>
   </si>
   <si>
@@ -689,6 +686,21 @@
   </si>
   <si>
     <t>MulticastKitUpdated</t>
+  </si>
+  <si>
+    <t>RequestUnlockLoadout</t>
+  </si>
+  <si>
+    <t>RequestUpgradeLoadout</t>
+  </si>
+  <si>
+    <t>ulong fromPlayer, ulong player, string loadoutName</t>
+  </si>
+  <si>
+    <t>ulong fromPlayer, ulong player, Class @class, string displayName</t>
+  </si>
+  <si>
+    <t>ulong fromPlayer, ulong player, Class @class, string loadoutName</t>
   </si>
 </sst>
 </file>
@@ -1233,10 +1245,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E117" totalsRowShown="0">
-  <autoFilter ref="A1:E117" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E117">
-    <sortCondition ref="B1:B117"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E119" totalsRowShown="0">
+  <autoFilter ref="A1:E119" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E119">
+    <sortCondition ref="B1:B119"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="NetCall Field Name"/>
@@ -1546,10 +1558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E117"/>
+  <dimension ref="A1:E119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E106" sqref="E106"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1722,7 +1734,7 @@
         <v>1008</v>
       </c>
       <c r="C10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D10" t="s">
         <v>2</v>
@@ -1920,7 +1932,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B22">
         <v>1020</v>
@@ -1932,12 +1944,12 @@
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B23">
         <v>1021</v>
@@ -1949,7 +1961,7 @@
         <v>17</v>
       </c>
       <c r="E23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2189,50 +2201,50 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B38">
         <v>1100</v>
       </c>
       <c r="C38" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D38" t="s">
         <v>17</v>
       </c>
       <c r="E38" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B39">
         <v>1101</v>
       </c>
       <c r="C39" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D39" t="s">
         <v>2</v>
       </c>
       <c r="E39" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B40">
         <v>1102</v>
       </c>
       <c r="C40" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D40" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2345,7 +2357,7 @@
         <v>1109</v>
       </c>
       <c r="C47" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D47" t="s">
         <v>17</v>
@@ -2362,13 +2374,13 @@
         <v>1110</v>
       </c>
       <c r="C48" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D48" t="s">
         <v>17</v>
       </c>
       <c r="E48" t="s">
-        <v>169</v>
+        <v>225</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -2379,7 +2391,7 @@
         <v>1111</v>
       </c>
       <c r="C49" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D49" t="s">
         <v>2</v>
@@ -2413,7 +2425,7 @@
         <v>1113</v>
       </c>
       <c r="C51" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D51" t="s">
         <v>17</v>
@@ -2430,7 +2442,7 @@
         <v>1114</v>
       </c>
       <c r="C52" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D52" t="s">
         <v>2</v>
@@ -2447,7 +2459,7 @@
         <v>1115</v>
       </c>
       <c r="C53" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D53" t="s">
         <v>17</v>
@@ -2464,7 +2476,7 @@
         <v>1116</v>
       </c>
       <c r="C54" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D54" t="s">
         <v>17</v>
@@ -2481,7 +2493,7 @@
         <v>1117</v>
       </c>
       <c r="C55" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D55" t="s">
         <v>2</v>
@@ -2498,7 +2510,7 @@
         <v>1118</v>
       </c>
       <c r="C56" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D56" t="s">
         <v>2</v>
@@ -2642,7 +2654,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B65">
         <v>1127</v>
@@ -2654,7 +2666,7 @@
         <v>2</v>
       </c>
       <c r="E65" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -2690,197 +2702,197 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B68">
         <v>1132</v>
       </c>
       <c r="C68" t="s">
+        <v>176</v>
+      </c>
+      <c r="D68" t="s">
+        <v>17</v>
+      </c>
+      <c r="E68" t="s">
         <v>177</v>
-      </c>
-      <c r="D68" t="s">
-        <v>17</v>
-      </c>
-      <c r="E68" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B69">
         <v>1133</v>
       </c>
       <c r="C69" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D69" t="s">
         <v>2</v>
       </c>
       <c r="E69" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B70">
         <v>1134</v>
       </c>
       <c r="C70" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D70" t="s">
         <v>17</v>
       </c>
       <c r="E70" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B71">
         <v>1135</v>
       </c>
       <c r="C71" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D71" t="s">
         <v>2</v>
       </c>
       <c r="E71" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B72">
         <v>1136</v>
       </c>
       <c r="C72" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D72" t="s">
         <v>17</v>
       </c>
       <c r="E72" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B73">
         <v>1137</v>
       </c>
       <c r="C73" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D73" t="s">
         <v>2</v>
       </c>
       <c r="E73" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B74">
         <v>1138</v>
       </c>
       <c r="C74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D74" t="s">
         <v>2</v>
       </c>
       <c r="E74" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B75">
         <v>1139</v>
       </c>
       <c r="C75" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D75" t="s">
         <v>17</v>
       </c>
       <c r="E75" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B76">
         <v>1140</v>
       </c>
       <c r="C76" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D76" t="s">
         <v>17</v>
       </c>
       <c r="E76" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>110</v>
+        <v>223</v>
       </c>
       <c r="B77">
-        <v>2000</v>
+        <v>1141</v>
       </c>
       <c r="C77" t="s">
-        <v>109</v>
+        <v>176</v>
       </c>
       <c r="D77" t="s">
         <v>17</v>
       </c>
       <c r="E77" t="s">
-        <v>24</v>
+        <v>224</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>124</v>
+        <v>222</v>
       </c>
       <c r="B78">
-        <v>2001</v>
+        <v>1142</v>
       </c>
       <c r="C78" t="s">
-        <v>109</v>
+        <v>176</v>
       </c>
       <c r="D78" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E78" t="s">
-        <v>146</v>
+        <v>226</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B79">
-        <v>2002</v>
+        <v>2000</v>
       </c>
       <c r="C79" t="s">
         <v>109</v>
@@ -2889,15 +2901,15 @@
         <v>17</v>
       </c>
       <c r="E79" t="s">
-        <v>139</v>
+        <v>24</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B80">
-        <v>2003</v>
+        <v>2001</v>
       </c>
       <c r="C80" t="s">
         <v>109</v>
@@ -2906,15 +2918,15 @@
         <v>2</v>
       </c>
       <c r="E80" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B81">
-        <v>2004</v>
+        <v>2002</v>
       </c>
       <c r="C81" t="s">
         <v>109</v>
@@ -2923,15 +2935,15 @@
         <v>17</v>
       </c>
       <c r="E81" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B82">
-        <v>2005</v>
+        <v>2003</v>
       </c>
       <c r="C82" t="s">
         <v>109</v>
@@ -2940,15 +2952,15 @@
         <v>2</v>
       </c>
       <c r="E82" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B83">
-        <v>2006</v>
+        <v>2004</v>
       </c>
       <c r="C83" t="s">
         <v>109</v>
@@ -2957,15 +2969,15 @@
         <v>17</v>
       </c>
       <c r="E83" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B84">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="C84" t="s">
         <v>109</v>
@@ -2974,15 +2986,15 @@
         <v>2</v>
       </c>
       <c r="E84" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B85">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="C85" t="s">
         <v>109</v>
@@ -2991,15 +3003,15 @@
         <v>17</v>
       </c>
       <c r="E85" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B86">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="C86" t="s">
         <v>109</v>
@@ -3008,15 +3020,15 @@
         <v>2</v>
       </c>
       <c r="E86" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B87">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="C87" t="s">
         <v>109</v>
@@ -3024,13 +3036,16 @@
       <c r="D87" t="s">
         <v>17</v>
       </c>
+      <c r="E87" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B88">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="C88" t="s">
         <v>109</v>
@@ -3039,15 +3054,15 @@
         <v>2</v>
       </c>
       <c r="E88" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B89">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="C89" t="s">
         <v>109</v>
@@ -3058,10 +3073,10 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B90">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="C90" t="s">
         <v>109</v>
@@ -3070,49 +3085,46 @@
         <v>2</v>
       </c>
       <c r="E90" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="B91">
-        <v>2019</v>
+        <v>2012</v>
       </c>
       <c r="C91" t="s">
         <v>109</v>
       </c>
       <c r="D91" t="s">
-        <v>2</v>
-      </c>
-      <c r="E91" t="s">
-        <v>151</v>
+        <v>17</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="B92">
-        <v>2020</v>
+        <v>2013</v>
       </c>
       <c r="C92" t="s">
         <v>109</v>
       </c>
       <c r="D92" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E92" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B93">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="C93" t="s">
         <v>109</v>
@@ -3121,32 +3133,32 @@
         <v>2</v>
       </c>
       <c r="E93" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="B94">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="C94" t="s">
         <v>109</v>
       </c>
       <c r="D94" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E94" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B95">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="C95" t="s">
         <v>109</v>
@@ -3155,15 +3167,15 @@
         <v>2</v>
       </c>
       <c r="E95" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B96">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C96" t="s">
         <v>109</v>
@@ -3172,43 +3184,49 @@
         <v>2</v>
       </c>
       <c r="E96" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="B97">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="C97" t="s">
         <v>109</v>
       </c>
       <c r="D97" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E97" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="B98">
-        <v>2026</v>
+        <v>2024</v>
       </c>
       <c r="C98" t="s">
         <v>109</v>
       </c>
       <c r="D98" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E98" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B99">
-        <v>2027</v>
+        <v>2025</v>
       </c>
       <c r="C99" t="s">
         <v>109</v>
@@ -3219,10 +3237,10 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B100">
-        <v>2028</v>
+        <v>2026</v>
       </c>
       <c r="C100" t="s">
         <v>109</v>
@@ -3233,44 +3251,38 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="B101">
-        <v>2090</v>
+        <v>2027</v>
       </c>
       <c r="C101" t="s">
         <v>109</v>
       </c>
       <c r="D101" t="s">
-        <v>2</v>
-      </c>
-      <c r="E101" t="s">
-        <v>156</v>
+        <v>17</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="B102">
-        <v>2091</v>
+        <v>2028</v>
       </c>
       <c r="C102" t="s">
         <v>109</v>
       </c>
       <c r="D102" t="s">
-        <v>2</v>
-      </c>
-      <c r="E102" t="s">
-        <v>145</v>
+        <v>17</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B103">
-        <v>2092</v>
+        <v>2090</v>
       </c>
       <c r="C103" t="s">
         <v>109</v>
@@ -3279,15 +3291,15 @@
         <v>2</v>
       </c>
       <c r="E103" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B104">
-        <v>2093</v>
+        <v>2091</v>
       </c>
       <c r="C104" t="s">
         <v>109</v>
@@ -3296,15 +3308,15 @@
         <v>2</v>
       </c>
       <c r="E104" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B105">
-        <v>2094</v>
+        <v>2092</v>
       </c>
       <c r="C105" t="s">
         <v>109</v>
@@ -3313,208 +3325,242 @@
         <v>2</v>
       </c>
       <c r="E105" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>200</v>
+        <v>137</v>
       </c>
       <c r="B106">
-        <v>3000</v>
+        <v>2093</v>
       </c>
       <c r="C106" t="s">
-        <v>202</v>
+        <v>109</v>
       </c>
       <c r="D106" t="s">
-        <v>190</v>
+        <v>2</v>
       </c>
       <c r="E106" t="s">
-        <v>203</v>
+        <v>158</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>201</v>
+        <v>138</v>
       </c>
       <c r="B107">
-        <v>3001</v>
+        <v>2094</v>
       </c>
       <c r="C107" t="s">
-        <v>202</v>
+        <v>109</v>
       </c>
       <c r="D107" t="s">
-        <v>190</v>
+        <v>2</v>
       </c>
       <c r="E107" t="s">
-        <v>204</v>
+        <v>159</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="B108">
-        <v>3002</v>
+        <v>3000</v>
       </c>
       <c r="C108" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="D108" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E108" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="B109">
-        <v>3003</v>
+        <v>3001</v>
       </c>
       <c r="C109" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="D109" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E109" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B110">
-        <v>3004</v>
+        <v>3002</v>
       </c>
       <c r="C110" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D110" t="s">
-        <v>190</v>
+        <v>189</v>
+      </c>
+      <c r="E110" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B111">
-        <v>3005</v>
+        <v>3003</v>
       </c>
       <c r="C111" t="s">
+        <v>190</v>
+      </c>
+      <c r="D111" t="s">
+        <v>189</v>
+      </c>
+      <c r="E111" t="s">
         <v>191</v>
-      </c>
-      <c r="D111" t="s">
-        <v>190</v>
-      </c>
-      <c r="E111" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="B112">
-        <v>3006</v>
+        <v>3004</v>
       </c>
       <c r="C112" t="s">
-        <v>218</v>
+        <v>190</v>
       </c>
       <c r="D112" t="s">
-        <v>190</v>
-      </c>
-      <c r="E112" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>220</v>
+        <v>195</v>
       </c>
       <c r="B113">
-        <v>3007</v>
+        <v>3005</v>
       </c>
       <c r="C113" t="s">
-        <v>218</v>
+        <v>190</v>
       </c>
       <c r="D113" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E113" t="s">
-        <v>221</v>
+        <v>196</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B114">
-        <v>3008</v>
+        <v>3006</v>
       </c>
       <c r="C114" t="s">
+        <v>217</v>
+      </c>
+      <c r="D114" t="s">
+        <v>189</v>
+      </c>
+      <c r="E114" t="s">
         <v>218</v>
-      </c>
-      <c r="D114" t="s">
-        <v>190</v>
-      </c>
-      <c r="E114" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>96</v>
+        <v>219</v>
       </c>
       <c r="B115">
-        <v>4000</v>
+        <v>3007</v>
       </c>
       <c r="C115" t="s">
-        <v>97</v>
+        <v>217</v>
       </c>
       <c r="D115" t="s">
-        <v>2</v>
+        <v>189</v>
       </c>
       <c r="E115" t="s">
-        <v>98</v>
+        <v>220</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>99</v>
+        <v>221</v>
       </c>
       <c r="B116">
-        <v>4001</v>
+        <v>3008</v>
       </c>
       <c r="C116" t="s">
-        <v>97</v>
+        <v>217</v>
       </c>
       <c r="D116" t="s">
-        <v>17</v>
+        <v>189</v>
       </c>
       <c r="E116" t="s">
-        <v>100</v>
+        <v>218</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>207</v>
+        <v>96</v>
       </c>
       <c r="B117">
-        <v>4002</v>
+        <v>4000</v>
       </c>
       <c r="C117" t="s">
         <v>97</v>
       </c>
       <c r="D117" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E117" t="s">
-        <v>208</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>99</v>
+      </c>
+      <c r="B118">
+        <v>4001</v>
+      </c>
+      <c r="C118" t="s">
+        <v>97</v>
+      </c>
+      <c r="D118" t="s">
+        <v>17</v>
+      </c>
+      <c r="E118" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>206</v>
+      </c>
+      <c r="B119">
+        <v>4002</v>
+      </c>
+      <c r="C119" t="s">
+        <v>97</v>
+      </c>
+      <c r="D119" t="s">
+        <v>17</v>
+      </c>
+      <c r="E119" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Full support for new loadout unlocking system, raised the theoretical loadout limit per person from 26 to 2147483647. Added the ability to favorite kits so they show up first in the loadout list (this was already a feature just only doable through the unimplemented kit ui). Added commands: /kit upgrade <id> <class> /kit unlock <id> /kit lock <id> /request upgrade /kit favorite [id] /kit unfavorite [id] + the ability to use /kit give by looking at the sign.
Now have a method to open tickets from in-game and to check if a player is in the discord server.
</commit_message>
<xml_diff>
--- a/netcalls.xlsx
+++ b/netcalls.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\UncreatedWarfare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC7196EB-493B-4F42-AF7F-694759D0D446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7776018B-9239-4177-97F0-92F54E308786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="6675" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="netcalls" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="233">
   <si>
     <t>SendPlayerList</t>
   </si>
@@ -701,6 +701,24 @@
   </si>
   <si>
     <t>ulong fromPlayer, ulong player, Class @class, string loadoutName</t>
+  </si>
+  <si>
+    <t>CheckUserInDiscordServerRequest</t>
+  </si>
+  <si>
+    <t>ulong discordId</t>
+  </si>
+  <si>
+    <t>RequestOpenTicket</t>
+  </si>
+  <si>
+    <t>ulong player, ulong user, TicketType type, string? launchOptions</t>
+  </si>
+  <si>
+    <t>RequestIsModifyLoadoutTicketOpen</t>
+  </si>
+  <si>
+    <t>ulong user, int loadoutId</t>
   </si>
 </sst>
 </file>
@@ -1245,10 +1263,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E119" totalsRowShown="0">
-  <autoFilter ref="A1:E119" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E119">
-    <sortCondition ref="B1:B119"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E122" totalsRowShown="0">
+  <autoFilter ref="A1:E122" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E122">
+    <sortCondition ref="B1:B122"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="NetCall Field Name"/>
@@ -1558,10 +1576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E119"/>
+  <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1966,101 +1984,101 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>160</v>
+        <v>227</v>
       </c>
       <c r="B24">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>161</v>
+        <v>228</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>160</v>
       </c>
       <c r="B25">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="C25" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="D25" t="s">
         <v>17</v>
       </c>
       <c r="E25" t="s">
-        <v>30</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B26">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="C26" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="D26" t="s">
         <v>17</v>
       </c>
       <c r="E26" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B27">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="C27" t="s">
         <v>32</v>
       </c>
       <c r="D27" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B28">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="C28" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="D28" t="s">
         <v>2</v>
       </c>
       <c r="E28" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B29">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="C29" t="s">
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E29" t="s">
         <v>37</v>
@@ -2068,41 +2086,41 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="D30" t="s">
         <v>17</v>
+      </c>
+      <c r="E30" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B31">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="C31" t="s">
         <v>40</v>
       </c>
       <c r="D31" t="s">
-        <v>2</v>
-      </c>
-      <c r="E31" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B32">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="C32" t="s">
         <v>40</v>
@@ -2111,199 +2129,199 @@
         <v>2</v>
       </c>
       <c r="E32" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B33">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="C33" t="s">
         <v>40</v>
       </c>
       <c r="D33" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B34">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="C34" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="D34" t="s">
         <v>17</v>
       </c>
       <c r="E34" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B35">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="C35" t="s">
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E35" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B36">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="C36" t="s">
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E36" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B37">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="C37" t="s">
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E37" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>169</v>
+        <v>51</v>
       </c>
       <c r="B38">
-        <v>1100</v>
+        <v>1036</v>
       </c>
       <c r="C38" t="s">
-        <v>176</v>
+        <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E38" t="s">
-        <v>170</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>171</v>
+        <v>229</v>
       </c>
       <c r="B39">
-        <v>1101</v>
+        <v>1037</v>
       </c>
       <c r="C39" t="s">
-        <v>176</v>
+        <v>1</v>
       </c>
       <c r="D39" t="s">
         <v>2</v>
       </c>
       <c r="E39" t="s">
-        <v>172</v>
+        <v>230</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>209</v>
+        <v>231</v>
       </c>
       <c r="B40">
-        <v>1102</v>
+        <v>1038</v>
       </c>
       <c r="C40" t="s">
-        <v>208</v>
+        <v>176</v>
       </c>
       <c r="D40" t="s">
-        <v>189</v>
+        <v>2</v>
+      </c>
+      <c r="E40" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>53</v>
+        <v>169</v>
       </c>
       <c r="B41">
-        <v>1103</v>
+        <v>1100</v>
       </c>
       <c r="C41" t="s">
-        <v>5</v>
+        <v>176</v>
       </c>
       <c r="D41" t="s">
         <v>17</v>
       </c>
       <c r="E41" t="s">
-        <v>47</v>
+        <v>170</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>54</v>
+        <v>171</v>
       </c>
       <c r="B42">
-        <v>1104</v>
+        <v>1101</v>
       </c>
       <c r="C42" t="s">
-        <v>5</v>
+        <v>176</v>
       </c>
       <c r="D42" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E42" t="s">
-        <v>47</v>
+        <v>172</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>55</v>
+        <v>209</v>
       </c>
       <c r="B43">
-        <v>1105</v>
+        <v>1102</v>
       </c>
       <c r="C43" t="s">
-        <v>5</v>
+        <v>208</v>
       </c>
       <c r="D43" t="s">
-        <v>17</v>
-      </c>
-      <c r="E43" t="s">
-        <v>47</v>
+        <v>189</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B44">
-        <v>1106</v>
+        <v>1103</v>
       </c>
       <c r="C44" t="s">
         <v>5</v>
@@ -2317,10 +2335,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B45">
-        <v>1107</v>
+        <v>1104</v>
       </c>
       <c r="C45" t="s">
         <v>5</v>
@@ -2334,10 +2352,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B46">
-        <v>1108</v>
+        <v>1105</v>
       </c>
       <c r="C46" t="s">
         <v>5</v>
@@ -2351,78 +2369,78 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B47">
-        <v>1109</v>
+        <v>1106</v>
       </c>
       <c r="C47" t="s">
-        <v>176</v>
+        <v>5</v>
       </c>
       <c r="D47" t="s">
         <v>17</v>
       </c>
       <c r="E47" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>166</v>
+        <v>57</v>
       </c>
       <c r="B48">
-        <v>1110</v>
+        <v>1107</v>
       </c>
       <c r="C48" t="s">
-        <v>176</v>
+        <v>5</v>
       </c>
       <c r="D48" t="s">
         <v>17</v>
       </c>
       <c r="E48" t="s">
-        <v>225</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>167</v>
+        <v>58</v>
       </c>
       <c r="B49">
-        <v>1111</v>
+        <v>1108</v>
       </c>
       <c r="C49" t="s">
-        <v>176</v>
+        <v>5</v>
       </c>
       <c r="D49" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E49" t="s">
-        <v>168</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B50">
-        <v>1112</v>
+        <v>1109</v>
       </c>
       <c r="C50" t="s">
-        <v>5</v>
+        <v>176</v>
       </c>
       <c r="D50" t="s">
         <v>17</v>
       </c>
       <c r="E50" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>62</v>
+        <v>166</v>
       </c>
       <c r="B51">
-        <v>1113</v>
+        <v>1110</v>
       </c>
       <c r="C51" t="s">
         <v>176</v>
@@ -2431,15 +2449,15 @@
         <v>17</v>
       </c>
       <c r="E51" t="s">
-        <v>63</v>
+        <v>225</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>64</v>
+        <v>167</v>
       </c>
       <c r="B52">
-        <v>1114</v>
+        <v>1111</v>
       </c>
       <c r="C52" t="s">
         <v>176</v>
@@ -2448,32 +2466,32 @@
         <v>2</v>
       </c>
       <c r="E52" t="s">
-        <v>88</v>
+        <v>168</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B53">
-        <v>1115</v>
+        <v>1112</v>
       </c>
       <c r="C53" t="s">
-        <v>176</v>
+        <v>5</v>
       </c>
       <c r="D53" t="s">
         <v>17</v>
       </c>
       <c r="E53" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B54">
-        <v>1116</v>
+        <v>1113</v>
       </c>
       <c r="C54" t="s">
         <v>176</v>
@@ -2482,15 +2500,15 @@
         <v>17</v>
       </c>
       <c r="E54" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B55">
-        <v>1117</v>
+        <v>1114</v>
       </c>
       <c r="C55" t="s">
         <v>176</v>
@@ -2499,315 +2517,315 @@
         <v>2</v>
       </c>
       <c r="E55" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B56">
-        <v>1118</v>
+        <v>1115</v>
       </c>
       <c r="C56" t="s">
         <v>176</v>
       </c>
       <c r="D56" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E56" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B57">
-        <v>1119</v>
+        <v>1116</v>
       </c>
       <c r="C57" t="s">
-        <v>32</v>
+        <v>176</v>
       </c>
       <c r="D57" t="s">
         <v>17</v>
       </c>
       <c r="E57" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="B58">
-        <v>1120</v>
+        <v>1117</v>
       </c>
       <c r="C58" t="s">
-        <v>32</v>
+        <v>176</v>
       </c>
       <c r="D58" t="s">
         <v>2</v>
       </c>
       <c r="E58" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B59">
-        <v>1121</v>
+        <v>1118</v>
       </c>
       <c r="C59" t="s">
-        <v>32</v>
+        <v>176</v>
       </c>
       <c r="D59" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E59" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="B60">
-        <v>1122</v>
+        <v>1119</v>
       </c>
       <c r="C60" t="s">
         <v>32</v>
       </c>
       <c r="D60" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E60" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B61">
-        <v>1123</v>
+        <v>1120</v>
       </c>
       <c r="C61" t="s">
         <v>32</v>
       </c>
       <c r="D61" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E61" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B62">
-        <v>1124</v>
+        <v>1121</v>
       </c>
       <c r="C62" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="D62" t="s">
         <v>17</v>
       </c>
       <c r="E62" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="B63">
-        <v>1125</v>
+        <v>1122</v>
       </c>
       <c r="C63" t="s">
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="D63" t="s">
         <v>2</v>
       </c>
       <c r="E63" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B64">
-        <v>1126</v>
+        <v>1123</v>
       </c>
       <c r="C64" t="s">
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="D64" t="s">
         <v>17</v>
-      </c>
-      <c r="E64" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>204</v>
+        <v>76</v>
       </c>
       <c r="B65">
-        <v>1127</v>
+        <v>1124</v>
       </c>
       <c r="C65" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D65" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E65" t="s">
-        <v>205</v>
+        <v>78</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B66">
-        <v>1128</v>
+        <v>1125</v>
       </c>
       <c r="C66" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D66" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E66" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>162</v>
+        <v>82</v>
       </c>
       <c r="B67">
-        <v>1131</v>
+        <v>1126</v>
       </c>
       <c r="C67" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D67" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E67" t="s">
-        <v>163</v>
+        <v>83</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>175</v>
+        <v>204</v>
       </c>
       <c r="B68">
-        <v>1132</v>
+        <v>1127</v>
       </c>
       <c r="C68" t="s">
-        <v>176</v>
+        <v>84</v>
       </c>
       <c r="D68" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E68" t="s">
-        <v>177</v>
+        <v>205</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>173</v>
+        <v>85</v>
       </c>
       <c r="B69">
-        <v>1133</v>
+        <v>1128</v>
       </c>
       <c r="C69" t="s">
-        <v>176</v>
+        <v>84</v>
       </c>
       <c r="D69" t="s">
-        <v>2</v>
-      </c>
-      <c r="E69" t="s">
-        <v>174</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="B70">
-        <v>1134</v>
+        <v>1131</v>
       </c>
       <c r="C70" t="s">
-        <v>176</v>
+        <v>40</v>
       </c>
       <c r="D70" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E70" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B71">
-        <v>1135</v>
+        <v>1132</v>
       </c>
       <c r="C71" t="s">
         <v>176</v>
       </c>
       <c r="D71" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E71" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="B72">
-        <v>1136</v>
+        <v>1133</v>
       </c>
       <c r="C72" t="s">
         <v>176</v>
       </c>
       <c r="D72" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E72" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B73">
-        <v>1137</v>
+        <v>1134</v>
       </c>
       <c r="C73" t="s">
         <v>176</v>
       </c>
       <c r="D73" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E73" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>211</v>
+        <v>180</v>
       </c>
       <c r="B74">
-        <v>1138</v>
+        <v>1135</v>
       </c>
       <c r="C74" t="s">
         <v>176</v>
@@ -2816,15 +2834,15 @@
         <v>2</v>
       </c>
       <c r="E74" t="s">
-        <v>210</v>
+        <v>184</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>213</v>
+        <v>181</v>
       </c>
       <c r="B75">
-        <v>1139</v>
+        <v>1136</v>
       </c>
       <c r="C75" t="s">
         <v>176</v>
@@ -2833,49 +2851,49 @@
         <v>17</v>
       </c>
       <c r="E75" t="s">
-        <v>214</v>
+        <v>182</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>212</v>
+        <v>183</v>
       </c>
       <c r="B76">
-        <v>1140</v>
+        <v>1137</v>
       </c>
       <c r="C76" t="s">
         <v>176</v>
       </c>
       <c r="D76" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E76" t="s">
-        <v>215</v>
+        <v>185</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="B77">
-        <v>1141</v>
+        <v>1138</v>
       </c>
       <c r="C77" t="s">
         <v>176</v>
       </c>
       <c r="D77" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E77" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="B78">
-        <v>1142</v>
+        <v>1139</v>
       </c>
       <c r="C78" t="s">
         <v>176</v>
@@ -2884,247 +2902,250 @@
         <v>17</v>
       </c>
       <c r="E78" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>110</v>
+        <v>212</v>
       </c>
       <c r="B79">
-        <v>2000</v>
+        <v>1140</v>
       </c>
       <c r="C79" t="s">
-        <v>109</v>
+        <v>176</v>
       </c>
       <c r="D79" t="s">
         <v>17</v>
       </c>
       <c r="E79" t="s">
-        <v>24</v>
+        <v>215</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>124</v>
+        <v>223</v>
       </c>
       <c r="B80">
-        <v>2001</v>
+        <v>1141</v>
       </c>
       <c r="C80" t="s">
-        <v>109</v>
+        <v>176</v>
       </c>
       <c r="D80" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E80" t="s">
-        <v>146</v>
+        <v>224</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>111</v>
+        <v>222</v>
       </c>
       <c r="B81">
-        <v>2002</v>
+        <v>1142</v>
       </c>
       <c r="C81" t="s">
-        <v>109</v>
+        <v>176</v>
       </c>
       <c r="D81" t="s">
         <v>17</v>
       </c>
       <c r="E81" t="s">
-        <v>139</v>
+        <v>226</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B82">
-        <v>2003</v>
+        <v>2000</v>
       </c>
       <c r="C82" t="s">
         <v>109</v>
       </c>
       <c r="D82" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E82" t="s">
-        <v>144</v>
+        <v>24</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="B83">
-        <v>2004</v>
+        <v>2001</v>
       </c>
       <c r="C83" t="s">
         <v>109</v>
       </c>
       <c r="D83" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E83" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B84">
-        <v>2005</v>
+        <v>2002</v>
       </c>
       <c r="C84" t="s">
         <v>109</v>
       </c>
       <c r="D84" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E84" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B85">
-        <v>2006</v>
+        <v>2003</v>
       </c>
       <c r="C85" t="s">
         <v>109</v>
       </c>
       <c r="D85" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E85" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="B86">
-        <v>2007</v>
+        <v>2004</v>
       </c>
       <c r="C86" t="s">
         <v>109</v>
       </c>
       <c r="D86" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E86" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="B87">
-        <v>2008</v>
+        <v>2005</v>
       </c>
       <c r="C87" t="s">
         <v>109</v>
       </c>
       <c r="D87" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E87" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="B88">
-        <v>2009</v>
+        <v>2006</v>
       </c>
       <c r="C88" t="s">
         <v>109</v>
       </c>
       <c r="D88" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E88" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="B89">
-        <v>2010</v>
+        <v>2007</v>
       </c>
       <c r="C89" t="s">
         <v>109</v>
       </c>
       <c r="D89" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E89" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="B90">
-        <v>2011</v>
+        <v>2008</v>
       </c>
       <c r="C90" t="s">
         <v>109</v>
       </c>
       <c r="D90" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E90" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="B91">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="C91" t="s">
         <v>109</v>
       </c>
       <c r="D91" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E91" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="B92">
-        <v>2013</v>
+        <v>2010</v>
       </c>
       <c r="C92" t="s">
         <v>109</v>
       </c>
       <c r="D92" t="s">
-        <v>2</v>
-      </c>
-      <c r="E92" t="s">
-        <v>150</v>
+        <v>17</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B93">
-        <v>2019</v>
+        <v>2011</v>
       </c>
       <c r="C93" t="s">
         <v>109</v>
@@ -3133,15 +3154,15 @@
         <v>2</v>
       </c>
       <c r="E93" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B94">
-        <v>2020</v>
+        <v>2012</v>
       </c>
       <c r="C94" t="s">
         <v>109</v>
@@ -3149,16 +3170,13 @@
       <c r="D94" t="s">
         <v>17</v>
       </c>
-      <c r="E94" t="s">
-        <v>143</v>
-      </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B95">
-        <v>2021</v>
+        <v>2013</v>
       </c>
       <c r="C95" t="s">
         <v>109</v>
@@ -3167,15 +3185,15 @@
         <v>2</v>
       </c>
       <c r="E95" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B96">
-        <v>2022</v>
+        <v>2019</v>
       </c>
       <c r="C96" t="s">
         <v>109</v>
@@ -3184,32 +3202,32 @@
         <v>2</v>
       </c>
       <c r="E96" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="B97">
-        <v>2023</v>
+        <v>2020</v>
       </c>
       <c r="C97" t="s">
         <v>109</v>
       </c>
       <c r="D97" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E97" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B98">
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="C98" t="s">
         <v>109</v>
@@ -3218,57 +3236,66 @@
         <v>2</v>
       </c>
       <c r="E98" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="B99">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="C99" t="s">
         <v>109</v>
       </c>
       <c r="D99" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E99" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="B100">
-        <v>2026</v>
+        <v>2023</v>
       </c>
       <c r="C100" t="s">
         <v>109</v>
       </c>
       <c r="D100" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E100" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="B101">
-        <v>2027</v>
+        <v>2024</v>
       </c>
       <c r="C101" t="s">
         <v>109</v>
       </c>
       <c r="D101" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E101" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B102">
-        <v>2028</v>
+        <v>2025</v>
       </c>
       <c r="C102" t="s">
         <v>109</v>
@@ -3279,61 +3306,52 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B103">
-        <v>2090</v>
+        <v>2026</v>
       </c>
       <c r="C103" t="s">
         <v>109</v>
       </c>
       <c r="D103" t="s">
-        <v>2</v>
-      </c>
-      <c r="E103" t="s">
-        <v>156</v>
+        <v>17</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="B104">
-        <v>2091</v>
+        <v>2027</v>
       </c>
       <c r="C104" t="s">
         <v>109</v>
       </c>
       <c r="D104" t="s">
-        <v>2</v>
-      </c>
-      <c r="E104" t="s">
-        <v>145</v>
+        <v>17</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B105">
-        <v>2092</v>
+        <v>2028</v>
       </c>
       <c r="C105" t="s">
         <v>109</v>
       </c>
       <c r="D105" t="s">
-        <v>2</v>
-      </c>
-      <c r="E105" t="s">
-        <v>157</v>
+        <v>17</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B106">
-        <v>2093</v>
+        <v>2090</v>
       </c>
       <c r="C106" t="s">
         <v>109</v>
@@ -3342,15 +3360,15 @@
         <v>2</v>
       </c>
       <c r="E106" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B107">
-        <v>2094</v>
+        <v>2091</v>
       </c>
       <c r="C107" t="s">
         <v>109</v>
@@ -3359,97 +3377,100 @@
         <v>2</v>
       </c>
       <c r="E107" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>199</v>
+        <v>136</v>
       </c>
       <c r="B108">
-        <v>3000</v>
+        <v>2092</v>
       </c>
       <c r="C108" t="s">
-        <v>201</v>
+        <v>109</v>
       </c>
       <c r="D108" t="s">
-        <v>189</v>
+        <v>2</v>
       </c>
       <c r="E108" t="s">
-        <v>202</v>
+        <v>157</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>200</v>
+        <v>137</v>
       </c>
       <c r="B109">
-        <v>3001</v>
+        <v>2093</v>
       </c>
       <c r="C109" t="s">
-        <v>201</v>
+        <v>109</v>
       </c>
       <c r="D109" t="s">
-        <v>189</v>
+        <v>2</v>
       </c>
       <c r="E109" t="s">
-        <v>203</v>
+        <v>158</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>193</v>
+        <v>138</v>
       </c>
       <c r="B110">
-        <v>3002</v>
+        <v>2094</v>
       </c>
       <c r="C110" t="s">
-        <v>190</v>
+        <v>109</v>
       </c>
       <c r="D110" t="s">
-        <v>189</v>
+        <v>2</v>
       </c>
       <c r="E110" t="s">
-        <v>194</v>
+        <v>159</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="B111">
-        <v>3003</v>
+        <v>3000</v>
       </c>
       <c r="C111" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="D111" t="s">
         <v>189</v>
       </c>
       <c r="E111" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B112">
-        <v>3004</v>
+        <v>3001</v>
       </c>
       <c r="C112" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="D112" t="s">
         <v>189</v>
       </c>
+      <c r="E112" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B113">
-        <v>3005</v>
+        <v>3002</v>
       </c>
       <c r="C113" t="s">
         <v>190</v>
@@ -3458,108 +3479,156 @@
         <v>189</v>
       </c>
       <c r="E113" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>216</v>
+        <v>192</v>
       </c>
       <c r="B114">
-        <v>3006</v>
+        <v>3003</v>
       </c>
       <c r="C114" t="s">
-        <v>217</v>
+        <v>190</v>
       </c>
       <c r="D114" t="s">
         <v>189</v>
       </c>
       <c r="E114" t="s">
-        <v>218</v>
+        <v>191</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>219</v>
+        <v>197</v>
       </c>
       <c r="B115">
-        <v>3007</v>
+        <v>3004</v>
       </c>
       <c r="C115" t="s">
-        <v>217</v>
+        <v>190</v>
       </c>
       <c r="D115" t="s">
         <v>189</v>
       </c>
-      <c r="E115" t="s">
-        <v>220</v>
-      </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>221</v>
+        <v>195</v>
       </c>
       <c r="B116">
-        <v>3008</v>
+        <v>3005</v>
       </c>
       <c r="C116" t="s">
-        <v>217</v>
+        <v>190</v>
       </c>
       <c r="D116" t="s">
         <v>189</v>
       </c>
       <c r="E116" t="s">
-        <v>218</v>
+        <v>196</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>96</v>
+        <v>216</v>
       </c>
       <c r="B117">
-        <v>4000</v>
+        <v>3006</v>
       </c>
       <c r="C117" t="s">
-        <v>97</v>
+        <v>217</v>
       </c>
       <c r="D117" t="s">
-        <v>2</v>
+        <v>189</v>
       </c>
       <c r="E117" t="s">
-        <v>98</v>
+        <v>218</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>99</v>
+        <v>219</v>
       </c>
       <c r="B118">
-        <v>4001</v>
+        <v>3007</v>
       </c>
       <c r="C118" t="s">
-        <v>97</v>
+        <v>217</v>
       </c>
       <c r="D118" t="s">
-        <v>17</v>
+        <v>189</v>
       </c>
       <c r="E118" t="s">
-        <v>100</v>
+        <v>220</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
+        <v>221</v>
+      </c>
+      <c r="B119">
+        <v>3008</v>
+      </c>
+      <c r="C119" t="s">
+        <v>217</v>
+      </c>
+      <c r="D119" t="s">
+        <v>189</v>
+      </c>
+      <c r="E119" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>96</v>
+      </c>
+      <c r="B120">
+        <v>4000</v>
+      </c>
+      <c r="C120" t="s">
+        <v>97</v>
+      </c>
+      <c r="D120" t="s">
+        <v>2</v>
+      </c>
+      <c r="E120" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>99</v>
+      </c>
+      <c r="B121">
+        <v>4001</v>
+      </c>
+      <c r="C121" t="s">
+        <v>97</v>
+      </c>
+      <c r="D121" t="s">
+        <v>17</v>
+      </c>
+      <c r="E121" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>206</v>
       </c>
-      <c r="B119">
+      <c r="B122">
         <v>4002</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C122" t="s">
         <v>97</v>
       </c>
-      <c r="D119" t="s">
-        <v>17</v>
-      </c>
-      <c r="E119" t="s">
+      <c r="D122" t="s">
+        <v>17</v>
+      </c>
+      <c r="E122" t="s">
         <v>207</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new asset searching net methods, removed legacy ones. maybe fixed a fob quest it looks fine to me.
</commit_message>
<xml_diff>
--- a/netcalls.xlsx
+++ b/netcalls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\UncreatedWarfare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7776018B-9239-4177-97F0-92F54E308786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06252C6-01D0-44CC-8E1A-844B46D48986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="6585" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="netcalls" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="228">
   <si>
     <t>SendPlayerList</t>
   </si>
@@ -115,21 +115,9 @@
     <t>ulong target, bool hasQueueSkip</t>
   </si>
   <si>
-    <t>RequestAssetName</t>
-  </si>
-  <si>
     <t>UCAssetManager.NetCalls</t>
   </si>
   <si>
-    <t>ushort id, EAssetType category</t>
-  </si>
-  <si>
-    <t>SendAssetName</t>
-  </si>
-  <si>
-    <t>ushort id, EAssetType category, string friendlyName</t>
-  </si>
-  <si>
     <t>SendPlayerMuted</t>
   </si>
   <si>
@@ -235,21 +223,6 @@
     <t>Kit?[] kit</t>
   </si>
   <si>
-    <t>RequestItemInfo</t>
-  </si>
-  <si>
-    <t>ushort id</t>
-  </si>
-  <si>
-    <t>RequestItemInfos</t>
-  </si>
-  <si>
-    <t>ushort[] ids</t>
-  </si>
-  <si>
-    <t>RequestAllItemInfos</t>
-  </si>
-  <si>
     <t>SendDiscordKeyState</t>
   </si>
   <si>
@@ -280,12 +253,6 @@
     <t>RequestCurrentLog</t>
   </si>
   <si>
-    <t>SendItemInfo</t>
-  </si>
-  <si>
-    <t>ItemData? Data</t>
-  </si>
-  <si>
     <t>string kitName, EClass class, string displayName</t>
   </si>
   <si>
@@ -304,12 +271,6 @@
     <t>Method Signature</t>
   </si>
   <si>
-    <t>SendItemInfos</t>
-  </si>
-  <si>
-    <t>ItemData[]? Data</t>
-  </si>
-  <si>
     <t>SendReportInvocation</t>
   </si>
   <si>
@@ -719,6 +680,30 @@
   </si>
   <si>
     <t>ulong user, int loadoutId</t>
+  </si>
+  <si>
+    <t>RequestFindAssetById</t>
+  </si>
+  <si>
+    <t>ushort id, Type assetType</t>
+  </si>
+  <si>
+    <t>RequestFindAssetByText</t>
+  </si>
+  <si>
+    <t>RequestFindAssetByGuid</t>
+  </si>
+  <si>
+    <t>string name, Type assetType</t>
+  </si>
+  <si>
+    <t>Guid guid</t>
+  </si>
+  <si>
+    <t>SendFindAssets</t>
+  </si>
+  <si>
+    <t>AssetInfo[] results</t>
   </si>
 </sst>
 </file>
@@ -1263,10 +1248,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E122" totalsRowShown="0">
-  <autoFilter ref="A1:E122" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E122">
-    <sortCondition ref="B1:B122"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E119" totalsRowShown="0">
+  <autoFilter ref="A1:E119" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E119">
+    <sortCondition ref="B1:B119"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="NetCall Field Name"/>
@@ -1576,10 +1561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E122"/>
+  <dimension ref="A1:E119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1593,19 +1578,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="D1" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="E1" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1746,19 +1731,19 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="B10">
         <v>1008</v>
       </c>
       <c r="C10" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="D10" t="s">
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1814,70 +1799,70 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="B14">
         <v>1012</v>
       </c>
       <c r="C14" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="D14" t="s">
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="B15">
         <v>1013</v>
       </c>
       <c r="C15" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="D15" t="s">
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="B16">
         <v>1014</v>
       </c>
       <c r="C16" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="D16" t="s">
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="B17">
         <v>1015</v>
       </c>
       <c r="C17" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="D17" t="s">
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1950,7 +1935,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="B22">
         <v>1020</v>
@@ -1962,12 +1947,12 @@
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="B23">
         <v>1021</v>
@@ -1979,12 +1964,12 @@
         <v>17</v>
       </c>
       <c r="E23" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="B24">
         <v>1022</v>
@@ -1996,24 +1981,24 @@
         <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="B25">
         <v>1023</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D25" t="s">
         <v>17</v>
       </c>
       <c r="E25" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2035,16 +2020,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B27">
-        <v>1025</v>
+        <v>1027</v>
       </c>
       <c r="C27" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E27" t="s">
         <v>33</v>
@@ -2055,50 +2040,47 @@
         <v>34</v>
       </c>
       <c r="B28">
-        <v>1026</v>
+        <v>1028</v>
       </c>
       <c r="C28" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E28" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29">
+        <v>1029</v>
+      </c>
+      <c r="C29" t="s">
         <v>36</v>
       </c>
-      <c r="B29">
-        <v>1027</v>
-      </c>
-      <c r="C29" t="s">
-        <v>5</v>
-      </c>
       <c r="D29" t="s">
-        <v>2</v>
-      </c>
-      <c r="E29" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30">
+        <v>1030</v>
+      </c>
+      <c r="C30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" t="s">
         <v>38</v>
-      </c>
-      <c r="B30">
-        <v>1028</v>
-      </c>
-      <c r="C30" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2106,61 +2088,64 @@
         <v>39</v>
       </c>
       <c r="B31">
-        <v>1029</v>
+        <v>1031</v>
       </c>
       <c r="C31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" t="s">
         <v>40</v>
-      </c>
-      <c r="D31" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32">
+        <v>1032</v>
+      </c>
+      <c r="C32" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" t="s">
         <v>41</v>
-      </c>
-      <c r="B32">
-        <v>1030</v>
-      </c>
-      <c r="C32" t="s">
-        <v>40</v>
-      </c>
-      <c r="D32" t="s">
-        <v>2</v>
-      </c>
-      <c r="E32" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33">
+        <v>1033</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" t="s">
         <v>43</v>
-      </c>
-      <c r="B33">
-        <v>1031</v>
-      </c>
-      <c r="C33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D33" t="s">
-        <v>2</v>
-      </c>
-      <c r="E33" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B34">
-        <v>1032</v>
+        <v>1034</v>
       </c>
       <c r="C34" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E34" t="s">
         <v>45</v>
@@ -2171,7 +2156,7 @@
         <v>46</v>
       </c>
       <c r="B35">
-        <v>1033</v>
+        <v>1035</v>
       </c>
       <c r="C35" t="s">
         <v>1</v>
@@ -2180,15 +2165,15 @@
         <v>17</v>
       </c>
       <c r="E35" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B36">
-        <v>1034</v>
+        <v>1036</v>
       </c>
       <c r="C36" t="s">
         <v>1</v>
@@ -2197,131 +2182,131 @@
         <v>2</v>
       </c>
       <c r="E36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>216</v>
       </c>
       <c r="B37">
-        <v>1035</v>
+        <v>1037</v>
       </c>
       <c r="C37" t="s">
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E37" t="s">
-        <v>47</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>218</v>
       </c>
       <c r="B38">
-        <v>1036</v>
+        <v>1038</v>
       </c>
       <c r="C38" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="D38" t="s">
         <v>2</v>
       </c>
       <c r="E38" t="s">
-        <v>52</v>
+        <v>219</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>229</v>
+        <v>156</v>
       </c>
       <c r="B39">
-        <v>1037</v>
+        <v>1100</v>
       </c>
       <c r="C39" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="D39" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E39" t="s">
-        <v>230</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>231</v>
+        <v>158</v>
       </c>
       <c r="B40">
-        <v>1038</v>
+        <v>1101</v>
       </c>
       <c r="C40" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="D40" t="s">
         <v>2</v>
       </c>
       <c r="E40" t="s">
-        <v>232</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>169</v>
+        <v>196</v>
       </c>
       <c r="B41">
-        <v>1100</v>
+        <v>1102</v>
       </c>
       <c r="C41" t="s">
+        <v>195</v>
+      </c>
+      <c r="D41" t="s">
         <v>176</v>
-      </c>
-      <c r="D41" t="s">
-        <v>17</v>
-      </c>
-      <c r="E41" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>171</v>
+        <v>49</v>
       </c>
       <c r="B42">
-        <v>1101</v>
+        <v>1103</v>
       </c>
       <c r="C42" t="s">
-        <v>176</v>
+        <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E42" t="s">
-        <v>172</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>209</v>
+        <v>50</v>
       </c>
       <c r="B43">
-        <v>1102</v>
+        <v>1104</v>
       </c>
       <c r="C43" t="s">
-        <v>208</v>
+        <v>5</v>
       </c>
       <c r="D43" t="s">
-        <v>189</v>
+        <v>17</v>
+      </c>
+      <c r="E43" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B44">
-        <v>1103</v>
+        <v>1105</v>
       </c>
       <c r="C44" t="s">
         <v>5</v>
@@ -2330,15 +2315,15 @@
         <v>17</v>
       </c>
       <c r="E44" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B45">
-        <v>1104</v>
+        <v>1106</v>
       </c>
       <c r="C45" t="s">
         <v>5</v>
@@ -2347,15 +2332,15 @@
         <v>17</v>
       </c>
       <c r="E45" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B46">
-        <v>1105</v>
+        <v>1107</v>
       </c>
       <c r="C46" t="s">
         <v>5</v>
@@ -2364,15 +2349,15 @@
         <v>17</v>
       </c>
       <c r="E46" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B47">
-        <v>1106</v>
+        <v>1108</v>
       </c>
       <c r="C47" t="s">
         <v>5</v>
@@ -2381,1255 +2366,1207 @@
         <v>17</v>
       </c>
       <c r="E47" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B48">
-        <v>1107</v>
+        <v>1109</v>
       </c>
       <c r="C48" t="s">
-        <v>5</v>
+        <v>163</v>
       </c>
       <c r="D48" t="s">
         <v>17</v>
       </c>
       <c r="E48" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>58</v>
+        <v>153</v>
       </c>
       <c r="B49">
-        <v>1108</v>
+        <v>1110</v>
       </c>
       <c r="C49" t="s">
-        <v>5</v>
+        <v>163</v>
       </c>
       <c r="D49" t="s">
         <v>17</v>
       </c>
       <c r="E49" t="s">
-        <v>47</v>
+        <v>212</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>59</v>
+        <v>154</v>
       </c>
       <c r="B50">
-        <v>1109</v>
+        <v>1111</v>
       </c>
       <c r="C50" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="D50" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E50" t="s">
-        <v>60</v>
+        <v>155</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>166</v>
+        <v>57</v>
       </c>
       <c r="B51">
-        <v>1110</v>
+        <v>1112</v>
       </c>
       <c r="C51" t="s">
-        <v>176</v>
+        <v>5</v>
       </c>
       <c r="D51" t="s">
         <v>17</v>
       </c>
       <c r="E51" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>167</v>
+        <v>58</v>
       </c>
       <c r="B52">
-        <v>1111</v>
+        <v>1113</v>
       </c>
       <c r="C52" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="D52" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E52" t="s">
-        <v>168</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B53">
-        <v>1112</v>
+        <v>1114</v>
       </c>
       <c r="C53" t="s">
-        <v>5</v>
+        <v>163</v>
       </c>
       <c r="D53" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E53" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B54">
-        <v>1113</v>
+        <v>1115</v>
       </c>
       <c r="C54" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="D54" t="s">
         <v>17</v>
       </c>
       <c r="E54" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B55">
-        <v>1114</v>
+        <v>1116</v>
       </c>
       <c r="C55" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="D55" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E55" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B56">
-        <v>1115</v>
+        <v>1117</v>
       </c>
       <c r="C56" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="D56" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E56" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>65</v>
+      </c>
+      <c r="B57">
+        <v>1118</v>
+      </c>
+      <c r="C57" t="s">
+        <v>163</v>
+      </c>
+      <c r="D57" t="s">
+        <v>2</v>
+      </c>
+      <c r="E57" t="s">
         <v>66</v>
-      </c>
-      <c r="B57">
-        <v>1116</v>
-      </c>
-      <c r="C57" t="s">
-        <v>176</v>
-      </c>
-      <c r="D57" t="s">
-        <v>17</v>
-      </c>
-      <c r="E57" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>67</v>
+      </c>
+      <c r="B58">
+        <v>1124</v>
+      </c>
+      <c r="C58" t="s">
         <v>68</v>
       </c>
-      <c r="B58">
-        <v>1117</v>
-      </c>
-      <c r="C58" t="s">
-        <v>176</v>
-      </c>
       <c r="D58" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E58" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B59">
-        <v>1118</v>
+        <v>1125</v>
       </c>
       <c r="C59" t="s">
-        <v>176</v>
+        <v>71</v>
       </c>
       <c r="D59" t="s">
         <v>2</v>
       </c>
       <c r="E59" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>73</v>
+      </c>
+      <c r="B60">
+        <v>1126</v>
+      </c>
+      <c r="C60" t="s">
         <v>71</v>
       </c>
-      <c r="B60">
-        <v>1119</v>
-      </c>
-      <c r="C60" t="s">
-        <v>32</v>
-      </c>
       <c r="D60" t="s">
         <v>17</v>
       </c>
       <c r="E60" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>86</v>
+        <v>191</v>
       </c>
       <c r="B61">
-        <v>1120</v>
+        <v>1127</v>
       </c>
       <c r="C61" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="D61" t="s">
         <v>2</v>
       </c>
       <c r="E61" t="s">
-        <v>87</v>
+        <v>192</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B62">
-        <v>1121</v>
+        <v>1128</v>
       </c>
       <c r="C62" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="D62" t="s">
         <v>17</v>
-      </c>
-      <c r="E62" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>94</v>
+        <v>149</v>
       </c>
       <c r="B63">
-        <v>1122</v>
+        <v>1131</v>
       </c>
       <c r="C63" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D63" t="s">
         <v>2</v>
       </c>
       <c r="E63" t="s">
-        <v>95</v>
+        <v>150</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>75</v>
+        <v>162</v>
       </c>
       <c r="B64">
-        <v>1123</v>
+        <v>1132</v>
       </c>
       <c r="C64" t="s">
-        <v>32</v>
+        <v>163</v>
       </c>
       <c r="D64" t="s">
         <v>17</v>
+      </c>
+      <c r="E64" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>76</v>
+        <v>160</v>
       </c>
       <c r="B65">
-        <v>1124</v>
+        <v>1133</v>
       </c>
       <c r="C65" t="s">
-        <v>77</v>
+        <v>163</v>
       </c>
       <c r="D65" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E65" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>79</v>
+        <v>165</v>
       </c>
       <c r="B66">
-        <v>1125</v>
+        <v>1134</v>
       </c>
       <c r="C66" t="s">
-        <v>80</v>
+        <v>163</v>
       </c>
       <c r="D66" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E66" t="s">
-        <v>81</v>
+        <v>166</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>82</v>
+        <v>167</v>
       </c>
       <c r="B67">
-        <v>1126</v>
+        <v>1135</v>
       </c>
       <c r="C67" t="s">
-        <v>80</v>
+        <v>163</v>
       </c>
       <c r="D67" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E67" t="s">
-        <v>83</v>
+        <v>171</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>204</v>
+        <v>168</v>
       </c>
       <c r="B68">
-        <v>1127</v>
+        <v>1136</v>
       </c>
       <c r="C68" t="s">
-        <v>84</v>
+        <v>163</v>
       </c>
       <c r="D68" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E68" t="s">
-        <v>205</v>
+        <v>169</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>85</v>
+        <v>170</v>
       </c>
       <c r="B69">
-        <v>1128</v>
+        <v>1137</v>
       </c>
       <c r="C69" t="s">
-        <v>84</v>
+        <v>163</v>
       </c>
       <c r="D69" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E69" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>162</v>
+        <v>198</v>
       </c>
       <c r="B70">
-        <v>1131</v>
+        <v>1138</v>
       </c>
       <c r="C70" t="s">
-        <v>40</v>
+        <v>163</v>
       </c>
       <c r="D70" t="s">
         <v>2</v>
       </c>
       <c r="E70" t="s">
-        <v>163</v>
+        <v>197</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="B71">
-        <v>1132</v>
+        <v>1139</v>
       </c>
       <c r="C71" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="D71" t="s">
         <v>17</v>
       </c>
       <c r="E71" t="s">
-        <v>177</v>
+        <v>201</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>173</v>
+        <v>199</v>
       </c>
       <c r="B72">
-        <v>1133</v>
+        <v>1140</v>
       </c>
       <c r="C72" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="D72" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E72" t="s">
-        <v>174</v>
+        <v>202</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>178</v>
+        <v>210</v>
       </c>
       <c r="B73">
-        <v>1134</v>
+        <v>1141</v>
       </c>
       <c r="C73" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="D73" t="s">
         <v>17</v>
       </c>
       <c r="E73" t="s">
-        <v>179</v>
+        <v>211</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>180</v>
+        <v>209</v>
       </c>
       <c r="B74">
-        <v>1135</v>
+        <v>1142</v>
       </c>
       <c r="C74" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="D74" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E74" t="s">
-        <v>184</v>
+        <v>213</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>181</v>
+        <v>97</v>
       </c>
       <c r="B75">
-        <v>1136</v>
+        <v>2000</v>
       </c>
       <c r="C75" t="s">
-        <v>176</v>
+        <v>96</v>
       </c>
       <c r="D75" t="s">
         <v>17</v>
       </c>
       <c r="E75" t="s">
-        <v>182</v>
+        <v>24</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>183</v>
+        <v>111</v>
       </c>
       <c r="B76">
-        <v>1137</v>
+        <v>2001</v>
       </c>
       <c r="C76" t="s">
-        <v>176</v>
+        <v>96</v>
       </c>
       <c r="D76" t="s">
         <v>2</v>
       </c>
       <c r="E76" t="s">
-        <v>185</v>
+        <v>133</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>211</v>
+        <v>98</v>
       </c>
       <c r="B77">
-        <v>1138</v>
+        <v>2002</v>
       </c>
       <c r="C77" t="s">
-        <v>176</v>
+        <v>96</v>
       </c>
       <c r="D77" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E77" t="s">
-        <v>210</v>
+        <v>126</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>213</v>
+        <v>109</v>
       </c>
       <c r="B78">
-        <v>1139</v>
+        <v>2003</v>
       </c>
       <c r="C78" t="s">
-        <v>176</v>
+        <v>96</v>
       </c>
       <c r="D78" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E78" t="s">
-        <v>214</v>
+        <v>131</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>212</v>
+        <v>99</v>
       </c>
       <c r="B79">
-        <v>1140</v>
+        <v>2004</v>
       </c>
       <c r="C79" t="s">
-        <v>176</v>
+        <v>96</v>
       </c>
       <c r="D79" t="s">
         <v>17</v>
       </c>
       <c r="E79" t="s">
-        <v>215</v>
+        <v>127</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>223</v>
+        <v>110</v>
       </c>
       <c r="B80">
-        <v>1141</v>
+        <v>2005</v>
       </c>
       <c r="C80" t="s">
-        <v>176</v>
+        <v>96</v>
       </c>
       <c r="D80" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E80" t="s">
-        <v>224</v>
+        <v>132</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>222</v>
+        <v>100</v>
       </c>
       <c r="B81">
-        <v>1142</v>
+        <v>2006</v>
       </c>
       <c r="C81" t="s">
-        <v>176</v>
+        <v>96</v>
       </c>
       <c r="D81" t="s">
         <v>17</v>
       </c>
       <c r="E81" t="s">
-        <v>226</v>
+        <v>128</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B82">
-        <v>2000</v>
+        <v>2007</v>
       </c>
       <c r="C82" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D82" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E82" t="s">
-        <v>24</v>
+        <v>134</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="B83">
-        <v>2001</v>
+        <v>2008</v>
       </c>
       <c r="C83" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D83" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E83" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B84">
-        <v>2002</v>
+        <v>2009</v>
       </c>
       <c r="C84" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D84" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E84" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="B85">
-        <v>2003</v>
+        <v>2010</v>
       </c>
       <c r="C85" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D85" t="s">
-        <v>2</v>
-      </c>
-      <c r="E85" t="s">
-        <v>144</v>
+        <v>17</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B86">
-        <v>2004</v>
+        <v>2011</v>
       </c>
       <c r="C86" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D86" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E86" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="B87">
-        <v>2005</v>
+        <v>2012</v>
       </c>
       <c r="C87" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D87" t="s">
-        <v>2</v>
-      </c>
-      <c r="E87" t="s">
-        <v>145</v>
+        <v>17</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B88">
-        <v>2006</v>
+        <v>2013</v>
       </c>
       <c r="C88" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D88" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E88" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B89">
-        <v>2007</v>
+        <v>2019</v>
       </c>
       <c r="C89" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D89" t="s">
         <v>2</v>
       </c>
       <c r="E89" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B90">
-        <v>2008</v>
+        <v>2020</v>
       </c>
       <c r="C90" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D90" t="s">
         <v>17</v>
       </c>
       <c r="E90" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B91">
-        <v>2009</v>
+        <v>2021</v>
       </c>
       <c r="C91" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D91" t="s">
         <v>2</v>
       </c>
       <c r="E91" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B92">
-        <v>2010</v>
+        <v>2022</v>
       </c>
       <c r="C92" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D92" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E92" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B93">
-        <v>2011</v>
+        <v>2023</v>
       </c>
       <c r="C93" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D93" t="s">
         <v>2</v>
       </c>
       <c r="E93" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B94">
-        <v>2012</v>
+        <v>2024</v>
       </c>
       <c r="C94" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D94" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E94" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="B95">
-        <v>2013</v>
+        <v>2025</v>
       </c>
       <c r="C95" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D95" t="s">
-        <v>2</v>
-      </c>
-      <c r="E95" t="s">
-        <v>150</v>
+        <v>17</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="B96">
-        <v>2019</v>
+        <v>2026</v>
       </c>
       <c r="C96" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D96" t="s">
-        <v>2</v>
-      </c>
-      <c r="E96" t="s">
-        <v>151</v>
+        <v>17</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B97">
-        <v>2020</v>
+        <v>2027</v>
       </c>
       <c r="C97" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D97" t="s">
         <v>17</v>
-      </c>
-      <c r="E97" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
       <c r="B98">
-        <v>2021</v>
+        <v>2028</v>
       </c>
       <c r="C98" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D98" t="s">
-        <v>2</v>
-      </c>
-      <c r="E98" t="s">
-        <v>152</v>
+        <v>17</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B99">
-        <v>2022</v>
+        <v>2090</v>
       </c>
       <c r="C99" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D99" t="s">
         <v>2</v>
       </c>
       <c r="E99" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>122</v>
+      </c>
+      <c r="B100">
+        <v>2091</v>
+      </c>
+      <c r="C100" t="s">
+        <v>96</v>
+      </c>
+      <c r="D100" t="s">
+        <v>2</v>
+      </c>
+      <c r="E100" t="s">
         <v>132</v>
-      </c>
-      <c r="B100">
-        <v>2023</v>
-      </c>
-      <c r="C100" t="s">
-        <v>109</v>
-      </c>
-      <c r="D100" t="s">
-        <v>2</v>
-      </c>
-      <c r="E100" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B101">
-        <v>2024</v>
+        <v>2092</v>
       </c>
       <c r="C101" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D101" t="s">
         <v>2</v>
       </c>
       <c r="E101" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B102">
-        <v>2025</v>
+        <v>2093</v>
       </c>
       <c r="C102" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D102" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E102" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B103">
-        <v>2026</v>
+        <v>2094</v>
       </c>
       <c r="C103" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D103" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E103" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>120</v>
+        <v>186</v>
       </c>
       <c r="B104">
-        <v>2027</v>
+        <v>3000</v>
       </c>
       <c r="C104" t="s">
-        <v>109</v>
+        <v>188</v>
       </c>
       <c r="D104" t="s">
-        <v>17</v>
+        <v>176</v>
+      </c>
+      <c r="E104" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>121</v>
+        <v>187</v>
       </c>
       <c r="B105">
-        <v>2028</v>
+        <v>3001</v>
       </c>
       <c r="C105" t="s">
-        <v>109</v>
+        <v>188</v>
       </c>
       <c r="D105" t="s">
-        <v>17</v>
+        <v>176</v>
+      </c>
+      <c r="E105" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>134</v>
+        <v>180</v>
       </c>
       <c r="B106">
-        <v>2090</v>
+        <v>3002</v>
       </c>
       <c r="C106" t="s">
-        <v>109</v>
+        <v>177</v>
       </c>
       <c r="D106" t="s">
-        <v>2</v>
+        <v>176</v>
       </c>
       <c r="E106" t="s">
-        <v>156</v>
+        <v>181</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>135</v>
+        <v>179</v>
       </c>
       <c r="B107">
-        <v>2091</v>
+        <v>3003</v>
       </c>
       <c r="C107" t="s">
-        <v>109</v>
+        <v>177</v>
       </c>
       <c r="D107" t="s">
-        <v>2</v>
+        <v>176</v>
       </c>
       <c r="E107" t="s">
-        <v>145</v>
+        <v>178</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>136</v>
+        <v>184</v>
       </c>
       <c r="B108">
-        <v>2092</v>
+        <v>3004</v>
       </c>
       <c r="C108" t="s">
-        <v>109</v>
+        <v>177</v>
       </c>
       <c r="D108" t="s">
-        <v>2</v>
-      </c>
-      <c r="E108" t="s">
-        <v>157</v>
+        <v>176</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>137</v>
+        <v>182</v>
       </c>
       <c r="B109">
-        <v>2093</v>
+        <v>3005</v>
       </c>
       <c r="C109" t="s">
-        <v>109</v>
+        <v>177</v>
       </c>
       <c r="D109" t="s">
-        <v>2</v>
+        <v>176</v>
       </c>
       <c r="E109" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>138</v>
+        <v>203</v>
       </c>
       <c r="B110">
-        <v>2094</v>
+        <v>3006</v>
       </c>
       <c r="C110" t="s">
-        <v>109</v>
+        <v>204</v>
       </c>
       <c r="D110" t="s">
-        <v>2</v>
+        <v>176</v>
       </c>
       <c r="E110" t="s">
-        <v>159</v>
+        <v>205</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="B111">
-        <v>3000</v>
+        <v>3007</v>
       </c>
       <c r="C111" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D111" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="E111" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="B112">
-        <v>3001</v>
+        <v>3008</v>
       </c>
       <c r="C112" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D112" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="E112" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>193</v>
+        <v>220</v>
       </c>
       <c r="B113">
-        <v>3002</v>
+        <v>3100</v>
       </c>
       <c r="C113" t="s">
-        <v>190</v>
+        <v>31</v>
       </c>
       <c r="D113" t="s">
-        <v>189</v>
+        <v>17</v>
       </c>
       <c r="E113" t="s">
-        <v>194</v>
+        <v>221</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>192</v>
+        <v>222</v>
       </c>
       <c r="B114">
-        <v>3003</v>
+        <v>3101</v>
       </c>
       <c r="C114" t="s">
-        <v>190</v>
+        <v>31</v>
       </c>
       <c r="D114" t="s">
-        <v>189</v>
+        <v>17</v>
       </c>
       <c r="E114" t="s">
-        <v>191</v>
+        <v>224</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>197</v>
+        <v>223</v>
       </c>
       <c r="B115">
-        <v>3004</v>
+        <v>3102</v>
       </c>
       <c r="C115" t="s">
-        <v>190</v>
+        <v>31</v>
       </c>
       <c r="D115" t="s">
-        <v>189</v>
+        <v>17</v>
+      </c>
+      <c r="E115" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>195</v>
+        <v>226</v>
       </c>
       <c r="B116">
-        <v>3005</v>
+        <v>3103</v>
       </c>
       <c r="C116" t="s">
-        <v>190</v>
+        <v>31</v>
       </c>
       <c r="D116" t="s">
-        <v>189</v>
+        <v>17</v>
       </c>
       <c r="E116" t="s">
-        <v>196</v>
+        <v>227</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>216</v>
+        <v>83</v>
       </c>
       <c r="B117">
-        <v>3006</v>
+        <v>4000</v>
       </c>
       <c r="C117" t="s">
-        <v>217</v>
+        <v>84</v>
       </c>
       <c r="D117" t="s">
-        <v>189</v>
+        <v>2</v>
       </c>
       <c r="E117" t="s">
-        <v>218</v>
+        <v>85</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>219</v>
+        <v>86</v>
       </c>
       <c r="B118">
-        <v>3007</v>
+        <v>4001</v>
       </c>
       <c r="C118" t="s">
-        <v>217</v>
+        <v>84</v>
       </c>
       <c r="D118" t="s">
-        <v>189</v>
+        <v>17</v>
       </c>
       <c r="E118" t="s">
-        <v>220</v>
+        <v>87</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>221</v>
+        <v>193</v>
       </c>
       <c r="B119">
-        <v>3008</v>
+        <v>4002</v>
       </c>
       <c r="C119" t="s">
-        <v>217</v>
+        <v>84</v>
       </c>
       <c r="D119" t="s">
-        <v>189</v>
+        <v>17</v>
       </c>
       <c r="E119" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>96</v>
-      </c>
-      <c r="B120">
-        <v>4000</v>
-      </c>
-      <c r="C120" t="s">
-        <v>97</v>
-      </c>
-      <c r="D120" t="s">
-        <v>2</v>
-      </c>
-      <c r="E120" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>99</v>
-      </c>
-      <c r="B121">
-        <v>4001</v>
-      </c>
-      <c r="C121" t="s">
-        <v>97</v>
-      </c>
-      <c r="D121" t="s">
-        <v>17</v>
-      </c>
-      <c r="E121" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>206</v>
-      </c>
-      <c r="B122">
-        <v>4002</v>
-      </c>
-      <c r="C122" t="s">
-        <v>97</v>
-      </c>
-      <c r="D122" t="s">
-        <v>17</v>
-      </c>
-      <c r="E122" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added IP whitelists, and built-in IP whitelisting for common remote play services (GeForce Now). Fixed mortar warnings. Fixed /i ammo while on turret.
</commit_message>
<xml_diff>
--- a/netcalls.xlsx
+++ b/netcalls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\UncreatedWarfare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06252C6-01D0-44CC-8E1A-844B46D48986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EC066B-66E7-4DD2-A0F9-378292A4090E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="6585" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="232">
   <si>
     <t>SendPlayerList</t>
   </si>
@@ -40,36 +40,21 @@
     <t>OffenseManager.NetCalls</t>
   </si>
   <si>
-    <t>ulong target, ulong admin, string reason, int duration, DateTime timestamp</t>
-  </si>
-  <si>
     <t>SendPlayerUnbanned</t>
   </si>
   <si>
-    <t>ulong target, ulong admin, DateTime timestamp</t>
-  </si>
-  <si>
     <t>SendPlayerKicked</t>
   </si>
   <si>
-    <t>ulong target, ulong admin, string reason, DateTime timestamp</t>
-  </si>
-  <si>
     <t>SendPlayerWarned</t>
   </si>
   <si>
     <t>SendPlayerBattleyeKicked</t>
   </si>
   <si>
-    <t>ulong target, string reason, DateTime timestamp</t>
-  </si>
-  <si>
     <t>SendTeamkill</t>
   </si>
   <si>
-    <t>ulong teamkiller, ulong dead, string deathCause, string itemName, DateTime timestamp</t>
-  </si>
-  <si>
     <t>SendBanRequest</t>
   </si>
   <si>
@@ -544,9 +529,6 @@
     <t>SendPlayerUnmuted</t>
   </si>
   <si>
-    <t>ulong player, ulong admin, DateTime timestamp</t>
-  </si>
-  <si>
     <t>SendUnmuteRequest</t>
   </si>
   <si>
@@ -704,6 +686,36 @@
   </si>
   <si>
     <t>AssetInfo[] results</t>
+  </si>
+  <si>
+    <t>SendPlayerIPWhitelisted</t>
+  </si>
+  <si>
+    <t>ulong player, ulong admin, DateTimeOffset timestamp</t>
+  </si>
+  <si>
+    <t>ulong target, ulong admin, string reason, DateTimeOffset timestamp</t>
+  </si>
+  <si>
+    <t>ulong target, ulong admin, DateTimeOffset timestamp</t>
+  </si>
+  <si>
+    <t>ulong target, ulong admin, string reason, int duration, DateTimeOffset timestamp</t>
+  </si>
+  <si>
+    <t>ulong teamkiller, ulong dead, string deathCause, string itemName, DateTimeOffset timestamp</t>
+  </si>
+  <si>
+    <t>ulong target, string reason, DateTimeOffset timestamp</t>
+  </si>
+  <si>
+    <t>SendIPWhitelistRequest</t>
+  </si>
+  <si>
+    <t>ulong player, ulong admin, DateTimeOffset timestamp, uint ip, byte mask, bool added</t>
+  </si>
+  <si>
+    <t>ulong player, ulong admin, DateTimeOffset timestamp, uint ip, byte mask, bool add</t>
   </si>
 </sst>
 </file>
@@ -1248,10 +1260,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E119" totalsRowShown="0">
-  <autoFilter ref="A1:E119" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E119">
-    <sortCondition ref="B1:B119"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E121" totalsRowShown="0">
+  <autoFilter ref="A1:E121" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E121">
+    <sortCondition ref="B1:B121"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="NetCall Field Name"/>
@@ -1561,10 +1573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E119"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D108" sqref="D108"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1578,19 +1590,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1624,12 +1636,12 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>1002</v>
@@ -1641,12 +1653,12 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>1003</v>
@@ -1658,12 +1670,12 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>1004</v>
@@ -1675,12 +1687,12 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>1005</v>
@@ -1692,12 +1704,12 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>1006</v>
@@ -1709,12 +1721,12 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>1007</v>
@@ -1723,32 +1735,32 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>226</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B10">
         <v>1008</v>
       </c>
       <c r="C10" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D10" t="s">
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>1009</v>
@@ -1757,15 +1769,15 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>1010</v>
@@ -1774,15 +1786,15 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>1011</v>
@@ -1791,83 +1803,83 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>224</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B14">
         <v>1012</v>
       </c>
       <c r="C14" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D14" t="s">
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B15">
         <v>1013</v>
       </c>
       <c r="C15" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D15" t="s">
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B16">
         <v>1014</v>
       </c>
       <c r="C16" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D16" t="s">
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B17">
         <v>1015</v>
       </c>
       <c r="C17" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D17" t="s">
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>1016</v>
@@ -1879,12 +1891,12 @@
         <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>1017</v>
@@ -1896,12 +1908,12 @@
         <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B20">
         <v>1018</v>
@@ -1913,12 +1925,12 @@
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>1019</v>
@@ -1930,12 +1942,12 @@
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B22">
         <v>1020</v>
@@ -1947,12 +1959,12 @@
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>174</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B23">
         <v>1021</v>
@@ -1961,15 +1973,15 @@
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>174</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B24">
         <v>1022</v>
@@ -1981,29 +1993,29 @@
         <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B25">
         <v>1023</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D25" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>1024</v>
@@ -2012,168 +2024,168 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E26" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>222</v>
       </c>
       <c r="B27">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D27" t="s">
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>33</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>229</v>
       </c>
       <c r="B28">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="C28" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E28" t="s">
-        <v>33</v>
+        <v>231</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="C29" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E29" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B30">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="C30" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E30" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B31">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="C31" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D31" t="s">
-        <v>2</v>
-      </c>
-      <c r="E31" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B32">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="C32" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E32" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B33">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="C33" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E33" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B34">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="C34" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E34" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B35">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="C35" t="s">
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E35" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B36">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="C36" t="s">
         <v>1</v>
@@ -2182,1156 +2194,1156 @@
         <v>2</v>
       </c>
       <c r="E36" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>216</v>
+        <v>41</v>
       </c>
       <c r="B37">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="C37" t="s">
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E37" t="s">
-        <v>217</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>218</v>
+        <v>42</v>
       </c>
       <c r="B38">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="C38" t="s">
-        <v>163</v>
+        <v>1</v>
       </c>
       <c r="D38" t="s">
         <v>2</v>
       </c>
       <c r="E38" t="s">
-        <v>219</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>156</v>
+        <v>210</v>
       </c>
       <c r="B39">
-        <v>1100</v>
+        <v>1037</v>
       </c>
       <c r="C39" t="s">
-        <v>163</v>
+        <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E39" t="s">
-        <v>157</v>
+        <v>211</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>212</v>
+      </c>
+      <c r="B40">
+        <v>1038</v>
+      </c>
+      <c r="C40" t="s">
         <v>158</v>
       </c>
-      <c r="B40">
-        <v>1101</v>
-      </c>
-      <c r="C40" t="s">
-        <v>163</v>
-      </c>
       <c r="D40" t="s">
         <v>2</v>
       </c>
       <c r="E40" t="s">
-        <v>159</v>
+        <v>213</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>196</v>
+        <v>151</v>
       </c>
       <c r="B41">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="C41" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
       <c r="D41" t="s">
-        <v>176</v>
+        <v>12</v>
+      </c>
+      <c r="E41" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>153</v>
       </c>
       <c r="B42">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="C42" t="s">
-        <v>5</v>
+        <v>158</v>
       </c>
       <c r="D42" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E42" t="s">
-        <v>43</v>
+        <v>154</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>50</v>
+        <v>190</v>
       </c>
       <c r="B43">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C43" t="s">
-        <v>5</v>
+        <v>189</v>
       </c>
       <c r="D43" t="s">
-        <v>17</v>
-      </c>
-      <c r="E43" t="s">
-        <v>43</v>
+        <v>170</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B44">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="C44" t="s">
         <v>5</v>
       </c>
       <c r="D44" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E44" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B45">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="C45" t="s">
         <v>5</v>
       </c>
       <c r="D45" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E45" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B46">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="C46" t="s">
         <v>5</v>
       </c>
       <c r="D46" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E46" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B47">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="C47" t="s">
         <v>5</v>
       </c>
       <c r="D47" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E47" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B48">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="C48" t="s">
-        <v>163</v>
+        <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E48" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>153</v>
+        <v>49</v>
       </c>
       <c r="B49">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="C49" t="s">
-        <v>163</v>
+        <v>5</v>
       </c>
       <c r="D49" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E49" t="s">
-        <v>212</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>154</v>
+        <v>50</v>
       </c>
       <c r="B50">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="C50" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D50" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E50" t="s">
-        <v>155</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>57</v>
+        <v>148</v>
       </c>
       <c r="B51">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="C51" t="s">
-        <v>5</v>
+        <v>158</v>
       </c>
       <c r="D51" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E51" t="s">
-        <v>43</v>
+        <v>206</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>58</v>
+        <v>149</v>
       </c>
       <c r="B52">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="C52" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D52" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E52" t="s">
-        <v>59</v>
+        <v>150</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B53">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="C53" t="s">
-        <v>163</v>
+        <v>5</v>
       </c>
       <c r="D53" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E53" t="s">
-        <v>77</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B54">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="C54" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D54" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E54" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B55">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="C55" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D55" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E55" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B56">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="C56" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D56" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E56" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B57">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="C57" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D57" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E57" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B58">
-        <v>1124</v>
+        <v>1117</v>
       </c>
       <c r="C58" t="s">
-        <v>68</v>
+        <v>158</v>
       </c>
       <c r="D58" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E58" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B59">
-        <v>1125</v>
+        <v>1118</v>
       </c>
       <c r="C59" t="s">
-        <v>71</v>
+        <v>158</v>
       </c>
       <c r="D59" t="s">
         <v>2</v>
       </c>
       <c r="E59" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B60">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="C60" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D60" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E60" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>191</v>
+        <v>65</v>
       </c>
       <c r="B61">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="C61" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D61" t="s">
         <v>2</v>
       </c>
       <c r="E61" t="s">
-        <v>192</v>
+        <v>67</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B62">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="C62" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D62" t="s">
-        <v>17</v>
+        <v>12</v>
+      </c>
+      <c r="E62" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>149</v>
+        <v>185</v>
       </c>
       <c r="B63">
-        <v>1131</v>
+        <v>1127</v>
       </c>
       <c r="C63" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="D63" t="s">
         <v>2</v>
       </c>
       <c r="E63" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>162</v>
+        <v>71</v>
       </c>
       <c r="B64">
-        <v>1132</v>
+        <v>1128</v>
       </c>
       <c r="C64" t="s">
-        <v>163</v>
+        <v>70</v>
       </c>
       <c r="D64" t="s">
-        <v>17</v>
-      </c>
-      <c r="E64" t="s">
-        <v>164</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="B65">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="C65" t="s">
-        <v>163</v>
+        <v>31</v>
       </c>
       <c r="D65" t="s">
         <v>2</v>
       </c>
       <c r="E65" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B66">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="C66" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D66" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E66" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="B67">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="C67" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D67" t="s">
         <v>2</v>
       </c>
       <c r="E67" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B68">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="C68" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D68" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E68" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B69">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="C69" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D69" t="s">
         <v>2</v>
       </c>
       <c r="E69" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>198</v>
+        <v>163</v>
       </c>
       <c r="B70">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="C70" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D70" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E70" t="s">
-        <v>197</v>
+        <v>164</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>200</v>
+        <v>165</v>
       </c>
       <c r="B71">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="C71" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D71" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E71" t="s">
-        <v>201</v>
+        <v>167</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="B72">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="C72" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D72" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E72" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="B73">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="C73" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D73" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E73" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="B74">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="C74" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D74" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E74" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>97</v>
+        <v>204</v>
       </c>
       <c r="B75">
-        <v>2000</v>
+        <v>1141</v>
       </c>
       <c r="C75" t="s">
-        <v>96</v>
+        <v>158</v>
       </c>
       <c r="D75" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E75" t="s">
-        <v>24</v>
+        <v>205</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>111</v>
+        <v>203</v>
       </c>
       <c r="B76">
-        <v>2001</v>
+        <v>1142</v>
       </c>
       <c r="C76" t="s">
-        <v>96</v>
+        <v>158</v>
       </c>
       <c r="D76" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E76" t="s">
-        <v>133</v>
+        <v>207</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B77">
-        <v>2002</v>
+        <v>2000</v>
       </c>
       <c r="C77" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D77" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E77" t="s">
-        <v>126</v>
+        <v>19</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B78">
-        <v>2003</v>
+        <v>2001</v>
       </c>
       <c r="C78" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D78" t="s">
         <v>2</v>
       </c>
       <c r="E78" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B79">
-        <v>2004</v>
+        <v>2002</v>
       </c>
       <c r="C79" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D79" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E79" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B80">
-        <v>2005</v>
+        <v>2003</v>
       </c>
       <c r="C80" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D80" t="s">
         <v>2</v>
       </c>
       <c r="E80" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B81">
-        <v>2006</v>
+        <v>2004</v>
       </c>
       <c r="C81" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D81" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E81" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B82">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="C82" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D82" t="s">
         <v>2</v>
       </c>
       <c r="E82" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B83">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="C83" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D83" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E83" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B84">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="C84" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D84" t="s">
         <v>2</v>
       </c>
       <c r="E84" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B85">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="C85" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D85" t="s">
-        <v>17</v>
+        <v>12</v>
+      </c>
+      <c r="E85" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B86">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="C86" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D86" t="s">
         <v>2</v>
       </c>
       <c r="E86" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B87">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="C87" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D87" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B88">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="C88" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D88" t="s">
         <v>2</v>
       </c>
       <c r="E88" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="B89">
-        <v>2019</v>
+        <v>2012</v>
       </c>
       <c r="C89" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D89" t="s">
-        <v>2</v>
-      </c>
-      <c r="E89" t="s">
-        <v>138</v>
+        <v>12</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B90">
-        <v>2020</v>
+        <v>2013</v>
       </c>
       <c r="C90" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D90" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E90" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B91">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="C91" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D91" t="s">
         <v>2</v>
       </c>
       <c r="E91" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="B92">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="C92" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D92" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E92" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B93">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="C93" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D93" t="s">
         <v>2</v>
       </c>
       <c r="E93" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B94">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="C94" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D94" t="s">
         <v>2</v>
       </c>
       <c r="E94" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="B95">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="C95" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D95" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E95" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="B96">
-        <v>2026</v>
+        <v>2024</v>
       </c>
       <c r="C96" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D96" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="E96" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B97">
-        <v>2027</v>
+        <v>2025</v>
       </c>
       <c r="C97" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D97" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B98">
-        <v>2028</v>
+        <v>2026</v>
       </c>
       <c r="C98" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D98" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="B99">
-        <v>2090</v>
+        <v>2027</v>
       </c>
       <c r="C99" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D99" t="s">
-        <v>2</v>
-      </c>
-      <c r="E99" t="s">
-        <v>143</v>
+        <v>12</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="B100">
-        <v>2091</v>
+        <v>2028</v>
       </c>
       <c r="C100" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D100" t="s">
-        <v>2</v>
-      </c>
-      <c r="E100" t="s">
-        <v>132</v>
+        <v>12</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B101">
-        <v>2092</v>
+        <v>2090</v>
       </c>
       <c r="C101" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D101" t="s">
         <v>2</v>
       </c>
       <c r="E101" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B102">
-        <v>2093</v>
+        <v>2091</v>
       </c>
       <c r="C102" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D102" t="s">
         <v>2</v>
       </c>
       <c r="E102" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B103">
-        <v>2094</v>
+        <v>2092</v>
       </c>
       <c r="C103" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D103" t="s">
         <v>2</v>
       </c>
       <c r="E103" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>186</v>
+        <v>119</v>
       </c>
       <c r="B104">
-        <v>3000</v>
+        <v>2093</v>
       </c>
       <c r="C104" t="s">
-        <v>188</v>
+        <v>91</v>
       </c>
       <c r="D104" t="s">
-        <v>176</v>
+        <v>2</v>
       </c>
       <c r="E104" t="s">
-        <v>189</v>
+        <v>140</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>187</v>
+        <v>120</v>
       </c>
       <c r="B105">
-        <v>3001</v>
+        <v>2094</v>
       </c>
       <c r="C105" t="s">
-        <v>188</v>
+        <v>91</v>
       </c>
       <c r="D105" t="s">
-        <v>176</v>
+        <v>2</v>
       </c>
       <c r="E105" t="s">
-        <v>190</v>
+        <v>141</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -3339,234 +3351,268 @@
         <v>180</v>
       </c>
       <c r="B106">
-        <v>3002</v>
+        <v>3000</v>
       </c>
       <c r="C106" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="D106" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E106" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B107">
-        <v>3003</v>
+        <v>3001</v>
       </c>
       <c r="C107" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="D107" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E107" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="B108">
-        <v>3004</v>
+        <v>3002</v>
       </c>
       <c r="C108" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D108" t="s">
-        <v>176</v>
+        <v>170</v>
+      </c>
+      <c r="E108" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B109">
-        <v>3005</v>
+        <v>3003</v>
       </c>
       <c r="C109" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D109" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E109" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>203</v>
+        <v>178</v>
       </c>
       <c r="B110">
-        <v>3006</v>
+        <v>3004</v>
       </c>
       <c r="C110" t="s">
-        <v>204</v>
+        <v>171</v>
       </c>
       <c r="D110" t="s">
-        <v>176</v>
-      </c>
-      <c r="E110" t="s">
-        <v>205</v>
+        <v>170</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>206</v>
+        <v>176</v>
       </c>
       <c r="B111">
-        <v>3007</v>
+        <v>3005</v>
       </c>
       <c r="C111" t="s">
-        <v>204</v>
+        <v>171</v>
       </c>
       <c r="D111" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E111" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="B112">
-        <v>3008</v>
+        <v>3006</v>
       </c>
       <c r="C112" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="D112" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E112" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="B113">
-        <v>3100</v>
+        <v>3007</v>
       </c>
       <c r="C113" t="s">
-        <v>31</v>
+        <v>198</v>
       </c>
       <c r="D113" t="s">
-        <v>17</v>
+        <v>170</v>
       </c>
       <c r="E113" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="B114">
-        <v>3101</v>
+        <v>3008</v>
       </c>
       <c r="C114" t="s">
-        <v>31</v>
+        <v>198</v>
       </c>
       <c r="D114" t="s">
-        <v>17</v>
+        <v>170</v>
       </c>
       <c r="E114" t="s">
-        <v>224</v>
+        <v>199</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="B115">
-        <v>3102</v>
+        <v>3100</v>
       </c>
       <c r="C115" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D115" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E115" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="B116">
-        <v>3103</v>
+        <v>3101</v>
       </c>
       <c r="C116" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D116" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E116" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>83</v>
+        <v>217</v>
       </c>
       <c r="B117">
-        <v>4000</v>
+        <v>3102</v>
       </c>
       <c r="C117" t="s">
-        <v>84</v>
+        <v>26</v>
       </c>
       <c r="D117" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E117" t="s">
-        <v>85</v>
+        <v>219</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>86</v>
+        <v>220</v>
       </c>
       <c r="B118">
-        <v>4001</v>
+        <v>3103</v>
       </c>
       <c r="C118" t="s">
-        <v>84</v>
+        <v>26</v>
       </c>
       <c r="D118" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E118" t="s">
-        <v>87</v>
+        <v>221</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>193</v>
+        <v>78</v>
       </c>
       <c r="B119">
+        <v>4000</v>
+      </c>
+      <c r="C119" t="s">
+        <v>79</v>
+      </c>
+      <c r="D119" t="s">
+        <v>2</v>
+      </c>
+      <c r="E119" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>81</v>
+      </c>
+      <c r="B120">
+        <v>4001</v>
+      </c>
+      <c r="C120" t="s">
+        <v>79</v>
+      </c>
+      <c r="D120" t="s">
+        <v>12</v>
+      </c>
+      <c r="E120" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>187</v>
+      </c>
+      <c r="B121">
         <v>4002</v>
       </c>
-      <c r="C119" t="s">
-        <v>84</v>
-      </c>
-      <c r="D119" t="s">
-        <v>17</v>
-      </c>
-      <c r="E119" t="s">
-        <v>194</v>
+      <c r="C121" t="s">
+        <v>79</v>
+      </c>
+      <c r="D121" t="s">
+        <v>12</v>
+      </c>
+      <c r="E121" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started moving kits to EF
</commit_message>
<xml_diff>
--- a/netcalls.xlsx
+++ b/netcalls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\UncreatedWarfare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EC066B-66E7-4DD2-A0F9-378292A4090E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C89D99-4536-40F0-8A57-A0A5E9073941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="6585" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="5250" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="netcalls" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="224">
   <si>
     <t>SendPlayerList</t>
   </si>
@@ -172,12 +172,6 @@
     <t>RevokeHelperRequest</t>
   </si>
   <si>
-    <t>CreateKit</t>
-  </si>
-  <si>
-    <t>Kit? kit</t>
-  </si>
-  <si>
     <t>SendVehicleTeamkilled</t>
   </si>
   <si>
@@ -188,24 +182,6 @@
   </si>
   <si>
     <t>SendKitClass</t>
-  </si>
-  <si>
-    <t>RequestKit</t>
-  </si>
-  <si>
-    <t>RequestKits</t>
-  </si>
-  <si>
-    <t>string[] kitNames</t>
-  </si>
-  <si>
-    <t>SendKit</t>
-  </si>
-  <si>
-    <t>SendKits</t>
-  </si>
-  <si>
-    <t>Kit?[] kit</t>
   </si>
   <si>
     <t>SendDiscordKeyState</t>
@@ -1260,10 +1236,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E121" totalsRowShown="0">
-  <autoFilter ref="A1:E121" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E121">
-    <sortCondition ref="B1:B121"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E116" totalsRowShown="0">
+  <autoFilter ref="A1:E116" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E116">
+    <sortCondition ref="B1:B116"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="NetCall Field Name"/>
@@ -1573,10 +1549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E121"/>
+  <dimension ref="A1:E116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1590,19 +1566,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1636,7 +1612,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1653,7 +1629,7 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1670,7 +1646,7 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1687,7 +1663,7 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1704,7 +1680,7 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1721,7 +1697,7 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1738,24 +1714,24 @@
         <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B10">
         <v>1008</v>
       </c>
       <c r="C10" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="D10" t="s">
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1772,7 +1748,7 @@
         <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1789,7 +1765,7 @@
         <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1806,75 +1782,75 @@
         <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B14">
         <v>1012</v>
       </c>
       <c r="C14" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D14" t="s">
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B15">
         <v>1013</v>
       </c>
       <c r="C15" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D15" t="s">
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B16">
         <v>1014</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D16" t="s">
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B17">
         <v>1015</v>
       </c>
       <c r="C17" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D17" t="s">
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1947,7 +1923,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B22">
         <v>1020</v>
@@ -1959,12 +1935,12 @@
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="B23">
         <v>1021</v>
@@ -1976,12 +1952,12 @@
         <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B24">
         <v>1022</v>
@@ -1993,12 +1969,12 @@
         <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B25">
         <v>1023</v>
@@ -2010,7 +1986,7 @@
         <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2032,7 +2008,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="B27">
         <v>1025</v>
@@ -2044,12 +2020,12 @@
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B28">
         <v>1026</v>
@@ -2061,7 +2037,7 @@
         <v>12</v>
       </c>
       <c r="E28" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2233,7 +2209,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B39">
         <v>1037</v>
@@ -2245,72 +2221,72 @@
         <v>2</v>
       </c>
       <c r="E39" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B40">
         <v>1038</v>
       </c>
       <c r="C40" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="D40" t="s">
         <v>2</v>
       </c>
       <c r="E40" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B41">
         <v>1100</v>
       </c>
       <c r="C41" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="D41" t="s">
         <v>12</v>
       </c>
       <c r="E41" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B42">
         <v>1101</v>
       </c>
       <c r="C42" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="D42" t="s">
         <v>2</v>
       </c>
       <c r="E42" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="B43">
         <v>1102</v>
       </c>
       <c r="C43" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D43" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2417,70 +2393,70 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>140</v>
       </c>
       <c r="B50">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="C50" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="D50" t="s">
         <v>12</v>
       </c>
       <c r="E50" t="s">
-        <v>51</v>
+        <v>198</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B51">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="C51" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="D51" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E51" t="s">
-        <v>206</v>
+        <v>142</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>149</v>
+        <v>50</v>
       </c>
       <c r="B52">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="C52" t="s">
-        <v>158</v>
+        <v>5</v>
       </c>
       <c r="D52" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E52" t="s">
-        <v>150</v>
+        <v>38</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>1113</v>
+      </c>
+      <c r="C53" t="s">
+        <v>150</v>
+      </c>
+      <c r="D53" t="s">
+        <v>12</v>
+      </c>
+      <c r="E53" t="s">
         <v>52</v>
-      </c>
-      <c r="B53">
-        <v>1112</v>
-      </c>
-      <c r="C53" t="s">
-        <v>5</v>
-      </c>
-      <c r="D53" t="s">
-        <v>12</v>
-      </c>
-      <c r="E53" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -2488,200 +2464,200 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="C54" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="D54" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E54" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>1124</v>
+      </c>
+      <c r="C55" t="s">
         <v>55</v>
       </c>
-      <c r="B55">
-        <v>1114</v>
-      </c>
-      <c r="C55" t="s">
-        <v>158</v>
-      </c>
       <c r="D55" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E55" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B56">
-        <v>1115</v>
+        <v>1125</v>
       </c>
       <c r="C56" t="s">
-        <v>158</v>
+        <v>58</v>
       </c>
       <c r="D56" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E56" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B57">
-        <v>1116</v>
+        <v>1126</v>
       </c>
       <c r="C57" t="s">
-        <v>158</v>
+        <v>58</v>
       </c>
       <c r="D57" t="s">
         <v>12</v>
       </c>
       <c r="E57" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>59</v>
+        <v>177</v>
       </c>
       <c r="B58">
-        <v>1117</v>
+        <v>1127</v>
       </c>
       <c r="C58" t="s">
-        <v>158</v>
+        <v>62</v>
       </c>
       <c r="D58" t="s">
         <v>2</v>
       </c>
       <c r="E58" t="s">
-        <v>51</v>
+        <v>178</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B59">
-        <v>1118</v>
+        <v>1128</v>
       </c>
       <c r="C59" t="s">
-        <v>158</v>
+        <v>62</v>
       </c>
       <c r="D59" t="s">
-        <v>2</v>
-      </c>
-      <c r="E59" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>136</v>
       </c>
       <c r="B60">
-        <v>1124</v>
+        <v>1131</v>
       </c>
       <c r="C60" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="D60" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E60" t="s">
-        <v>64</v>
+        <v>137</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>65</v>
+        <v>149</v>
       </c>
       <c r="B61">
-        <v>1125</v>
+        <v>1132</v>
       </c>
       <c r="C61" t="s">
-        <v>66</v>
+        <v>150</v>
       </c>
       <c r="D61" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E61" t="s">
-        <v>67</v>
+        <v>151</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>68</v>
+        <v>147</v>
       </c>
       <c r="B62">
-        <v>1126</v>
+        <v>1133</v>
       </c>
       <c r="C62" t="s">
-        <v>66</v>
+        <v>150</v>
       </c>
       <c r="D62" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E62" t="s">
-        <v>69</v>
+        <v>148</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>185</v>
+        <v>152</v>
       </c>
       <c r="B63">
-        <v>1127</v>
+        <v>1134</v>
       </c>
       <c r="C63" t="s">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="D63" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E63" t="s">
-        <v>186</v>
+        <v>153</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>71</v>
+        <v>154</v>
       </c>
       <c r="B64">
-        <v>1128</v>
+        <v>1135</v>
       </c>
       <c r="C64" t="s">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="D64" t="s">
-        <v>12</v>
+        <v>2</v>
+      </c>
+      <c r="E64" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="B65">
-        <v>1131</v>
+        <v>1136</v>
       </c>
       <c r="C65" t="s">
-        <v>31</v>
+        <v>150</v>
       </c>
       <c r="D65" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E65" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -2689,13 +2665,13 @@
         <v>157</v>
       </c>
       <c r="B66">
-        <v>1132</v>
+        <v>1137</v>
       </c>
       <c r="C66" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="D66" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E66" t="s">
         <v>159</v>
@@ -2703,220 +2679,220 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>155</v>
+        <v>184</v>
       </c>
       <c r="B67">
-        <v>1133</v>
+        <v>1138</v>
       </c>
       <c r="C67" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="D67" t="s">
         <v>2</v>
       </c>
       <c r="E67" t="s">
-        <v>156</v>
+        <v>183</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>160</v>
+        <v>186</v>
       </c>
       <c r="B68">
-        <v>1134</v>
+        <v>1139</v>
       </c>
       <c r="C68" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="D68" t="s">
         <v>12</v>
       </c>
       <c r="E68" t="s">
-        <v>161</v>
+        <v>187</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>162</v>
+        <v>185</v>
       </c>
       <c r="B69">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="C69" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="D69" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E69" t="s">
-        <v>166</v>
+        <v>188</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>163</v>
+        <v>196</v>
       </c>
       <c r="B70">
-        <v>1136</v>
+        <v>1141</v>
       </c>
       <c r="C70" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="D70" t="s">
         <v>12</v>
       </c>
       <c r="E70" t="s">
-        <v>164</v>
+        <v>197</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>165</v>
+        <v>195</v>
       </c>
       <c r="B71">
-        <v>1137</v>
+        <v>1142</v>
       </c>
       <c r="C71" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="D71" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E71" t="s">
-        <v>167</v>
+        <v>199</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>192</v>
+        <v>84</v>
       </c>
       <c r="B72">
-        <v>1138</v>
+        <v>2000</v>
       </c>
       <c r="C72" t="s">
-        <v>158</v>
+        <v>83</v>
       </c>
       <c r="D72" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E72" t="s">
-        <v>191</v>
+        <v>19</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>194</v>
+        <v>98</v>
       </c>
       <c r="B73">
-        <v>1139</v>
+        <v>2001</v>
       </c>
       <c r="C73" t="s">
-        <v>158</v>
+        <v>83</v>
       </c>
       <c r="D73" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E73" t="s">
-        <v>195</v>
+        <v>120</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>193</v>
+        <v>85</v>
       </c>
       <c r="B74">
-        <v>1140</v>
+        <v>2002</v>
       </c>
       <c r="C74" t="s">
-        <v>158</v>
+        <v>83</v>
       </c>
       <c r="D74" t="s">
         <v>12</v>
       </c>
       <c r="E74" t="s">
-        <v>196</v>
+        <v>113</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>204</v>
+        <v>96</v>
       </c>
       <c r="B75">
-        <v>1141</v>
+        <v>2003</v>
       </c>
       <c r="C75" t="s">
-        <v>158</v>
+        <v>83</v>
       </c>
       <c r="D75" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E75" t="s">
-        <v>205</v>
+        <v>118</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>203</v>
+        <v>86</v>
       </c>
       <c r="B76">
-        <v>1142</v>
+        <v>2004</v>
       </c>
       <c r="C76" t="s">
-        <v>158</v>
+        <v>83</v>
       </c>
       <c r="D76" t="s">
         <v>12</v>
       </c>
       <c r="E76" t="s">
-        <v>207</v>
+        <v>114</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B77">
-        <v>2000</v>
+        <v>2005</v>
       </c>
       <c r="C77" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D77" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E77" t="s">
-        <v>19</v>
+        <v>119</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="B78">
-        <v>2001</v>
+        <v>2006</v>
       </c>
       <c r="C78" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D78" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E78" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B79">
-        <v>2002</v>
+        <v>2007</v>
       </c>
       <c r="C79" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D79" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E79" t="s">
         <v>121</v>
@@ -2924,33 +2900,33 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="B80">
-        <v>2003</v>
+        <v>2008</v>
       </c>
       <c r="C80" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D80" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E80" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B81">
-        <v>2004</v>
+        <v>2009</v>
       </c>
       <c r="C81" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D81" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E81" t="s">
         <v>122</v>
@@ -2958,33 +2934,30 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="B82">
-        <v>2005</v>
+        <v>2010</v>
       </c>
       <c r="C82" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D82" t="s">
-        <v>2</v>
-      </c>
-      <c r="E82" t="s">
-        <v>127</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B83">
-        <v>2006</v>
+        <v>2011</v>
       </c>
       <c r="C83" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D83" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E83" t="s">
         <v>123</v>
@@ -2992,33 +2965,30 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="B84">
-        <v>2007</v>
+        <v>2012</v>
       </c>
       <c r="C84" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D84" t="s">
-        <v>2</v>
-      </c>
-      <c r="E84" t="s">
-        <v>129</v>
+        <v>12</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B85">
-        <v>2008</v>
+        <v>2013</v>
       </c>
       <c r="C85" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D85" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E85" t="s">
         <v>124</v>
@@ -3026,593 +2996,514 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B86">
-        <v>2009</v>
+        <v>2019</v>
       </c>
       <c r="C86" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D86" t="s">
         <v>2</v>
       </c>
       <c r="E86" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B87">
-        <v>2010</v>
+        <v>2020</v>
       </c>
       <c r="C87" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D87" t="s">
         <v>12</v>
+      </c>
+      <c r="E87" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B88">
-        <v>2011</v>
+        <v>2021</v>
       </c>
       <c r="C88" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D88" t="s">
         <v>2</v>
       </c>
       <c r="E88" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="B89">
-        <v>2012</v>
+        <v>2022</v>
       </c>
       <c r="C89" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D89" t="s">
-        <v>12</v>
+        <v>2</v>
+      </c>
+      <c r="E89" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B90">
-        <v>2013</v>
+        <v>2023</v>
       </c>
       <c r="C90" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D90" t="s">
         <v>2</v>
       </c>
       <c r="E90" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B91">
-        <v>2019</v>
+        <v>2024</v>
       </c>
       <c r="C91" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D91" t="s">
         <v>2</v>
       </c>
       <c r="E91" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B92">
-        <v>2020</v>
+        <v>2025</v>
       </c>
       <c r="C92" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D92" t="s">
         <v>12</v>
-      </c>
-      <c r="E92" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="B93">
-        <v>2021</v>
+        <v>2026</v>
       </c>
       <c r="C93" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D93" t="s">
-        <v>2</v>
-      </c>
-      <c r="E93" t="s">
-        <v>134</v>
+        <v>12</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="B94">
-        <v>2022</v>
+        <v>2027</v>
       </c>
       <c r="C94" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D94" t="s">
-        <v>2</v>
-      </c>
-      <c r="E94" t="s">
-        <v>135</v>
+        <v>12</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="B95">
-        <v>2023</v>
+        <v>2028</v>
       </c>
       <c r="C95" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D95" t="s">
-        <v>2</v>
-      </c>
-      <c r="E95" t="s">
-        <v>136</v>
+        <v>12</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B96">
-        <v>2024</v>
+        <v>2090</v>
       </c>
       <c r="C96" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D96" t="s">
         <v>2</v>
       </c>
       <c r="E96" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="B97">
-        <v>2025</v>
+        <v>2091</v>
       </c>
       <c r="C97" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D97" t="s">
-        <v>12</v>
+        <v>2</v>
+      </c>
+      <c r="E97" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="B98">
-        <v>2026</v>
+        <v>2092</v>
       </c>
       <c r="C98" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D98" t="s">
-        <v>12</v>
+        <v>2</v>
+      </c>
+      <c r="E98" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="B99">
-        <v>2027</v>
+        <v>2093</v>
       </c>
       <c r="C99" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D99" t="s">
-        <v>12</v>
+        <v>2</v>
+      </c>
+      <c r="E99" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="B100">
-        <v>2028</v>
+        <v>2094</v>
       </c>
       <c r="C100" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D100" t="s">
-        <v>12</v>
+        <v>2</v>
+      </c>
+      <c r="E100" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>116</v>
+        <v>172</v>
       </c>
       <c r="B101">
-        <v>2090</v>
+        <v>3000</v>
       </c>
       <c r="C101" t="s">
-        <v>91</v>
+        <v>174</v>
       </c>
       <c r="D101" t="s">
-        <v>2</v>
+        <v>162</v>
       </c>
       <c r="E101" t="s">
-        <v>138</v>
+        <v>175</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>117</v>
+        <v>173</v>
       </c>
       <c r="B102">
-        <v>2091</v>
+        <v>3001</v>
       </c>
       <c r="C102" t="s">
-        <v>91</v>
+        <v>174</v>
       </c>
       <c r="D102" t="s">
-        <v>2</v>
+        <v>162</v>
       </c>
       <c r="E102" t="s">
-        <v>127</v>
+        <v>176</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>118</v>
+        <v>166</v>
       </c>
       <c r="B103">
-        <v>2092</v>
+        <v>3002</v>
       </c>
       <c r="C103" t="s">
-        <v>91</v>
+        <v>163</v>
       </c>
       <c r="D103" t="s">
-        <v>2</v>
+        <v>162</v>
       </c>
       <c r="E103" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>119</v>
+        <v>165</v>
       </c>
       <c r="B104">
-        <v>2093</v>
+        <v>3003</v>
       </c>
       <c r="C104" t="s">
-        <v>91</v>
+        <v>163</v>
       </c>
       <c r="D104" t="s">
-        <v>2</v>
+        <v>162</v>
       </c>
       <c r="E104" t="s">
-        <v>140</v>
+        <v>164</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>120</v>
+        <v>170</v>
       </c>
       <c r="B105">
-        <v>2094</v>
+        <v>3004</v>
       </c>
       <c r="C105" t="s">
-        <v>91</v>
+        <v>163</v>
       </c>
       <c r="D105" t="s">
-        <v>2</v>
-      </c>
-      <c r="E105" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="B106">
-        <v>3000</v>
+        <v>3005</v>
       </c>
       <c r="C106" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="D106" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="E106" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="B107">
-        <v>3001</v>
+        <v>3006</v>
       </c>
       <c r="C107" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="D107" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="E107" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="B108">
-        <v>3002</v>
+        <v>3007</v>
       </c>
       <c r="C108" t="s">
-        <v>171</v>
+        <v>190</v>
       </c>
       <c r="D108" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="E108" t="s">
-        <v>175</v>
+        <v>193</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>173</v>
+        <v>194</v>
       </c>
       <c r="B109">
-        <v>3003</v>
+        <v>3008</v>
       </c>
       <c r="C109" t="s">
-        <v>171</v>
+        <v>190</v>
       </c>
       <c r="D109" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="E109" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>178</v>
+        <v>206</v>
       </c>
       <c r="B110">
-        <v>3004</v>
+        <v>3100</v>
       </c>
       <c r="C110" t="s">
-        <v>171</v>
+        <v>26</v>
       </c>
       <c r="D110" t="s">
-        <v>170</v>
+        <v>12</v>
+      </c>
+      <c r="E110" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>176</v>
+        <v>208</v>
       </c>
       <c r="B111">
-        <v>3005</v>
+        <v>3101</v>
       </c>
       <c r="C111" t="s">
-        <v>171</v>
+        <v>26</v>
       </c>
       <c r="D111" t="s">
-        <v>170</v>
+        <v>12</v>
       </c>
       <c r="E111" t="s">
-        <v>177</v>
+        <v>210</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>197</v>
+        <v>209</v>
       </c>
       <c r="B112">
-        <v>3006</v>
+        <v>3102</v>
       </c>
       <c r="C112" t="s">
-        <v>198</v>
+        <v>26</v>
       </c>
       <c r="D112" t="s">
-        <v>170</v>
+        <v>12</v>
       </c>
       <c r="E112" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="B113">
-        <v>3007</v>
+        <v>3103</v>
       </c>
       <c r="C113" t="s">
-        <v>198</v>
+        <v>26</v>
       </c>
       <c r="D113" t="s">
-        <v>170</v>
+        <v>12</v>
       </c>
       <c r="E113" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>202</v>
+        <v>70</v>
       </c>
       <c r="B114">
-        <v>3008</v>
+        <v>4000</v>
       </c>
       <c r="C114" t="s">
-        <v>198</v>
+        <v>71</v>
       </c>
       <c r="D114" t="s">
-        <v>170</v>
+        <v>2</v>
       </c>
       <c r="E114" t="s">
-        <v>199</v>
+        <v>72</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>214</v>
+        <v>73</v>
       </c>
       <c r="B115">
-        <v>3100</v>
+        <v>4001</v>
       </c>
       <c r="C115" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="D115" t="s">
         <v>12</v>
       </c>
       <c r="E115" t="s">
-        <v>215</v>
+        <v>74</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>216</v>
+        <v>179</v>
       </c>
       <c r="B116">
-        <v>3101</v>
+        <v>4002</v>
       </c>
       <c r="C116" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="D116" t="s">
         <v>12</v>
       </c>
       <c r="E116" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>217</v>
-      </c>
-      <c r="B117">
-        <v>3102</v>
-      </c>
-      <c r="C117" t="s">
-        <v>26</v>
-      </c>
-      <c r="D117" t="s">
-        <v>12</v>
-      </c>
-      <c r="E117" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>220</v>
-      </c>
-      <c r="B118">
-        <v>3103</v>
-      </c>
-      <c r="C118" t="s">
-        <v>26</v>
-      </c>
-      <c r="D118" t="s">
-        <v>12</v>
-      </c>
-      <c r="E118" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>78</v>
-      </c>
-      <c r="B119">
-        <v>4000</v>
-      </c>
-      <c r="C119" t="s">
-        <v>79</v>
-      </c>
-      <c r="D119" t="s">
-        <v>2</v>
-      </c>
-      <c r="E119" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>81</v>
-      </c>
-      <c r="B120">
-        <v>4001</v>
-      </c>
-      <c r="C120" t="s">
-        <v>79</v>
-      </c>
-      <c r="D120" t="s">
-        <v>12</v>
-      </c>
-      <c r="E120" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>187</v>
-      </c>
-      <c r="B121">
-        <v>4002</v>
-      </c>
-      <c r="C121" t="s">
-        <v>79</v>
-      </c>
-      <c r="D121" t="s">
-        <v>12</v>
-      </c>
-      <c r="E121" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finally removed config sync and family, fixed some bugs relating to the kit cache and other minor kit bugs.
</commit_message>
<xml_diff>
--- a/netcalls.xlsx
+++ b/netcalls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\UncreatedWarfare\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\UncreatedStaff\UncreatedWarfare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C89D99-4536-40F0-8A57-A0A5E9073941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD71E0D-ABA1-42FD-AC9A-755C4E513709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5250" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="27580" windowHeight="17740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="netcalls" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="211">
   <si>
     <t>SendPlayerList</t>
   </si>
@@ -511,46 +511,7 @@
     <t>FROM_EITHER</t>
   </si>
   <si>
-    <t>ConfigSync.NetCalls</t>
-  </si>
-  <si>
-    <t>SyncPacket packet</t>
-  </si>
-  <si>
-    <t>ReceiveSyncPacket</t>
-  </si>
-  <si>
-    <t>SendSingleProperty</t>
-  </si>
-  <si>
-    <t>PropertyValue property</t>
-  </si>
-  <si>
-    <t>BulkSendProperties</t>
-  </si>
-  <si>
-    <t>&lt;custom&gt;</t>
-  </si>
-  <si>
-    <t>RequestFullSyncPacket</t>
-  </si>
-  <si>
     <t>Data.NetCalls</t>
-  </si>
-  <si>
-    <t>MulticastListItemUpdated</t>
-  </si>
-  <si>
-    <t>MulticastListItemsUpdated</t>
-  </si>
-  <si>
-    <t>ListSync.NetCalls</t>
-  </si>
-  <si>
-    <t>ushort syncId, int pk</t>
-  </si>
-  <si>
-    <t>ushort syncId, int[] pks</t>
   </si>
   <si>
     <t>SendLog</t>
@@ -1236,10 +1197,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E116" totalsRowShown="0">
-  <autoFilter ref="A1:E116" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E116">
-    <sortCondition ref="B1:B116"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E110" totalsRowShown="0">
+  <autoFilter ref="A1:E110" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E110">
+    <sortCondition ref="B1:B110"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="NetCall Field Name"/>
@@ -1549,22 +1510,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E116"/>
+  <dimension ref="A1:E110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.5703125" customWidth="1"/>
+    <col min="1" max="1" width="38.54296875" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.26953125" customWidth="1"/>
+    <col min="5" max="5" width="81.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>65</v>
       </c>
@@ -1581,7 +1542,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1598,7 +1559,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1612,10 +1573,10 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1629,10 +1590,10 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1646,10 +1607,10 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1663,10 +1624,10 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1680,10 +1641,10 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1697,10 +1658,10 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1714,10 +1675,10 @@
         <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>138</v>
       </c>
@@ -1725,7 +1686,7 @@
         <v>1008</v>
       </c>
       <c r="C10" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="D10" t="s">
         <v>2</v>
@@ -1734,7 +1695,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1748,10 +1709,10 @@
         <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1765,10 +1726,10 @@
         <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1782,10 +1743,10 @@
         <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>75</v>
       </c>
@@ -1802,7 +1763,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>76</v>
       </c>
@@ -1819,7 +1780,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>77</v>
       </c>
@@ -1836,7 +1797,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>78</v>
       </c>
@@ -1853,7 +1814,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1870,7 +1831,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1887,7 +1848,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1904,7 +1865,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1921,7 +1882,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>160</v>
       </c>
@@ -1935,10 +1896,10 @@
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>161</v>
       </c>
@@ -1952,12 +1913,12 @@
         <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="B24">
         <v>1022</v>
@@ -1969,10 +1930,10 @@
         <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>134</v>
       </c>
@@ -1989,7 +1950,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -2006,9 +1967,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="B27">
         <v>1025</v>
@@ -2020,12 +1981,12 @@
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="B28">
         <v>1026</v>
@@ -2037,10 +1998,10 @@
         <v>12</v>
       </c>
       <c r="E28" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -2057,7 +2018,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -2074,7 +2035,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -2088,7 +2049,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -2105,7 +2066,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -2122,7 +2083,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -2139,7 +2100,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -2156,7 +2117,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -2173,7 +2134,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -2190,7 +2151,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -2207,9 +2168,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="B39">
         <v>1037</v>
@@ -2221,12 +2182,12 @@
         <v>2</v>
       </c>
       <c r="E39" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="B40">
         <v>1038</v>
@@ -2238,10 +2199,10 @@
         <v>2</v>
       </c>
       <c r="E40" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>143</v>
       </c>
@@ -2258,7 +2219,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>145</v>
       </c>
@@ -2275,21 +2236,21 @@
         <v>146</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="B43">
         <v>1102</v>
       </c>
       <c r="C43" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="D43" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -2306,7 +2267,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -2323,7 +2284,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -2340,7 +2301,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -2357,7 +2318,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -2374,7 +2335,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -2391,7 +2352,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>140</v>
       </c>
@@ -2405,10 +2366,10 @@
         <v>12</v>
       </c>
       <c r="E50" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>141</v>
       </c>
@@ -2425,7 +2386,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -2442,7 +2403,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -2459,7 +2420,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -2476,7 +2437,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -2493,7 +2454,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>57</v>
       </c>
@@ -2510,7 +2471,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -2527,9 +2488,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="B58">
         <v>1127</v>
@@ -2541,10 +2502,10 @@
         <v>2</v>
       </c>
       <c r="E58" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>63</v>
       </c>
@@ -2558,7 +2519,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>136</v>
       </c>
@@ -2575,7 +2536,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>149</v>
       </c>
@@ -2592,7 +2553,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>147</v>
       </c>
@@ -2609,7 +2570,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>152</v>
       </c>
@@ -2626,7 +2587,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>154</v>
       </c>
@@ -2643,7 +2604,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>155</v>
       </c>
@@ -2660,7 +2621,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>157</v>
       </c>
@@ -2677,9 +2638,9 @@
         <v>159</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="B67">
         <v>1138</v>
@@ -2691,12 +2652,12 @@
         <v>2</v>
       </c>
       <c r="E67" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="B68">
         <v>1139</v>
@@ -2708,12 +2669,12 @@
         <v>12</v>
       </c>
       <c r="E68" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="B69">
         <v>1140</v>
@@ -2725,12 +2686,12 @@
         <v>12</v>
       </c>
       <c r="E69" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="B70">
         <v>1141</v>
@@ -2742,12 +2703,12 @@
         <v>12</v>
       </c>
       <c r="E70" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="B71">
         <v>1142</v>
@@ -2759,10 +2720,10 @@
         <v>12</v>
       </c>
       <c r="E71" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>84</v>
       </c>
@@ -2779,7 +2740,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>98</v>
       </c>
@@ -2796,7 +2757,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>85</v>
       </c>
@@ -2813,7 +2774,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>96</v>
       </c>
@@ -2830,7 +2791,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>86</v>
       </c>
@@ -2847,7 +2808,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>97</v>
       </c>
@@ -2864,7 +2825,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>87</v>
       </c>
@@ -2881,7 +2842,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>99</v>
       </c>
@@ -2898,7 +2859,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>88</v>
       </c>
@@ -2915,7 +2876,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>100</v>
       </c>
@@ -2932,7 +2893,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>89</v>
       </c>
@@ -2946,7 +2907,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>101</v>
       </c>
@@ -2963,7 +2924,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>90</v>
       </c>
@@ -2977,7 +2938,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>102</v>
       </c>
@@ -2994,7 +2955,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>103</v>
       </c>
@@ -3011,7 +2972,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>91</v>
       </c>
@@ -3028,7 +2989,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>104</v>
       </c>
@@ -3045,7 +3006,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>105</v>
       </c>
@@ -3062,7 +3023,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>106</v>
       </c>
@@ -3079,7 +3040,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>107</v>
       </c>
@@ -3096,7 +3057,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>92</v>
       </c>
@@ -3110,7 +3071,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>93</v>
       </c>
@@ -3124,7 +3085,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>94</v>
       </c>
@@ -3138,7 +3099,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>95</v>
       </c>
@@ -3152,7 +3113,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>108</v>
       </c>
@@ -3169,7 +3130,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>109</v>
       </c>
@@ -3186,7 +3147,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>110</v>
       </c>
@@ -3203,7 +3164,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>111</v>
       </c>
@@ -3220,7 +3181,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>112</v>
       </c>
@@ -3237,273 +3198,174 @@
         <v>133</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B101">
-        <v>3000</v>
+        <v>3006</v>
       </c>
       <c r="C101" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D101" t="s">
         <v>162</v>
       </c>
       <c r="E101" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B102">
-        <v>3001</v>
+        <v>3007</v>
       </c>
       <c r="C102" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D102" t="s">
         <v>162</v>
       </c>
       <c r="E102" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
       <c r="B103">
-        <v>3002</v>
+        <v>3008</v>
       </c>
       <c r="C103" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="D103" t="s">
         <v>162</v>
       </c>
       <c r="E103" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>193</v>
+      </c>
+      <c r="B104">
+        <v>3100</v>
+      </c>
+      <c r="C104" t="s">
+        <v>26</v>
+      </c>
+      <c r="D104" t="s">
+        <v>12</v>
+      </c>
+      <c r="E104" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>195</v>
+      </c>
+      <c r="B105">
+        <v>3101</v>
+      </c>
+      <c r="C105" t="s">
+        <v>26</v>
+      </c>
+      <c r="D105" t="s">
+        <v>12</v>
+      </c>
+      <c r="E105" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>196</v>
+      </c>
+      <c r="B106">
+        <v>3102</v>
+      </c>
+      <c r="C106" t="s">
+        <v>26</v>
+      </c>
+      <c r="D106" t="s">
+        <v>12</v>
+      </c>
+      <c r="E106" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>199</v>
+      </c>
+      <c r="B107">
+        <v>3103</v>
+      </c>
+      <c r="C107" t="s">
+        <v>26</v>
+      </c>
+      <c r="D107" t="s">
+        <v>12</v>
+      </c>
+      <c r="E107" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>70</v>
+      </c>
+      <c r="B108">
+        <v>4000</v>
+      </c>
+      <c r="C108" t="s">
+        <v>71</v>
+      </c>
+      <c r="D108" t="s">
+        <v>2</v>
+      </c>
+      <c r="E108" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>73</v>
+      </c>
+      <c r="B109">
+        <v>4001</v>
+      </c>
+      <c r="C109" t="s">
+        <v>71</v>
+      </c>
+      <c r="D109" t="s">
+        <v>12</v>
+      </c>
+      <c r="E109" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>166</v>
+      </c>
+      <c r="B110">
+        <v>4002</v>
+      </c>
+      <c r="C110" t="s">
+        <v>71</v>
+      </c>
+      <c r="D110" t="s">
+        <v>12</v>
+      </c>
+      <c r="E110" t="s">
         <v>167</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>165</v>
-      </c>
-      <c r="B104">
-        <v>3003</v>
-      </c>
-      <c r="C104" t="s">
-        <v>163</v>
-      </c>
-      <c r="D104" t="s">
-        <v>162</v>
-      </c>
-      <c r="E104" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>170</v>
-      </c>
-      <c r="B105">
-        <v>3004</v>
-      </c>
-      <c r="C105" t="s">
-        <v>163</v>
-      </c>
-      <c r="D105" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>168</v>
-      </c>
-      <c r="B106">
-        <v>3005</v>
-      </c>
-      <c r="C106" t="s">
-        <v>163</v>
-      </c>
-      <c r="D106" t="s">
-        <v>162</v>
-      </c>
-      <c r="E106" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>189</v>
-      </c>
-      <c r="B107">
-        <v>3006</v>
-      </c>
-      <c r="C107" t="s">
-        <v>190</v>
-      </c>
-      <c r="D107" t="s">
-        <v>162</v>
-      </c>
-      <c r="E107" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>192</v>
-      </c>
-      <c r="B108">
-        <v>3007</v>
-      </c>
-      <c r="C108" t="s">
-        <v>190</v>
-      </c>
-      <c r="D108" t="s">
-        <v>162</v>
-      </c>
-      <c r="E108" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>194</v>
-      </c>
-      <c r="B109">
-        <v>3008</v>
-      </c>
-      <c r="C109" t="s">
-        <v>190</v>
-      </c>
-      <c r="D109" t="s">
-        <v>162</v>
-      </c>
-      <c r="E109" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>206</v>
-      </c>
-      <c r="B110">
-        <v>3100</v>
-      </c>
-      <c r="C110" t="s">
-        <v>26</v>
-      </c>
-      <c r="D110" t="s">
-        <v>12</v>
-      </c>
-      <c r="E110" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>208</v>
-      </c>
-      <c r="B111">
-        <v>3101</v>
-      </c>
-      <c r="C111" t="s">
-        <v>26</v>
-      </c>
-      <c r="D111" t="s">
-        <v>12</v>
-      </c>
-      <c r="E111" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>209</v>
-      </c>
-      <c r="B112">
-        <v>3102</v>
-      </c>
-      <c r="C112" t="s">
-        <v>26</v>
-      </c>
-      <c r="D112" t="s">
-        <v>12</v>
-      </c>
-      <c r="E112" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>212</v>
-      </c>
-      <c r="B113">
-        <v>3103</v>
-      </c>
-      <c r="C113" t="s">
-        <v>26</v>
-      </c>
-      <c r="D113" t="s">
-        <v>12</v>
-      </c>
-      <c r="E113" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>70</v>
-      </c>
-      <c r="B114">
-        <v>4000</v>
-      </c>
-      <c r="C114" t="s">
-        <v>71</v>
-      </c>
-      <c r="D114" t="s">
-        <v>2</v>
-      </c>
-      <c r="E114" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>73</v>
-      </c>
-      <c r="B115">
-        <v>4001</v>
-      </c>
-      <c r="C115" t="s">
-        <v>71</v>
-      </c>
-      <c r="D115" t="s">
-        <v>12</v>
-      </c>
-      <c r="E115" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>179</v>
-      </c>
-      <c r="B116">
-        <v>4002</v>
-      </c>
-      <c r="C116" t="s">
-        <v>71</v>
-      </c>
-      <c r="D116" t="s">
-        <v>12</v>
-      </c>
-      <c r="E116" t="s">
-        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>